<commit_message>
Extract functions from report Rmd
</commit_message>
<xml_diff>
--- a/data-raw/params_out.xlsx
+++ b/data-raw/params_out.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/Dropbox/Dropbox/R/Fortran/RGrWat/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/Data/GitHub/grwat/data-raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{099802D3-3B00-764A-A58B-57F2BEF562A7}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{DCFA66C9-4920-FC44-B75F-00FAD6FAC267}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="500" yWindow="1840" windowWidth="28300" windowHeight="14680" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="8000" yWindow="1660" windowWidth="28300" windowHeight="14680" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="581" uniqueCount="218">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="639" uniqueCount="219">
   <si>
     <t>year_number</t>
   </si>
@@ -114,15 +114,9 @@
     <t>Минимальный 30-суточный расход за лето</t>
   </si>
   <si>
-    <t>date30s(1)</t>
-  </si>
-  <si>
     <t>Дата начала минимального 30-суточного расхода за лето</t>
   </si>
   <si>
-    <t>date30s(2)</t>
-  </si>
-  <si>
     <t>Дата окончания минимального 30-суточного расхода за лето</t>
   </si>
   <si>
@@ -132,15 +126,9 @@
     <t>Минимальный 30-суточный расход за зиму</t>
   </si>
   <si>
-    <t>date30w(1)</t>
-  </si>
-  <si>
     <t>Дата начала минимального 30-суточного расхода за зиму</t>
   </si>
   <si>
-    <t>date30w(2)</t>
-  </si>
-  <si>
     <t>Дата окончания минимального 30-суточного расхода за зиму</t>
   </si>
   <si>
@@ -150,15 +138,9 @@
     <t>Минимальный 10-суточный расход за лето</t>
   </si>
   <si>
-    <t>date10s(1)</t>
-  </si>
-  <si>
     <t>Дата начала минимального 10-суточного расхода за лето</t>
   </si>
   <si>
-    <t>date10s(2)</t>
-  </si>
-  <si>
     <t>Дата окончания минимального 10-суточного расхода за лето</t>
   </si>
   <si>
@@ -171,9 +153,6 @@
     <t>Дата начала минимального 10-суточного расхода за зиму</t>
   </si>
   <si>
-    <t>date10w(2)</t>
-  </si>
-  <si>
     <t>Дата окончания минимального 10-суточного расхода за зиму</t>
   </si>
   <si>
@@ -183,15 +162,9 @@
     <t>Минимальный 5-суточный расход за лето</t>
   </si>
   <si>
-    <t>date5s(1)</t>
-  </si>
-  <si>
     <t>Дата начала минимального 5-суточного расхода за лето</t>
   </si>
   <si>
-    <t>date5s(2)</t>
-  </si>
-  <si>
     <t>Дата окончания минимального 5-суточного расхода за лето</t>
   </si>
   <si>
@@ -204,9 +177,6 @@
     <t>Дата начала минимального 5-суточного расхода за зиму</t>
   </si>
   <si>
-    <t>date5w(2)</t>
-  </si>
-  <si>
     <t>Дата окончания минимального 5-суточного расхода за зиму</t>
   </si>
   <si>
@@ -381,12 +351,6 @@
     <t>Date</t>
   </si>
   <si>
-    <t>date10w(1)</t>
-  </si>
-  <si>
-    <t>date5w(1)</t>
-  </si>
-  <si>
     <t>Winter</t>
   </si>
   <si>
@@ -405,9 +369,6 @@
     <t>none</t>
   </si>
   <si>
-    <t>Range Rule</t>
-  </si>
-  <si>
     <t>Problems</t>
   </si>
   <si>
@@ -682,6 +643,48 @@
   </si>
   <si>
     <t>plate</t>
+  </si>
+  <si>
+    <t>date30s1</t>
+  </si>
+  <si>
+    <t>date30s2</t>
+  </si>
+  <si>
+    <t>date30w1</t>
+  </si>
+  <si>
+    <t>date30w2</t>
+  </si>
+  <si>
+    <t>date10s1</t>
+  </si>
+  <si>
+    <t>date10s2</t>
+  </si>
+  <si>
+    <t>date10w1</t>
+  </si>
+  <si>
+    <t>date10w2</t>
+  </si>
+  <si>
+    <t>date5s1</t>
+  </si>
+  <si>
+    <t>date5s2</t>
+  </si>
+  <si>
+    <t>date5w1</t>
+  </si>
+  <si>
+    <t>date5w2</t>
+  </si>
+  <si>
+    <t>Range</t>
+  </si>
+  <si>
+    <t>Readtype</t>
   </si>
 </sst>
 </file>
@@ -1293,10 +1296,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:R58"/>
+  <dimension ref="A1:S58"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="81" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="I24" sqref="I24"/>
+      <selection activeCell="J3" sqref="J3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16"/>
@@ -1308,72 +1311,76 @@
     <col min="5" max="5" width="15" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="7" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="8.1640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="7.5" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="75.6640625" customWidth="1"/>
-    <col min="10" max="10" width="61.6640625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="34.33203125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="7.5" style="2" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="6.5" style="2" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="14.1640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="6.83203125" style="2" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="11.6640625" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="50.83203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.5" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="7.5" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="75.6640625" customWidth="1"/>
+    <col min="11" max="11" width="61.6640625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="34.33203125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="7.5" style="2" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="6.5" style="2" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="14.1640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="6.83203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="50.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" s="1" customFormat="1" ht="19" customHeight="1">
+    <row r="1" spans="1:19" s="1" customFormat="1" ht="19" customHeight="1">
       <c r="A1" s="15" t="s">
-        <v>105</v>
+        <v>95</v>
       </c>
       <c r="B1" s="15" t="s">
-        <v>111</v>
+        <v>101</v>
       </c>
       <c r="C1" s="15" t="s">
-        <v>112</v>
+        <v>102</v>
       </c>
       <c r="D1" s="15" t="s">
-        <v>133</v>
+        <v>120</v>
       </c>
       <c r="E1" s="15" t="s">
-        <v>106</v>
+        <v>96</v>
       </c>
       <c r="F1" s="15" t="s">
+        <v>97</v>
+      </c>
+      <c r="G1" s="15" t="s">
+        <v>178</v>
+      </c>
+      <c r="H1" s="15" t="s">
+        <v>218</v>
+      </c>
+      <c r="I1" s="15" t="s">
+        <v>103</v>
+      </c>
+      <c r="J1" s="15" t="s">
+        <v>177</v>
+      </c>
+      <c r="K1" s="15" t="s">
+        <v>143</v>
+      </c>
+      <c r="L1" s="15" t="s">
+        <v>94</v>
+      </c>
+      <c r="M1" s="15" t="s">
         <v>107</v>
       </c>
-      <c r="G1" s="15" t="s">
-        <v>191</v>
-      </c>
-      <c r="H1" s="15" t="s">
+      <c r="N1" s="15" t="s">
+        <v>110</v>
+      </c>
+      <c r="O1" s="15" t="s">
+        <v>118</v>
+      </c>
+      <c r="P1" s="15" t="s">
+        <v>117</v>
+      </c>
+      <c r="Q1" s="16" t="s">
+        <v>217</v>
+      </c>
+      <c r="R1" s="8" t="s">
         <v>113</v>
       </c>
-      <c r="I1" s="15" t="s">
-        <v>190</v>
-      </c>
-      <c r="J1" s="15" t="s">
-        <v>156</v>
-      </c>
-      <c r="K1" s="15" t="s">
-        <v>104</v>
-      </c>
-      <c r="L1" s="15" t="s">
-        <v>119</v>
-      </c>
-      <c r="M1" s="15" t="s">
-        <v>122</v>
-      </c>
-      <c r="N1" s="15" t="s">
-        <v>131</v>
-      </c>
-      <c r="O1" s="15" t="s">
-        <v>130</v>
-      </c>
-      <c r="P1" s="16" t="s">
-        <v>125</v>
-      </c>
-      <c r="Q1" s="8" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="2" spans="1:18" ht="17" customHeight="1">
+    </row>
+    <row r="2" spans="1:19" ht="17" customHeight="1">
       <c r="A2" s="12">
         <v>1</v>
       </c>
@@ -1392,35 +1399,38 @@
       <c r="F2" s="10"/>
       <c r="G2" s="10"/>
       <c r="H2" s="10" t="s">
-        <v>114</v>
+        <v>104</v>
       </c>
       <c r="I2" s="10" t="s">
-        <v>1</v>
-      </c>
-      <c r="J2" s="11" t="s">
-        <v>166</v>
-      </c>
-      <c r="K2" s="12" t="s">
-        <v>108</v>
-      </c>
-      <c r="L2" s="13">
-        <v>0</v>
-      </c>
-      <c r="M2" s="14" t="s">
-        <v>124</v>
-      </c>
-      <c r="N2" s="17" t="s">
-        <v>135</v>
-      </c>
-      <c r="O2" s="9">
-        <v>0</v>
-      </c>
-      <c r="P2" s="18" t="s">
-        <v>120</v>
-      </c>
-      <c r="Q2" s="9"/>
-    </row>
-    <row r="3" spans="1:18">
+        <v>104</v>
+      </c>
+      <c r="J2" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="K2" s="11" t="s">
+        <v>153</v>
+      </c>
+      <c r="L2" s="12" t="s">
+        <v>98</v>
+      </c>
+      <c r="M2" s="13">
+        <v>0</v>
+      </c>
+      <c r="N2" s="14" t="s">
+        <v>112</v>
+      </c>
+      <c r="O2" s="17" t="s">
+        <v>122</v>
+      </c>
+      <c r="P2" s="9">
+        <v>0</v>
+      </c>
+      <c r="Q2" s="18" t="s">
+        <v>108</v>
+      </c>
+      <c r="R2" s="9"/>
+    </row>
+    <row r="3" spans="1:19">
       <c r="A3" s="12">
         <v>2</v>
       </c>
@@ -1437,41 +1447,44 @@
         <v>2</v>
       </c>
       <c r="F3" s="10" t="s">
-        <v>197</v>
+        <v>184</v>
       </c>
       <c r="G3" s="10" t="s">
-        <v>192</v>
+        <v>179</v>
       </c>
       <c r="H3" s="10" t="s">
-        <v>114</v>
+        <v>104</v>
       </c>
       <c r="I3" s="10" t="s">
+        <v>104</v>
+      </c>
+      <c r="J3" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="J3" s="11" t="s">
-        <v>201</v>
-      </c>
-      <c r="K3" s="12" t="s">
-        <v>108</v>
-      </c>
-      <c r="L3" s="13">
-        <v>0</v>
-      </c>
-      <c r="M3" s="14" t="s">
-        <v>124</v>
-      </c>
-      <c r="N3" s="17" t="s">
-        <v>135</v>
-      </c>
-      <c r="O3" s="9">
-        <v>0</v>
-      </c>
-      <c r="P3" s="18" t="s">
-        <v>120</v>
-      </c>
-      <c r="Q3" s="9"/>
-    </row>
-    <row r="4" spans="1:18">
+      <c r="K3" s="11" t="s">
+        <v>188</v>
+      </c>
+      <c r="L3" s="12" t="s">
+        <v>98</v>
+      </c>
+      <c r="M3" s="13">
+        <v>0</v>
+      </c>
+      <c r="N3" s="14" t="s">
+        <v>112</v>
+      </c>
+      <c r="O3" s="17" t="s">
+        <v>122</v>
+      </c>
+      <c r="P3" s="9">
+        <v>0</v>
+      </c>
+      <c r="Q3" s="18" t="s">
+        <v>108</v>
+      </c>
+      <c r="R3" s="9"/>
+    </row>
+    <row r="4" spans="1:19">
       <c r="A4" s="12">
         <v>3</v>
       </c>
@@ -1488,41 +1501,44 @@
         <v>4</v>
       </c>
       <c r="F4" s="10" t="s">
-        <v>197</v>
+        <v>184</v>
       </c>
       <c r="G4" s="10" t="s">
-        <v>192</v>
+        <v>179</v>
       </c>
       <c r="H4" s="10" t="s">
-        <v>114</v>
+        <v>104</v>
       </c>
       <c r="I4" s="10" t="s">
+        <v>104</v>
+      </c>
+      <c r="J4" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="J4" s="11" t="s">
-        <v>202</v>
-      </c>
-      <c r="K4" s="12" t="s">
-        <v>108</v>
-      </c>
-      <c r="L4" s="13">
-        <v>0</v>
-      </c>
-      <c r="M4" s="14" t="s">
-        <v>124</v>
-      </c>
-      <c r="N4" s="17" t="s">
-        <v>135</v>
-      </c>
-      <c r="O4" s="9">
-        <v>0</v>
-      </c>
-      <c r="P4" s="18" t="s">
-        <v>120</v>
-      </c>
-      <c r="Q4" s="9"/>
-    </row>
-    <row r="5" spans="1:18">
+      <c r="K4" s="11" t="s">
+        <v>189</v>
+      </c>
+      <c r="L4" s="12" t="s">
+        <v>98</v>
+      </c>
+      <c r="M4" s="13">
+        <v>0</v>
+      </c>
+      <c r="N4" s="14" t="s">
+        <v>112</v>
+      </c>
+      <c r="O4" s="17" t="s">
+        <v>122</v>
+      </c>
+      <c r="P4" s="9">
+        <v>0</v>
+      </c>
+      <c r="Q4" s="18" t="s">
+        <v>108</v>
+      </c>
+      <c r="R4" s="9"/>
+    </row>
+    <row r="5" spans="1:19">
       <c r="A5" s="12">
         <v>4</v>
       </c>
@@ -1539,41 +1555,44 @@
         <v>6</v>
       </c>
       <c r="F5" s="10" t="s">
-        <v>198</v>
+        <v>185</v>
       </c>
       <c r="G5" s="10" t="s">
+        <v>106</v>
+      </c>
+      <c r="H5" s="10" t="s">
+        <v>106</v>
+      </c>
+      <c r="I5" s="10" t="s">
+        <v>106</v>
+      </c>
+      <c r="J5" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="K5" s="11" t="s">
+        <v>154</v>
+      </c>
+      <c r="L5" s="12" t="s">
+        <v>98</v>
+      </c>
+      <c r="M5" s="13">
+        <v>2</v>
+      </c>
+      <c r="N5" s="14" t="s">
         <v>116</v>
       </c>
-      <c r="H5" s="10" t="s">
-        <v>116</v>
-      </c>
-      <c r="I5" s="10" t="s">
-        <v>7</v>
-      </c>
-      <c r="J5" s="11" t="s">
-        <v>167</v>
-      </c>
-      <c r="K5" s="12" t="s">
-        <v>108</v>
-      </c>
-      <c r="L5" s="13">
-        <v>2</v>
-      </c>
-      <c r="M5" s="14" t="s">
-        <v>129</v>
-      </c>
-      <c r="N5" s="19" t="s">
-        <v>188</v>
-      </c>
-      <c r="O5" s="9">
+      <c r="O5" s="19" t="s">
+        <v>175</v>
+      </c>
+      <c r="P5" s="9">
         <v>14</v>
       </c>
-      <c r="P5" s="18" t="s">
-        <v>120</v>
-      </c>
-      <c r="Q5" s="9"/>
-    </row>
-    <row r="6" spans="1:18">
+      <c r="Q5" s="18" t="s">
+        <v>108</v>
+      </c>
+      <c r="R5" s="9"/>
+    </row>
+    <row r="6" spans="1:19">
       <c r="A6" s="12">
         <v>5</v>
       </c>
@@ -1590,41 +1609,44 @@
         <v>8</v>
       </c>
       <c r="F6" s="10" t="s">
-        <v>198</v>
+        <v>185</v>
       </c>
       <c r="G6" s="10" t="s">
+        <v>106</v>
+      </c>
+      <c r="H6" s="10" t="s">
+        <v>106</v>
+      </c>
+      <c r="I6" s="10" t="s">
+        <v>106</v>
+      </c>
+      <c r="J6" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="K6" s="11" t="s">
+        <v>155</v>
+      </c>
+      <c r="L6" s="12" t="s">
+        <v>98</v>
+      </c>
+      <c r="M6" s="13">
+        <v>2</v>
+      </c>
+      <c r="N6" s="14" t="s">
         <v>116</v>
       </c>
-      <c r="H6" s="10" t="s">
-        <v>116</v>
-      </c>
-      <c r="I6" s="10" t="s">
-        <v>9</v>
-      </c>
-      <c r="J6" s="11" t="s">
-        <v>168</v>
-      </c>
-      <c r="K6" s="12" t="s">
-        <v>108</v>
-      </c>
-      <c r="L6" s="13">
-        <v>2</v>
-      </c>
-      <c r="M6" s="14" t="s">
-        <v>129</v>
-      </c>
-      <c r="N6" s="19" t="s">
-        <v>188</v>
-      </c>
-      <c r="O6" s="9">
+      <c r="O6" s="19" t="s">
+        <v>175</v>
+      </c>
+      <c r="P6" s="9">
         <v>16</v>
       </c>
-      <c r="P6" s="18" t="s">
-        <v>120</v>
-      </c>
-      <c r="Q6" s="9"/>
-    </row>
-    <row r="7" spans="1:18">
+      <c r="Q6" s="18" t="s">
+        <v>108</v>
+      </c>
+      <c r="R6" s="9"/>
+    </row>
+    <row r="7" spans="1:19">
       <c r="A7" s="12">
         <v>6</v>
       </c>
@@ -1641,41 +1663,44 @@
         <v>10</v>
       </c>
       <c r="F7" s="10" t="s">
-        <v>216</v>
+        <v>203</v>
       </c>
       <c r="G7" s="10" t="s">
-        <v>193</v>
+        <v>180</v>
       </c>
       <c r="H7" s="10" t="s">
-        <v>115</v>
+        <v>105</v>
       </c>
       <c r="I7" s="10" t="s">
+        <v>105</v>
+      </c>
+      <c r="J7" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="J7" s="11" t="s">
-        <v>137</v>
-      </c>
-      <c r="K7" s="12" t="s">
-        <v>108</v>
-      </c>
-      <c r="L7" s="13">
-        <v>0</v>
-      </c>
-      <c r="M7" s="14" t="s">
-        <v>121</v>
-      </c>
-      <c r="N7" s="10" t="s">
-        <v>185</v>
-      </c>
-      <c r="O7" s="9">
+      <c r="K7" s="11" t="s">
+        <v>124</v>
+      </c>
+      <c r="L7" s="12" t="s">
+        <v>98</v>
+      </c>
+      <c r="M7" s="13">
+        <v>0</v>
+      </c>
+      <c r="N7" s="14" t="s">
+        <v>109</v>
+      </c>
+      <c r="O7" s="10" t="s">
+        <v>172</v>
+      </c>
+      <c r="P7" s="9">
         <v>13</v>
       </c>
-      <c r="P7" s="18" t="s">
-        <v>120</v>
-      </c>
-      <c r="Q7" s="9"/>
-    </row>
-    <row r="8" spans="1:18">
+      <c r="Q7" s="18" t="s">
+        <v>108</v>
+      </c>
+      <c r="R7" s="9"/>
+    </row>
+    <row r="8" spans="1:19">
       <c r="A8" s="12">
         <v>7</v>
       </c>
@@ -1692,41 +1717,44 @@
         <v>12</v>
       </c>
       <c r="F8" s="10" t="s">
-        <v>216</v>
+        <v>203</v>
       </c>
       <c r="G8" s="10" t="s">
-        <v>193</v>
+        <v>180</v>
       </c>
       <c r="H8" s="10" t="s">
-        <v>115</v>
+        <v>105</v>
       </c>
       <c r="I8" s="10" t="s">
+        <v>105</v>
+      </c>
+      <c r="J8" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="J8" s="11" t="s">
-        <v>138</v>
-      </c>
-      <c r="K8" s="12" t="s">
-        <v>108</v>
-      </c>
-      <c r="L8" s="13">
-        <v>0</v>
-      </c>
-      <c r="M8" s="14" t="s">
-        <v>121</v>
-      </c>
-      <c r="N8" s="19" t="s">
-        <v>188</v>
-      </c>
-      <c r="O8" s="9">
+      <c r="K8" s="11" t="s">
+        <v>125</v>
+      </c>
+      <c r="L8" s="12" t="s">
+        <v>98</v>
+      </c>
+      <c r="M8" s="13">
+        <v>0</v>
+      </c>
+      <c r="N8" s="14" t="s">
+        <v>109</v>
+      </c>
+      <c r="O8" s="19" t="s">
+        <v>175</v>
+      </c>
+      <c r="P8" s="9">
         <v>17</v>
       </c>
-      <c r="P8" s="18" t="s">
-        <v>120</v>
-      </c>
-      <c r="Q8" s="9"/>
-    </row>
-    <row r="9" spans="1:18">
+      <c r="Q8" s="18" t="s">
+        <v>108</v>
+      </c>
+      <c r="R8" s="9"/>
+    </row>
+    <row r="9" spans="1:19">
       <c r="A9" s="12">
         <v>8</v>
       </c>
@@ -1743,41 +1771,44 @@
         <v>14</v>
       </c>
       <c r="F9" s="10" t="s">
-        <v>198</v>
+        <v>185</v>
       </c>
       <c r="G9" s="10" t="s">
+        <v>106</v>
+      </c>
+      <c r="H9" s="10" t="s">
+        <v>106</v>
+      </c>
+      <c r="I9" s="10" t="s">
+        <v>106</v>
+      </c>
+      <c r="J9" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="K9" s="11" t="s">
+        <v>152</v>
+      </c>
+      <c r="L9" s="12" t="s">
+        <v>98</v>
+      </c>
+      <c r="M9" s="13">
+        <v>2</v>
+      </c>
+      <c r="N9" s="14" t="s">
         <v>116</v>
       </c>
-      <c r="H9" s="10" t="s">
-        <v>116</v>
-      </c>
-      <c r="I9" s="10" t="s">
-        <v>15</v>
-      </c>
-      <c r="J9" s="11" t="s">
-        <v>165</v>
-      </c>
-      <c r="K9" s="12" t="s">
-        <v>108</v>
-      </c>
-      <c r="L9" s="13">
-        <v>2</v>
-      </c>
-      <c r="M9" s="14" t="s">
-        <v>129</v>
-      </c>
-      <c r="N9" s="19" t="s">
-        <v>188</v>
-      </c>
-      <c r="O9" s="9">
+      <c r="O9" s="19" t="s">
+        <v>175</v>
+      </c>
+      <c r="P9" s="9">
         <v>18</v>
       </c>
-      <c r="P9" s="18" t="s">
-        <v>120</v>
-      </c>
-      <c r="Q9" s="9"/>
-    </row>
-    <row r="10" spans="1:18" s="6" customFormat="1" ht="19" customHeight="1">
+      <c r="Q9" s="18" t="s">
+        <v>108</v>
+      </c>
+      <c r="R9" s="9"/>
+    </row>
+    <row r="10" spans="1:19" s="6" customFormat="1" ht="19" customHeight="1">
       <c r="A10" s="12">
         <v>10</v>
       </c>
@@ -1794,42 +1825,45 @@
         <v>16</v>
       </c>
       <c r="F10" s="10" t="s">
-        <v>216</v>
+        <v>203</v>
       </c>
       <c r="G10" s="10" t="s">
-        <v>193</v>
+        <v>180</v>
       </c>
       <c r="H10" s="10" t="s">
-        <v>115</v>
+        <v>105</v>
       </c>
       <c r="I10" s="10" t="s">
+        <v>105</v>
+      </c>
+      <c r="J10" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="J10" s="21" t="s">
-        <v>204</v>
-      </c>
-      <c r="K10" s="12" t="s">
-        <v>108</v>
-      </c>
-      <c r="L10" s="22">
-        <v>0</v>
-      </c>
-      <c r="M10" s="23" t="s">
-        <v>121</v>
-      </c>
-      <c r="N10" s="10" t="s">
-        <v>185</v>
-      </c>
-      <c r="O10" s="20">
+      <c r="K10" s="21" t="s">
+        <v>191</v>
+      </c>
+      <c r="L10" s="12" t="s">
+        <v>98</v>
+      </c>
+      <c r="M10" s="22">
+        <v>0</v>
+      </c>
+      <c r="N10" s="23" t="s">
+        <v>109</v>
+      </c>
+      <c r="O10" s="10" t="s">
+        <v>172</v>
+      </c>
+      <c r="P10" s="20">
         <v>15</v>
       </c>
-      <c r="P10" s="18" t="s">
-        <v>120</v>
-      </c>
-      <c r="Q10" s="20"/>
-      <c r="R10"/>
-    </row>
-    <row r="11" spans="1:18">
+      <c r="Q10" s="18" t="s">
+        <v>108</v>
+      </c>
+      <c r="R10" s="20"/>
+      <c r="S10"/>
+    </row>
+    <row r="11" spans="1:19">
       <c r="A11" s="24">
         <v>11</v>
       </c>
@@ -1846,41 +1880,44 @@
         <v>18</v>
       </c>
       <c r="F11" s="25" t="s">
-        <v>216</v>
+        <v>203</v>
       </c>
       <c r="G11" s="25" t="s">
-        <v>193</v>
+        <v>180</v>
       </c>
       <c r="H11" s="25" t="s">
-        <v>115</v>
+        <v>105</v>
       </c>
       <c r="I11" s="25" t="s">
+        <v>105</v>
+      </c>
+      <c r="J11" s="25" t="s">
         <v>19</v>
       </c>
-      <c r="J11" s="26" t="s">
-        <v>139</v>
-      </c>
-      <c r="K11" s="24" t="s">
+      <c r="K11" s="26" t="s">
+        <v>126</v>
+      </c>
+      <c r="L11" s="24" t="s">
+        <v>99</v>
+      </c>
+      <c r="M11" s="27">
+        <v>0</v>
+      </c>
+      <c r="N11" s="28" t="s">
         <v>109</v>
       </c>
-      <c r="L11" s="27">
-        <v>0</v>
-      </c>
-      <c r="M11" s="28" t="s">
-        <v>121</v>
-      </c>
-      <c r="N11" s="29" t="s">
-        <v>189</v>
-      </c>
-      <c r="O11" s="30">
+      <c r="O11" s="29" t="s">
+        <v>176</v>
+      </c>
+      <c r="P11" s="30">
         <v>23</v>
       </c>
-      <c r="P11" s="31" t="s">
-        <v>120</v>
-      </c>
-      <c r="Q11" s="17"/>
-    </row>
-    <row r="12" spans="1:18">
+      <c r="Q11" s="31" t="s">
+        <v>108</v>
+      </c>
+      <c r="R11" s="17"/>
+    </row>
+    <row r="12" spans="1:19">
       <c r="A12" s="24">
         <v>12</v>
       </c>
@@ -1897,43 +1934,46 @@
         <v>20</v>
       </c>
       <c r="F12" s="25" t="s">
-        <v>199</v>
+        <v>186</v>
       </c>
       <c r="G12" s="25" t="s">
-        <v>195</v>
+        <v>182</v>
       </c>
       <c r="H12" s="41" t="s">
-        <v>115</v>
-      </c>
-      <c r="I12" s="25" t="s">
+        <v>105</v>
+      </c>
+      <c r="I12" s="41" t="s">
+        <v>106</v>
+      </c>
+      <c r="J12" s="25" t="s">
         <v>21</v>
       </c>
-      <c r="J12" s="26" t="s">
-        <v>162</v>
-      </c>
-      <c r="K12" s="24" t="s">
-        <v>109</v>
-      </c>
-      <c r="L12" s="27">
-        <v>0</v>
-      </c>
-      <c r="M12" s="32" t="s">
-        <v>217</v>
-      </c>
-      <c r="N12" s="29" t="s">
-        <v>189</v>
-      </c>
-      <c r="O12" s="30">
+      <c r="K12" s="26" t="s">
+        <v>149</v>
+      </c>
+      <c r="L12" s="24" t="s">
+        <v>99</v>
+      </c>
+      <c r="M12" s="27">
+        <v>0</v>
+      </c>
+      <c r="N12" s="32" t="s">
+        <v>204</v>
+      </c>
+      <c r="O12" s="29" t="s">
+        <v>176</v>
+      </c>
+      <c r="P12" s="30">
         <v>24</v>
       </c>
-      <c r="P12" s="31" t="s">
-        <v>120</v>
-      </c>
-      <c r="Q12" s="17" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="13" spans="1:18">
+      <c r="Q12" s="31" t="s">
+        <v>108</v>
+      </c>
+      <c r="R12" s="17" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="13" spans="1:19">
       <c r="A13" s="24">
         <v>13</v>
       </c>
@@ -1950,41 +1990,44 @@
         <v>22</v>
       </c>
       <c r="F13" s="25" t="s">
-        <v>216</v>
+        <v>203</v>
       </c>
       <c r="G13" s="25" t="s">
-        <v>193</v>
+        <v>180</v>
       </c>
       <c r="H13" s="25" t="s">
-        <v>115</v>
+        <v>105</v>
       </c>
       <c r="I13" s="25" t="s">
+        <v>105</v>
+      </c>
+      <c r="J13" s="25" t="s">
         <v>23</v>
       </c>
-      <c r="J13" s="26" t="s">
-        <v>140</v>
-      </c>
-      <c r="K13" s="24" t="s">
+      <c r="K13" s="26" t="s">
+        <v>127</v>
+      </c>
+      <c r="L13" s="24" t="s">
+        <v>99</v>
+      </c>
+      <c r="M13" s="27">
+        <v>0</v>
+      </c>
+      <c r="N13" s="32" t="s">
         <v>109</v>
       </c>
-      <c r="L13" s="27">
-        <v>0</v>
-      </c>
-      <c r="M13" s="32" t="s">
-        <v>121</v>
-      </c>
-      <c r="N13" s="33" t="s">
-        <v>136</v>
-      </c>
-      <c r="O13" s="30">
+      <c r="O13" s="33" t="s">
+        <v>123</v>
+      </c>
+      <c r="P13" s="30">
         <v>21</v>
       </c>
-      <c r="P13" s="31" t="s">
-        <v>120</v>
-      </c>
-      <c r="Q13" s="17"/>
-    </row>
-    <row r="14" spans="1:18">
+      <c r="Q13" s="31" t="s">
+        <v>108</v>
+      </c>
+      <c r="R13" s="17"/>
+    </row>
+    <row r="14" spans="1:19">
       <c r="A14" s="24">
         <v>14</v>
       </c>
@@ -2001,43 +2044,46 @@
         <v>24</v>
       </c>
       <c r="F14" s="25" t="s">
-        <v>199</v>
+        <v>186</v>
       </c>
       <c r="G14" s="25" t="s">
-        <v>195</v>
+        <v>182</v>
       </c>
       <c r="H14" s="41" t="s">
-        <v>115</v>
-      </c>
-      <c r="I14" s="25" t="s">
+        <v>105</v>
+      </c>
+      <c r="I14" s="41" t="s">
+        <v>106</v>
+      </c>
+      <c r="J14" s="25" t="s">
         <v>25</v>
       </c>
-      <c r="J14" s="26" t="s">
-        <v>163</v>
-      </c>
-      <c r="K14" s="24" t="s">
-        <v>109</v>
-      </c>
-      <c r="L14" s="27">
-        <v>1</v>
-      </c>
-      <c r="M14" s="32" t="s">
-        <v>217</v>
-      </c>
-      <c r="N14" s="34" t="s">
-        <v>136</v>
-      </c>
-      <c r="O14" s="30">
+      <c r="K14" s="26" t="s">
+        <v>150</v>
+      </c>
+      <c r="L14" s="24" t="s">
+        <v>99</v>
+      </c>
+      <c r="M14" s="27">
+        <v>1</v>
+      </c>
+      <c r="N14" s="32" t="s">
+        <v>204</v>
+      </c>
+      <c r="O14" s="34" t="s">
+        <v>123</v>
+      </c>
+      <c r="P14" s="30">
         <v>22</v>
       </c>
-      <c r="P14" s="31" t="s">
-        <v>120</v>
-      </c>
-      <c r="Q14" s="17" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="15" spans="1:18">
+      <c r="Q14" s="31" t="s">
+        <v>108</v>
+      </c>
+      <c r="R14" s="17" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="15" spans="1:19">
       <c r="A15" s="24">
         <v>15</v>
       </c>
@@ -2054,41 +2100,44 @@
         <v>26</v>
       </c>
       <c r="F15" s="25" t="s">
-        <v>216</v>
+        <v>203</v>
       </c>
       <c r="G15" s="25" t="s">
-        <v>193</v>
+        <v>180</v>
       </c>
       <c r="H15" s="25" t="s">
-        <v>115</v>
+        <v>105</v>
       </c>
       <c r="I15" s="25" t="s">
+        <v>105</v>
+      </c>
+      <c r="J15" s="25" t="s">
         <v>27</v>
       </c>
-      <c r="J15" s="26" t="s">
-        <v>141</v>
-      </c>
-      <c r="K15" s="24" t="s">
+      <c r="K15" s="26" t="s">
+        <v>128</v>
+      </c>
+      <c r="L15" s="24" t="s">
+        <v>99</v>
+      </c>
+      <c r="M15" s="27">
+        <v>0</v>
+      </c>
+      <c r="N15" s="32" t="s">
         <v>109</v>
       </c>
-      <c r="L15" s="27">
-        <v>0</v>
-      </c>
-      <c r="M15" s="32" t="s">
-        <v>121</v>
-      </c>
-      <c r="N15" s="29" t="s">
-        <v>189</v>
-      </c>
-      <c r="O15" s="30">
+      <c r="O15" s="29" t="s">
+        <v>176</v>
+      </c>
+      <c r="P15" s="30">
         <v>27</v>
       </c>
-      <c r="P15" s="31" t="s">
-        <v>120</v>
-      </c>
-      <c r="Q15" s="17"/>
-    </row>
-    <row r="16" spans="1:18">
+      <c r="Q15" s="31" t="s">
+        <v>108</v>
+      </c>
+      <c r="R15" s="17"/>
+    </row>
+    <row r="16" spans="1:19">
       <c r="A16" s="24">
         <v>16</v>
       </c>
@@ -2102,44 +2151,47 @@
         <v>1</v>
       </c>
       <c r="E16" s="25" t="s">
+        <v>205</v>
+      </c>
+      <c r="F16" s="25" t="s">
+        <v>185</v>
+      </c>
+      <c r="G16" s="25" t="s">
+        <v>106</v>
+      </c>
+      <c r="H16" s="25" t="s">
+        <v>106</v>
+      </c>
+      <c r="I16" s="25" t="s">
+        <v>106</v>
+      </c>
+      <c r="J16" s="25" t="s">
         <v>28</v>
       </c>
-      <c r="F16" s="25" t="s">
-        <v>198</v>
-      </c>
-      <c r="G16" s="25" t="s">
+      <c r="K16" s="26" t="s">
+        <v>144</v>
+      </c>
+      <c r="L16" s="24" t="s">
+        <v>99</v>
+      </c>
+      <c r="M16" s="27">
+        <v>0</v>
+      </c>
+      <c r="N16" s="32" t="s">
         <v>116</v>
       </c>
-      <c r="H16" s="25" t="s">
-        <v>116</v>
-      </c>
-      <c r="I16" s="25" t="s">
-        <v>29</v>
-      </c>
-      <c r="J16" s="26" t="s">
-        <v>157</v>
-      </c>
-      <c r="K16" s="24" t="s">
-        <v>109</v>
-      </c>
-      <c r="L16" s="27">
-        <v>0</v>
-      </c>
-      <c r="M16" s="32" t="s">
-        <v>129</v>
-      </c>
-      <c r="N16" s="29" t="s">
-        <v>189</v>
-      </c>
-      <c r="O16" s="30">
+      <c r="O16" s="29" t="s">
+        <v>176</v>
+      </c>
+      <c r="P16" s="30">
         <v>28</v>
       </c>
-      <c r="P16" s="31" t="s">
-        <v>120</v>
-      </c>
-      <c r="Q16" s="17"/>
-    </row>
-    <row r="17" spans="1:17">
+      <c r="Q16" s="31" t="s">
+        <v>108</v>
+      </c>
+      <c r="R16" s="17"/>
+    </row>
+    <row r="17" spans="1:18">
       <c r="A17" s="24">
         <v>17</v>
       </c>
@@ -2153,44 +2205,47 @@
         <v>1</v>
       </c>
       <c r="E17" s="25" t="s">
-        <v>30</v>
+        <v>206</v>
       </c>
       <c r="F17" s="25" t="s">
-        <v>198</v>
+        <v>185</v>
       </c>
       <c r="G17" s="25" t="s">
+        <v>106</v>
+      </c>
+      <c r="H17" s="25" t="s">
+        <v>106</v>
+      </c>
+      <c r="I17" s="25" t="s">
+        <v>106</v>
+      </c>
+      <c r="J17" s="25" t="s">
+        <v>29</v>
+      </c>
+      <c r="K17" s="26" t="s">
+        <v>145</v>
+      </c>
+      <c r="L17" s="24" t="s">
+        <v>99</v>
+      </c>
+      <c r="M17" s="27">
+        <v>0</v>
+      </c>
+      <c r="N17" s="32" t="s">
         <v>116</v>
       </c>
-      <c r="H17" s="25" t="s">
-        <v>116</v>
-      </c>
-      <c r="I17" s="25" t="s">
-        <v>31</v>
-      </c>
-      <c r="J17" s="26" t="s">
-        <v>158</v>
-      </c>
-      <c r="K17" s="24" t="s">
-        <v>109</v>
-      </c>
-      <c r="L17" s="27">
-        <v>0</v>
-      </c>
-      <c r="M17" s="32" t="s">
-        <v>129</v>
-      </c>
-      <c r="N17" s="17" t="s">
-        <v>135</v>
-      </c>
-      <c r="O17" s="30">
-        <v>0</v>
-      </c>
-      <c r="P17" s="31" t="s">
-        <v>120</v>
-      </c>
-      <c r="Q17" s="17"/>
-    </row>
-    <row r="18" spans="1:17">
+      <c r="O17" s="17" t="s">
+        <v>122</v>
+      </c>
+      <c r="P17" s="30">
+        <v>0</v>
+      </c>
+      <c r="Q17" s="31" t="s">
+        <v>108</v>
+      </c>
+      <c r="R17" s="17"/>
+    </row>
+    <row r="18" spans="1:18">
       <c r="A18" s="24">
         <v>18</v>
       </c>
@@ -2204,44 +2259,47 @@
         <v>1</v>
       </c>
       <c r="E18" s="25" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="F18" s="25" t="s">
-        <v>216</v>
+        <v>203</v>
       </c>
       <c r="G18" s="25" t="s">
-        <v>193</v>
+        <v>180</v>
       </c>
       <c r="H18" s="25" t="s">
-        <v>115</v>
+        <v>105</v>
       </c>
       <c r="I18" s="25" t="s">
-        <v>33</v>
-      </c>
-      <c r="J18" s="26" t="s">
-        <v>142</v>
-      </c>
-      <c r="K18" s="24" t="s">
+        <v>105</v>
+      </c>
+      <c r="J18" s="25" t="s">
+        <v>31</v>
+      </c>
+      <c r="K18" s="26" t="s">
+        <v>129</v>
+      </c>
+      <c r="L18" s="24" t="s">
+        <v>99</v>
+      </c>
+      <c r="M18" s="27">
+        <v>0</v>
+      </c>
+      <c r="N18" s="32" t="s">
         <v>109</v>
       </c>
-      <c r="L18" s="27">
-        <v>0</v>
-      </c>
-      <c r="M18" s="32" t="s">
-        <v>121</v>
-      </c>
-      <c r="N18" s="33" t="s">
-        <v>136</v>
-      </c>
-      <c r="O18" s="30">
+      <c r="O18" s="33" t="s">
+        <v>123</v>
+      </c>
+      <c r="P18" s="30">
         <v>25</v>
       </c>
-      <c r="P18" s="31" t="s">
-        <v>120</v>
-      </c>
-      <c r="Q18" s="17"/>
-    </row>
-    <row r="19" spans="1:17">
+      <c r="Q18" s="31" t="s">
+        <v>108</v>
+      </c>
+      <c r="R18" s="17"/>
+    </row>
+    <row r="19" spans="1:18">
       <c r="A19" s="24">
         <v>19</v>
       </c>
@@ -2255,44 +2313,47 @@
         <v>1</v>
       </c>
       <c r="E19" s="25" t="s">
-        <v>34</v>
+        <v>207</v>
       </c>
       <c r="F19" s="25" t="s">
-        <v>198</v>
+        <v>185</v>
       </c>
       <c r="G19" s="25" t="s">
+        <v>106</v>
+      </c>
+      <c r="H19" s="25" t="s">
+        <v>106</v>
+      </c>
+      <c r="I19" s="25" t="s">
+        <v>106</v>
+      </c>
+      <c r="J19" s="25" t="s">
+        <v>32</v>
+      </c>
+      <c r="K19" s="26" t="s">
+        <v>151</v>
+      </c>
+      <c r="L19" s="24" t="s">
+        <v>99</v>
+      </c>
+      <c r="M19" s="27">
+        <v>1</v>
+      </c>
+      <c r="N19" s="32" t="s">
         <v>116</v>
       </c>
-      <c r="H19" s="25" t="s">
-        <v>116</v>
-      </c>
-      <c r="I19" s="25" t="s">
-        <v>35</v>
-      </c>
-      <c r="J19" s="26" t="s">
-        <v>164</v>
-      </c>
-      <c r="K19" s="24" t="s">
-        <v>109</v>
-      </c>
-      <c r="L19" s="27">
-        <v>1</v>
-      </c>
-      <c r="M19" s="32" t="s">
-        <v>129</v>
-      </c>
-      <c r="N19" s="34" t="s">
-        <v>136</v>
-      </c>
-      <c r="O19" s="30">
+      <c r="O19" s="34" t="s">
+        <v>123</v>
+      </c>
+      <c r="P19" s="30">
         <v>26</v>
       </c>
-      <c r="P19" s="31" t="s">
-        <v>120</v>
-      </c>
-      <c r="Q19" s="17"/>
-    </row>
-    <row r="20" spans="1:17">
+      <c r="Q19" s="31" t="s">
+        <v>108</v>
+      </c>
+      <c r="R19" s="17"/>
+    </row>
+    <row r="20" spans="1:18">
       <c r="A20" s="24">
         <v>20</v>
       </c>
@@ -2306,44 +2367,47 @@
         <v>1</v>
       </c>
       <c r="E20" s="25" t="s">
-        <v>36</v>
+        <v>208</v>
       </c>
       <c r="F20" s="25" t="s">
-        <v>198</v>
+        <v>185</v>
       </c>
       <c r="G20" s="25" t="s">
+        <v>106</v>
+      </c>
+      <c r="H20" s="25" t="s">
+        <v>106</v>
+      </c>
+      <c r="I20" s="25" t="s">
+        <v>106</v>
+      </c>
+      <c r="J20" s="25" t="s">
+        <v>33</v>
+      </c>
+      <c r="K20" s="26" t="s">
+        <v>146</v>
+      </c>
+      <c r="L20" s="24" t="s">
+        <v>99</v>
+      </c>
+      <c r="M20" s="27">
+        <v>1</v>
+      </c>
+      <c r="N20" s="32" t="s">
         <v>116</v>
       </c>
-      <c r="H20" s="25" t="s">
-        <v>116</v>
-      </c>
-      <c r="I20" s="25" t="s">
-        <v>37</v>
-      </c>
-      <c r="J20" s="26" t="s">
-        <v>159</v>
-      </c>
-      <c r="K20" s="24" t="s">
-        <v>109</v>
-      </c>
-      <c r="L20" s="27">
-        <v>1</v>
-      </c>
-      <c r="M20" s="32" t="s">
-        <v>129</v>
-      </c>
-      <c r="N20" s="17" t="s">
-        <v>135</v>
-      </c>
-      <c r="O20" s="30">
-        <v>0</v>
-      </c>
-      <c r="P20" s="31" t="s">
-        <v>120</v>
-      </c>
-      <c r="Q20" s="17"/>
-    </row>
-    <row r="21" spans="1:17">
+      <c r="O20" s="17" t="s">
+        <v>122</v>
+      </c>
+      <c r="P20" s="30">
+        <v>0</v>
+      </c>
+      <c r="Q20" s="31" t="s">
+        <v>108</v>
+      </c>
+      <c r="R20" s="17"/>
+    </row>
+    <row r="21" spans="1:18">
       <c r="A21" s="24">
         <v>21</v>
       </c>
@@ -2357,44 +2421,47 @@
         <v>1</v>
       </c>
       <c r="E21" s="25" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="F21" s="25" t="s">
-        <v>216</v>
+        <v>203</v>
       </c>
       <c r="G21" s="25" t="s">
-        <v>193</v>
+        <v>180</v>
       </c>
       <c r="H21" s="25" t="s">
-        <v>115</v>
+        <v>105</v>
       </c>
       <c r="I21" s="25" t="s">
-        <v>39</v>
-      </c>
-      <c r="J21" s="26" t="s">
-        <v>143</v>
-      </c>
-      <c r="K21" s="24" t="s">
+        <v>105</v>
+      </c>
+      <c r="J21" s="25" t="s">
+        <v>35</v>
+      </c>
+      <c r="K21" s="26" t="s">
+        <v>130</v>
+      </c>
+      <c r="L21" s="24" t="s">
+        <v>99</v>
+      </c>
+      <c r="M21" s="27">
+        <v>0</v>
+      </c>
+      <c r="N21" s="32" t="s">
         <v>109</v>
       </c>
-      <c r="L21" s="27">
-        <v>0</v>
-      </c>
-      <c r="M21" s="32" t="s">
-        <v>121</v>
-      </c>
-      <c r="N21" s="29" t="s">
-        <v>189</v>
-      </c>
-      <c r="O21" s="30">
+      <c r="O21" s="29" t="s">
+        <v>176</v>
+      </c>
+      <c r="P21" s="30">
         <v>31</v>
       </c>
-      <c r="P21" s="31" t="s">
-        <v>120</v>
-      </c>
-      <c r="Q21" s="17"/>
-    </row>
-    <row r="22" spans="1:17">
+      <c r="Q21" s="31" t="s">
+        <v>108</v>
+      </c>
+      <c r="R21" s="17"/>
+    </row>
+    <row r="22" spans="1:18">
       <c r="A22" s="24">
         <v>22</v>
       </c>
@@ -2408,44 +2475,47 @@
         <v>1</v>
       </c>
       <c r="E22" s="25" t="s">
-        <v>40</v>
+        <v>209</v>
       </c>
       <c r="F22" s="25" t="s">
-        <v>198</v>
+        <v>185</v>
       </c>
       <c r="G22" s="25" t="s">
+        <v>106</v>
+      </c>
+      <c r="H22" s="25" t="s">
+        <v>106</v>
+      </c>
+      <c r="I22" s="25" t="s">
+        <v>106</v>
+      </c>
+      <c r="J22" s="25" t="s">
+        <v>36</v>
+      </c>
+      <c r="K22" s="26" t="s">
+        <v>147</v>
+      </c>
+      <c r="L22" s="24" t="s">
+        <v>99</v>
+      </c>
+      <c r="M22" s="27">
+        <v>0</v>
+      </c>
+      <c r="N22" s="32" t="s">
         <v>116</v>
       </c>
-      <c r="H22" s="25" t="s">
-        <v>116</v>
-      </c>
-      <c r="I22" s="25" t="s">
-        <v>41</v>
-      </c>
-      <c r="J22" s="26" t="s">
-        <v>160</v>
-      </c>
-      <c r="K22" s="24" t="s">
-        <v>109</v>
-      </c>
-      <c r="L22" s="27">
-        <v>0</v>
-      </c>
-      <c r="M22" s="32" t="s">
-        <v>129</v>
-      </c>
-      <c r="N22" s="29" t="s">
-        <v>189</v>
-      </c>
-      <c r="O22" s="30">
+      <c r="O22" s="29" t="s">
+        <v>176</v>
+      </c>
+      <c r="P22" s="30">
         <v>32</v>
       </c>
-      <c r="P22" s="31" t="s">
-        <v>120</v>
-      </c>
-      <c r="Q22" s="17"/>
-    </row>
-    <row r="23" spans="1:17">
+      <c r="Q22" s="31" t="s">
+        <v>108</v>
+      </c>
+      <c r="R22" s="17"/>
+    </row>
+    <row r="23" spans="1:18">
       <c r="A23" s="24">
         <v>23</v>
       </c>
@@ -2459,44 +2529,47 @@
         <v>1</v>
       </c>
       <c r="E23" s="25" t="s">
-        <v>42</v>
+        <v>210</v>
       </c>
       <c r="F23" s="25" t="s">
-        <v>198</v>
+        <v>185</v>
       </c>
       <c r="G23" s="25" t="s">
+        <v>106</v>
+      </c>
+      <c r="H23" s="25" t="s">
+        <v>106</v>
+      </c>
+      <c r="I23" s="25" t="s">
+        <v>106</v>
+      </c>
+      <c r="J23" s="25" t="s">
+        <v>37</v>
+      </c>
+      <c r="K23" s="26" t="s">
+        <v>148</v>
+      </c>
+      <c r="L23" s="24" t="s">
+        <v>99</v>
+      </c>
+      <c r="M23" s="27">
+        <v>0</v>
+      </c>
+      <c r="N23" s="32" t="s">
         <v>116</v>
       </c>
-      <c r="H23" s="25" t="s">
-        <v>116</v>
-      </c>
-      <c r="I23" s="25" t="s">
-        <v>43</v>
-      </c>
-      <c r="J23" s="26" t="s">
-        <v>161</v>
-      </c>
-      <c r="K23" s="24" t="s">
-        <v>109</v>
-      </c>
-      <c r="L23" s="27">
-        <v>0</v>
-      </c>
-      <c r="M23" s="32" t="s">
-        <v>129</v>
-      </c>
-      <c r="N23" s="17" t="s">
-        <v>135</v>
-      </c>
-      <c r="O23" s="30">
-        <v>0</v>
-      </c>
-      <c r="P23" s="31" t="s">
-        <v>120</v>
-      </c>
-      <c r="Q23" s="17"/>
-    </row>
-    <row r="24" spans="1:17">
+      <c r="O23" s="17" t="s">
+        <v>122</v>
+      </c>
+      <c r="P23" s="30">
+        <v>0</v>
+      </c>
+      <c r="Q23" s="31" t="s">
+        <v>108</v>
+      </c>
+      <c r="R23" s="17"/>
+    </row>
+    <row r="24" spans="1:18">
       <c r="A24" s="24">
         <v>24</v>
       </c>
@@ -2510,44 +2583,47 @@
         <v>1</v>
       </c>
       <c r="E24" s="25" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="F24" s="25" t="s">
-        <v>216</v>
+        <v>203</v>
       </c>
       <c r="G24" s="25" t="s">
-        <v>193</v>
+        <v>180</v>
       </c>
       <c r="H24" s="25" t="s">
-        <v>115</v>
+        <v>105</v>
       </c>
       <c r="I24" s="25" t="s">
-        <v>45</v>
-      </c>
-      <c r="J24" s="26" t="s">
-        <v>144</v>
-      </c>
-      <c r="K24" s="24" t="s">
+        <v>105</v>
+      </c>
+      <c r="J24" s="25" t="s">
+        <v>39</v>
+      </c>
+      <c r="K24" s="26" t="s">
+        <v>131</v>
+      </c>
+      <c r="L24" s="24" t="s">
+        <v>99</v>
+      </c>
+      <c r="M24" s="27">
+        <v>0</v>
+      </c>
+      <c r="N24" s="32" t="s">
         <v>109</v>
       </c>
-      <c r="L24" s="27">
-        <v>0</v>
-      </c>
-      <c r="M24" s="32" t="s">
-        <v>121</v>
-      </c>
-      <c r="N24" s="33" t="s">
-        <v>136</v>
-      </c>
-      <c r="O24" s="30">
+      <c r="O24" s="33" t="s">
+        <v>123</v>
+      </c>
+      <c r="P24" s="30">
         <v>29</v>
       </c>
-      <c r="P24" s="31" t="s">
-        <v>120</v>
-      </c>
-      <c r="Q24" s="17"/>
-    </row>
-    <row r="25" spans="1:17">
+      <c r="Q24" s="31" t="s">
+        <v>108</v>
+      </c>
+      <c r="R24" s="17"/>
+    </row>
+    <row r="25" spans="1:18">
       <c r="A25" s="24">
         <v>25</v>
       </c>
@@ -2561,44 +2637,47 @@
         <v>1</v>
       </c>
       <c r="E25" s="25" t="s">
-        <v>117</v>
+        <v>211</v>
       </c>
       <c r="F25" s="25" t="s">
-        <v>198</v>
+        <v>185</v>
       </c>
       <c r="G25" s="25" t="s">
+        <v>106</v>
+      </c>
+      <c r="H25" s="25" t="s">
+        <v>106</v>
+      </c>
+      <c r="I25" s="25" t="s">
+        <v>106</v>
+      </c>
+      <c r="J25" s="25" t="s">
+        <v>40</v>
+      </c>
+      <c r="K25" s="26" t="s">
+        <v>158</v>
+      </c>
+      <c r="L25" s="24" t="s">
+        <v>99</v>
+      </c>
+      <c r="M25" s="27">
+        <v>1</v>
+      </c>
+      <c r="N25" s="32" t="s">
         <v>116</v>
       </c>
-      <c r="H25" s="25" t="s">
-        <v>116</v>
-      </c>
-      <c r="I25" s="25" t="s">
-        <v>46</v>
-      </c>
-      <c r="J25" s="26" t="s">
-        <v>171</v>
-      </c>
-      <c r="K25" s="24" t="s">
-        <v>109</v>
-      </c>
-      <c r="L25" s="27">
-        <v>1</v>
-      </c>
-      <c r="M25" s="32" t="s">
-        <v>129</v>
-      </c>
-      <c r="N25" s="34" t="s">
-        <v>136</v>
-      </c>
-      <c r="O25" s="30">
+      <c r="O25" s="34" t="s">
+        <v>123</v>
+      </c>
+      <c r="P25" s="30">
         <v>30</v>
       </c>
-      <c r="P25" s="31" t="s">
-        <v>120</v>
-      </c>
-      <c r="Q25" s="17"/>
-    </row>
-    <row r="26" spans="1:17">
+      <c r="Q25" s="31" t="s">
+        <v>108</v>
+      </c>
+      <c r="R25" s="17"/>
+    </row>
+    <row r="26" spans="1:18">
       <c r="A26" s="24">
         <v>26</v>
       </c>
@@ -2612,44 +2691,47 @@
         <v>1</v>
       </c>
       <c r="E26" s="25" t="s">
-        <v>47</v>
+        <v>212</v>
       </c>
       <c r="F26" s="25" t="s">
-        <v>198</v>
+        <v>185</v>
       </c>
       <c r="G26" s="25" t="s">
+        <v>106</v>
+      </c>
+      <c r="H26" s="25" t="s">
+        <v>106</v>
+      </c>
+      <c r="I26" s="25" t="s">
+        <v>106</v>
+      </c>
+      <c r="J26" s="25" t="s">
+        <v>41</v>
+      </c>
+      <c r="K26" s="26" t="s">
+        <v>159</v>
+      </c>
+      <c r="L26" s="24" t="s">
+        <v>99</v>
+      </c>
+      <c r="M26" s="27">
+        <v>1</v>
+      </c>
+      <c r="N26" s="32" t="s">
         <v>116</v>
       </c>
-      <c r="H26" s="25" t="s">
-        <v>116</v>
-      </c>
-      <c r="I26" s="25" t="s">
-        <v>48</v>
-      </c>
-      <c r="J26" s="26" t="s">
-        <v>172</v>
-      </c>
-      <c r="K26" s="24" t="s">
-        <v>109</v>
-      </c>
-      <c r="L26" s="27">
-        <v>1</v>
-      </c>
-      <c r="M26" s="32" t="s">
-        <v>129</v>
-      </c>
-      <c r="N26" s="17" t="s">
-        <v>135</v>
-      </c>
-      <c r="O26" s="30">
-        <v>0</v>
-      </c>
-      <c r="P26" s="31" t="s">
-        <v>120</v>
-      </c>
-      <c r="Q26" s="17"/>
-    </row>
-    <row r="27" spans="1:17">
+      <c r="O26" s="17" t="s">
+        <v>122</v>
+      </c>
+      <c r="P26" s="30">
+        <v>0</v>
+      </c>
+      <c r="Q26" s="31" t="s">
+        <v>108</v>
+      </c>
+      <c r="R26" s="17"/>
+    </row>
+    <row r="27" spans="1:18">
       <c r="A27" s="24">
         <v>27</v>
       </c>
@@ -2663,44 +2745,47 @@
         <v>1</v>
       </c>
       <c r="E27" s="25" t="s">
-        <v>49</v>
+        <v>42</v>
       </c>
       <c r="F27" s="25" t="s">
-        <v>216</v>
+        <v>203</v>
       </c>
       <c r="G27" s="25" t="s">
-        <v>193</v>
+        <v>180</v>
       </c>
       <c r="H27" s="25" t="s">
-        <v>115</v>
+        <v>105</v>
       </c>
       <c r="I27" s="25" t="s">
-        <v>50</v>
-      </c>
-      <c r="J27" s="26" t="s">
-        <v>145</v>
-      </c>
-      <c r="K27" s="24" t="s">
+        <v>105</v>
+      </c>
+      <c r="J27" s="25" t="s">
+        <v>43</v>
+      </c>
+      <c r="K27" s="26" t="s">
+        <v>132</v>
+      </c>
+      <c r="L27" s="24" t="s">
+        <v>99</v>
+      </c>
+      <c r="M27" s="27">
+        <v>0</v>
+      </c>
+      <c r="N27" s="32" t="s">
         <v>109</v>
       </c>
-      <c r="L27" s="27">
-        <v>0</v>
-      </c>
-      <c r="M27" s="32" t="s">
-        <v>121</v>
-      </c>
-      <c r="N27" s="29" t="s">
-        <v>189</v>
-      </c>
-      <c r="O27" s="30">
+      <c r="O27" s="29" t="s">
+        <v>176</v>
+      </c>
+      <c r="P27" s="30">
         <v>35</v>
       </c>
-      <c r="P27" s="31" t="s">
-        <v>120</v>
-      </c>
-      <c r="Q27" s="17"/>
-    </row>
-    <row r="28" spans="1:17">
+      <c r="Q27" s="31" t="s">
+        <v>108</v>
+      </c>
+      <c r="R27" s="17"/>
+    </row>
+    <row r="28" spans="1:18">
       <c r="A28" s="24">
         <v>28</v>
       </c>
@@ -2714,44 +2799,47 @@
         <v>1</v>
       </c>
       <c r="E28" s="25" t="s">
-        <v>51</v>
+        <v>213</v>
       </c>
       <c r="F28" s="25" t="s">
-        <v>198</v>
+        <v>185</v>
       </c>
       <c r="G28" s="25" t="s">
+        <v>106</v>
+      </c>
+      <c r="H28" s="25" t="s">
+        <v>106</v>
+      </c>
+      <c r="I28" s="25" t="s">
+        <v>106</v>
+      </c>
+      <c r="J28" s="25" t="s">
+        <v>44</v>
+      </c>
+      <c r="K28" s="26" t="s">
+        <v>160</v>
+      </c>
+      <c r="L28" s="24" t="s">
+        <v>99</v>
+      </c>
+      <c r="M28" s="27">
+        <v>0</v>
+      </c>
+      <c r="N28" s="32" t="s">
         <v>116</v>
       </c>
-      <c r="H28" s="25" t="s">
-        <v>116</v>
-      </c>
-      <c r="I28" s="25" t="s">
-        <v>52</v>
-      </c>
-      <c r="J28" s="26" t="s">
-        <v>173</v>
-      </c>
-      <c r="K28" s="24" t="s">
-        <v>109</v>
-      </c>
-      <c r="L28" s="27">
-        <v>0</v>
-      </c>
-      <c r="M28" s="32" t="s">
-        <v>129</v>
-      </c>
-      <c r="N28" s="29" t="s">
-        <v>189</v>
-      </c>
-      <c r="O28" s="30">
+      <c r="O28" s="29" t="s">
+        <v>176</v>
+      </c>
+      <c r="P28" s="30">
         <v>36</v>
       </c>
-      <c r="P28" s="31" t="s">
-        <v>120</v>
-      </c>
-      <c r="Q28" s="17"/>
-    </row>
-    <row r="29" spans="1:17">
+      <c r="Q28" s="31" t="s">
+        <v>108</v>
+      </c>
+      <c r="R28" s="17"/>
+    </row>
+    <row r="29" spans="1:18">
       <c r="A29" s="24">
         <v>29</v>
       </c>
@@ -2765,44 +2853,47 @@
         <v>1</v>
       </c>
       <c r="E29" s="25" t="s">
-        <v>53</v>
+        <v>214</v>
       </c>
       <c r="F29" s="25" t="s">
-        <v>198</v>
+        <v>185</v>
       </c>
       <c r="G29" s="25" t="s">
+        <v>106</v>
+      </c>
+      <c r="H29" s="25" t="s">
+        <v>106</v>
+      </c>
+      <c r="I29" s="25" t="s">
+        <v>106</v>
+      </c>
+      <c r="J29" s="25" t="s">
+        <v>45</v>
+      </c>
+      <c r="K29" s="26" t="s">
+        <v>161</v>
+      </c>
+      <c r="L29" s="24" t="s">
+        <v>99</v>
+      </c>
+      <c r="M29" s="27">
+        <v>0</v>
+      </c>
+      <c r="N29" s="32" t="s">
         <v>116</v>
       </c>
-      <c r="H29" s="25" t="s">
-        <v>116</v>
-      </c>
-      <c r="I29" s="25" t="s">
-        <v>54</v>
-      </c>
-      <c r="J29" s="26" t="s">
-        <v>174</v>
-      </c>
-      <c r="K29" s="24" t="s">
-        <v>109</v>
-      </c>
-      <c r="L29" s="27">
-        <v>0</v>
-      </c>
-      <c r="M29" s="32" t="s">
-        <v>129</v>
-      </c>
-      <c r="N29" s="17" t="s">
-        <v>135</v>
-      </c>
-      <c r="O29" s="30">
-        <v>0</v>
-      </c>
-      <c r="P29" s="31" t="s">
-        <v>120</v>
-      </c>
-      <c r="Q29" s="17"/>
-    </row>
-    <row r="30" spans="1:17">
+      <c r="O29" s="17" t="s">
+        <v>122</v>
+      </c>
+      <c r="P29" s="30">
+        <v>0</v>
+      </c>
+      <c r="Q29" s="31" t="s">
+        <v>108</v>
+      </c>
+      <c r="R29" s="17"/>
+    </row>
+    <row r="30" spans="1:18">
       <c r="A30" s="24">
         <v>30</v>
       </c>
@@ -2816,44 +2907,47 @@
         <v>1</v>
       </c>
       <c r="E30" s="25" t="s">
-        <v>55</v>
+        <v>46</v>
       </c>
       <c r="F30" s="25" t="s">
-        <v>216</v>
+        <v>203</v>
       </c>
       <c r="G30" s="25" t="s">
-        <v>193</v>
+        <v>180</v>
       </c>
       <c r="H30" s="25" t="s">
-        <v>115</v>
+        <v>105</v>
       </c>
       <c r="I30" s="25" t="s">
-        <v>56</v>
-      </c>
-      <c r="J30" s="26" t="s">
-        <v>146</v>
-      </c>
-      <c r="K30" s="24" t="s">
+        <v>105</v>
+      </c>
+      <c r="J30" s="25" t="s">
+        <v>47</v>
+      </c>
+      <c r="K30" s="26" t="s">
+        <v>133</v>
+      </c>
+      <c r="L30" s="24" t="s">
+        <v>99</v>
+      </c>
+      <c r="M30" s="27">
+        <v>0</v>
+      </c>
+      <c r="N30" s="32" t="s">
         <v>109</v>
       </c>
-      <c r="L30" s="27">
-        <v>0</v>
-      </c>
-      <c r="M30" s="32" t="s">
-        <v>121</v>
-      </c>
-      <c r="N30" s="33" t="s">
-        <v>136</v>
-      </c>
-      <c r="O30" s="30">
+      <c r="O30" s="33" t="s">
+        <v>123</v>
+      </c>
+      <c r="P30" s="30">
         <v>33</v>
       </c>
-      <c r="P30" s="31" t="s">
-        <v>120</v>
-      </c>
-      <c r="Q30" s="17"/>
-    </row>
-    <row r="31" spans="1:17">
+      <c r="Q30" s="31" t="s">
+        <v>108</v>
+      </c>
+      <c r="R30" s="17"/>
+    </row>
+    <row r="31" spans="1:18">
       <c r="A31" s="24">
         <v>31</v>
       </c>
@@ -2867,44 +2961,47 @@
         <v>1</v>
       </c>
       <c r="E31" s="25" t="s">
-        <v>118</v>
+        <v>215</v>
       </c>
       <c r="F31" s="25" t="s">
-        <v>198</v>
+        <v>185</v>
       </c>
       <c r="G31" s="25" t="s">
+        <v>106</v>
+      </c>
+      <c r="H31" s="25" t="s">
+        <v>106</v>
+      </c>
+      <c r="I31" s="25" t="s">
+        <v>106</v>
+      </c>
+      <c r="J31" s="25" t="s">
+        <v>48</v>
+      </c>
+      <c r="K31" s="26" t="s">
+        <v>162</v>
+      </c>
+      <c r="L31" s="24" t="s">
+        <v>99</v>
+      </c>
+      <c r="M31" s="27">
+        <v>1</v>
+      </c>
+      <c r="N31" s="32" t="s">
         <v>116</v>
       </c>
-      <c r="H31" s="25" t="s">
-        <v>116</v>
-      </c>
-      <c r="I31" s="25" t="s">
-        <v>57</v>
-      </c>
-      <c r="J31" s="26" t="s">
-        <v>175</v>
-      </c>
-      <c r="K31" s="24" t="s">
-        <v>109</v>
-      </c>
-      <c r="L31" s="27">
-        <v>1</v>
-      </c>
-      <c r="M31" s="32" t="s">
-        <v>129</v>
-      </c>
-      <c r="N31" s="34" t="s">
-        <v>136</v>
-      </c>
-      <c r="O31" s="30">
+      <c r="O31" s="34" t="s">
+        <v>123</v>
+      </c>
+      <c r="P31" s="30">
         <v>34</v>
       </c>
-      <c r="P31" s="31" t="s">
-        <v>120</v>
-      </c>
-      <c r="Q31" s="17"/>
-    </row>
-    <row r="32" spans="1:17">
+      <c r="Q31" s="31" t="s">
+        <v>108</v>
+      </c>
+      <c r="R31" s="17"/>
+    </row>
+    <row r="32" spans="1:18">
       <c r="A32" s="24">
         <v>32</v>
       </c>
@@ -2918,44 +3015,47 @@
         <v>1</v>
       </c>
       <c r="E32" s="25" t="s">
-        <v>58</v>
+        <v>216</v>
       </c>
       <c r="F32" s="25" t="s">
-        <v>198</v>
+        <v>185</v>
       </c>
       <c r="G32" s="25" t="s">
+        <v>106</v>
+      </c>
+      <c r="H32" s="25" t="s">
+        <v>106</v>
+      </c>
+      <c r="I32" s="25" t="s">
+        <v>106</v>
+      </c>
+      <c r="J32" s="25" t="s">
+        <v>49</v>
+      </c>
+      <c r="K32" s="26" t="s">
+        <v>163</v>
+      </c>
+      <c r="L32" s="24" t="s">
+        <v>99</v>
+      </c>
+      <c r="M32" s="27">
+        <v>1</v>
+      </c>
+      <c r="N32" s="32" t="s">
         <v>116</v>
       </c>
-      <c r="H32" s="25" t="s">
-        <v>116</v>
-      </c>
-      <c r="I32" s="25" t="s">
-        <v>59</v>
-      </c>
-      <c r="J32" s="26" t="s">
-        <v>176</v>
-      </c>
-      <c r="K32" s="24" t="s">
-        <v>109</v>
-      </c>
-      <c r="L32" s="27">
-        <v>1</v>
-      </c>
-      <c r="M32" s="32" t="s">
-        <v>129</v>
-      </c>
-      <c r="N32" s="17" t="s">
-        <v>135</v>
-      </c>
-      <c r="O32" s="30">
-        <v>0</v>
-      </c>
-      <c r="P32" s="31" t="s">
-        <v>120</v>
-      </c>
-      <c r="Q32" s="17"/>
-    </row>
-    <row r="33" spans="1:17" ht="19" customHeight="1">
+      <c r="O32" s="17" t="s">
+        <v>122</v>
+      </c>
+      <c r="P32" s="30">
+        <v>0</v>
+      </c>
+      <c r="Q32" s="31" t="s">
+        <v>108</v>
+      </c>
+      <c r="R32" s="17"/>
+    </row>
+    <row r="33" spans="1:18" ht="19" customHeight="1">
       <c r="A33" s="24">
         <v>33</v>
       </c>
@@ -2969,44 +3069,47 @@
         <v>1</v>
       </c>
       <c r="E33" s="10" t="s">
-        <v>61</v>
+        <v>51</v>
       </c>
       <c r="F33" s="10" t="s">
-        <v>215</v>
+        <v>202</v>
       </c>
       <c r="G33" s="10" t="s">
-        <v>194</v>
+        <v>181</v>
       </c>
       <c r="H33" s="10" t="s">
-        <v>115</v>
+        <v>105</v>
       </c>
       <c r="I33" s="10" t="s">
-        <v>62</v>
-      </c>
-      <c r="J33" s="11" t="s">
-        <v>147</v>
-      </c>
-      <c r="K33" s="12" t="s">
-        <v>60</v>
-      </c>
-      <c r="L33" s="13">
-        <v>0</v>
-      </c>
-      <c r="M33" s="14" t="s">
-        <v>121</v>
-      </c>
-      <c r="N33" s="10" t="s">
-        <v>185</v>
-      </c>
-      <c r="O33" s="9">
-        <v>1</v>
-      </c>
-      <c r="P33" s="18" t="s">
-        <v>120</v>
-      </c>
-      <c r="Q33" s="9"/>
-    </row>
-    <row r="34" spans="1:17">
+        <v>105</v>
+      </c>
+      <c r="J33" s="10" t="s">
+        <v>52</v>
+      </c>
+      <c r="K33" s="11" t="s">
+        <v>134</v>
+      </c>
+      <c r="L33" s="12" t="s">
+        <v>50</v>
+      </c>
+      <c r="M33" s="13">
+        <v>0</v>
+      </c>
+      <c r="N33" s="14" t="s">
+        <v>109</v>
+      </c>
+      <c r="O33" s="10" t="s">
+        <v>172</v>
+      </c>
+      <c r="P33" s="9">
+        <v>1</v>
+      </c>
+      <c r="Q33" s="18" t="s">
+        <v>108</v>
+      </c>
+      <c r="R33" s="9"/>
+    </row>
+    <row r="34" spans="1:18">
       <c r="A34" s="24">
         <v>34</v>
       </c>
@@ -3020,44 +3123,47 @@
         <v>1</v>
       </c>
       <c r="E34" s="10" t="s">
-        <v>63</v>
+        <v>53</v>
       </c>
       <c r="F34" s="10" t="s">
-        <v>215</v>
+        <v>202</v>
       </c>
       <c r="G34" s="10" t="s">
-        <v>194</v>
+        <v>181</v>
       </c>
       <c r="H34" s="10" t="s">
-        <v>115</v>
+        <v>105</v>
       </c>
       <c r="I34" s="10" t="s">
-        <v>64</v>
-      </c>
-      <c r="J34" s="11" t="s">
-        <v>148</v>
-      </c>
-      <c r="K34" s="12" t="s">
-        <v>60</v>
-      </c>
-      <c r="L34" s="13">
-        <v>0</v>
-      </c>
-      <c r="M34" s="14" t="s">
-        <v>121</v>
-      </c>
-      <c r="N34" s="10" t="s">
-        <v>185</v>
-      </c>
-      <c r="O34" s="9">
+        <v>105</v>
+      </c>
+      <c r="J34" s="10" t="s">
+        <v>54</v>
+      </c>
+      <c r="K34" s="11" t="s">
+        <v>135</v>
+      </c>
+      <c r="L34" s="12" t="s">
+        <v>50</v>
+      </c>
+      <c r="M34" s="13">
+        <v>0</v>
+      </c>
+      <c r="N34" s="14" t="s">
+        <v>109</v>
+      </c>
+      <c r="O34" s="10" t="s">
+        <v>172</v>
+      </c>
+      <c r="P34" s="9">
         <v>3</v>
       </c>
-      <c r="P34" s="18" t="s">
-        <v>120</v>
-      </c>
-      <c r="Q34" s="9"/>
-    </row>
-    <row r="35" spans="1:17">
+      <c r="Q34" s="18" t="s">
+        <v>108</v>
+      </c>
+      <c r="R34" s="9"/>
+    </row>
+    <row r="35" spans="1:18">
       <c r="A35" s="24">
         <v>35</v>
       </c>
@@ -3071,44 +3177,47 @@
         <v>1</v>
       </c>
       <c r="E35" s="10" t="s">
-        <v>65</v>
+        <v>55</v>
       </c>
       <c r="F35" s="10" t="s">
-        <v>215</v>
+        <v>202</v>
       </c>
       <c r="G35" s="10" t="s">
-        <v>194</v>
+        <v>181</v>
       </c>
       <c r="H35" s="10" t="s">
-        <v>115</v>
+        <v>105</v>
       </c>
       <c r="I35" s="10" t="s">
-        <v>66</v>
-      </c>
-      <c r="J35" s="11" t="s">
-        <v>177</v>
-      </c>
-      <c r="K35" s="12" t="s">
-        <v>60</v>
-      </c>
-      <c r="L35" s="13">
-        <v>0</v>
-      </c>
-      <c r="M35" s="14" t="s">
-        <v>121</v>
-      </c>
-      <c r="N35" s="10" t="s">
-        <v>185</v>
-      </c>
-      <c r="O35" s="9">
+        <v>105</v>
+      </c>
+      <c r="J35" s="10" t="s">
+        <v>56</v>
+      </c>
+      <c r="K35" s="11" t="s">
+        <v>164</v>
+      </c>
+      <c r="L35" s="12" t="s">
+        <v>50</v>
+      </c>
+      <c r="M35" s="13">
+        <v>0</v>
+      </c>
+      <c r="N35" s="14" t="s">
+        <v>109</v>
+      </c>
+      <c r="O35" s="10" t="s">
+        <v>172</v>
+      </c>
+      <c r="P35" s="9">
         <v>4</v>
       </c>
-      <c r="P35" s="18" t="s">
-        <v>120</v>
-      </c>
-      <c r="Q35" s="9"/>
-    </row>
-    <row r="36" spans="1:17">
+      <c r="Q35" s="18" t="s">
+        <v>108</v>
+      </c>
+      <c r="R35" s="9"/>
+    </row>
+    <row r="36" spans="1:18">
       <c r="A36" s="24">
         <v>36</v>
       </c>
@@ -3122,44 +3231,47 @@
         <v>1</v>
       </c>
       <c r="E36" s="10" t="s">
-        <v>67</v>
+        <v>57</v>
       </c>
       <c r="F36" s="10" t="s">
-        <v>215</v>
+        <v>202</v>
       </c>
       <c r="G36" s="10" t="s">
-        <v>194</v>
+        <v>181</v>
       </c>
       <c r="H36" s="10" t="s">
-        <v>115</v>
+        <v>105</v>
       </c>
       <c r="I36" s="10" t="s">
-        <v>68</v>
-      </c>
-      <c r="J36" s="11" t="s">
-        <v>178</v>
-      </c>
-      <c r="K36" s="12" t="s">
-        <v>60</v>
-      </c>
-      <c r="L36" s="13">
-        <v>0</v>
-      </c>
-      <c r="M36" s="14" t="s">
-        <v>121</v>
-      </c>
-      <c r="N36" s="10" t="s">
-        <v>185</v>
-      </c>
-      <c r="O36" s="9">
+        <v>105</v>
+      </c>
+      <c r="J36" s="10" t="s">
+        <v>58</v>
+      </c>
+      <c r="K36" s="11" t="s">
+        <v>165</v>
+      </c>
+      <c r="L36" s="12" t="s">
+        <v>50</v>
+      </c>
+      <c r="M36" s="13">
+        <v>0</v>
+      </c>
+      <c r="N36" s="14" t="s">
+        <v>109</v>
+      </c>
+      <c r="O36" s="10" t="s">
+        <v>172</v>
+      </c>
+      <c r="P36" s="9">
         <v>2</v>
       </c>
-      <c r="P36" s="18" t="s">
-        <v>120</v>
-      </c>
-      <c r="Q36" s="9"/>
-    </row>
-    <row r="37" spans="1:17">
+      <c r="Q36" s="18" t="s">
+        <v>108</v>
+      </c>
+      <c r="R36" s="9"/>
+    </row>
+    <row r="37" spans="1:18">
       <c r="A37" s="24">
         <v>37</v>
       </c>
@@ -3173,44 +3285,47 @@
         <v>1</v>
       </c>
       <c r="E37" s="10" t="s">
-        <v>69</v>
+        <v>59</v>
       </c>
       <c r="F37" s="10" t="s">
-        <v>215</v>
+        <v>202</v>
       </c>
       <c r="G37" s="10" t="s">
-        <v>194</v>
+        <v>181</v>
       </c>
       <c r="H37" s="10" t="s">
-        <v>115</v>
+        <v>105</v>
       </c>
       <c r="I37" s="10" t="s">
-        <v>70</v>
-      </c>
-      <c r="J37" s="11" t="s">
-        <v>179</v>
-      </c>
-      <c r="K37" s="12" t="s">
+        <v>105</v>
+      </c>
+      <c r="J37" s="10" t="s">
         <v>60</v>
       </c>
-      <c r="L37" s="13">
-        <v>0</v>
-      </c>
-      <c r="M37" s="14" t="s">
-        <v>121</v>
-      </c>
-      <c r="N37" s="19" t="s">
-        <v>188</v>
-      </c>
-      <c r="O37" s="9">
+      <c r="K37" s="11" t="s">
+        <v>166</v>
+      </c>
+      <c r="L37" s="12" t="s">
+        <v>50</v>
+      </c>
+      <c r="M37" s="13">
+        <v>0</v>
+      </c>
+      <c r="N37" s="14" t="s">
+        <v>109</v>
+      </c>
+      <c r="O37" s="19" t="s">
+        <v>175</v>
+      </c>
+      <c r="P37" s="9">
         <v>19</v>
       </c>
-      <c r="P37" s="18" t="s">
-        <v>120</v>
-      </c>
-      <c r="Q37" s="9"/>
-    </row>
-    <row r="38" spans="1:17">
+      <c r="Q37" s="18" t="s">
+        <v>108</v>
+      </c>
+      <c r="R37" s="9"/>
+    </row>
+    <row r="38" spans="1:18">
       <c r="A38" s="24">
         <v>38</v>
       </c>
@@ -3224,44 +3339,47 @@
         <v>1</v>
       </c>
       <c r="E38" s="10" t="s">
-        <v>71</v>
+        <v>61</v>
       </c>
       <c r="F38" s="10" t="s">
-        <v>215</v>
+        <v>202</v>
       </c>
       <c r="G38" s="10" t="s">
-        <v>194</v>
+        <v>181</v>
       </c>
       <c r="H38" s="10" t="s">
-        <v>115</v>
+        <v>105</v>
       </c>
       <c r="I38" s="10" t="s">
-        <v>72</v>
-      </c>
-      <c r="J38" s="11" t="s">
-        <v>149</v>
-      </c>
-      <c r="K38" s="12" t="s">
-        <v>60</v>
-      </c>
-      <c r="L38" s="13">
-        <v>0</v>
-      </c>
-      <c r="M38" s="14" t="s">
-        <v>121</v>
-      </c>
-      <c r="N38" s="10" t="s">
-        <v>185</v>
-      </c>
-      <c r="O38" s="9">
+        <v>105</v>
+      </c>
+      <c r="J38" s="10" t="s">
+        <v>62</v>
+      </c>
+      <c r="K38" s="11" t="s">
+        <v>136</v>
+      </c>
+      <c r="L38" s="12" t="s">
+        <v>50</v>
+      </c>
+      <c r="M38" s="13">
+        <v>0</v>
+      </c>
+      <c r="N38" s="14" t="s">
+        <v>109</v>
+      </c>
+      <c r="O38" s="10" t="s">
+        <v>172</v>
+      </c>
+      <c r="P38" s="9">
         <v>6</v>
       </c>
-      <c r="P38" s="18" t="s">
-        <v>120</v>
-      </c>
-      <c r="Q38" s="9"/>
-    </row>
-    <row r="39" spans="1:17">
+      <c r="Q38" s="18" t="s">
+        <v>108</v>
+      </c>
+      <c r="R38" s="9"/>
+    </row>
+    <row r="39" spans="1:18">
       <c r="A39" s="24">
         <v>39</v>
       </c>
@@ -3275,44 +3393,47 @@
         <v>1</v>
       </c>
       <c r="E39" s="10" t="s">
-        <v>73</v>
+        <v>63</v>
       </c>
       <c r="F39" s="10" t="s">
-        <v>215</v>
+        <v>202</v>
       </c>
       <c r="G39" s="10" t="s">
-        <v>194</v>
+        <v>181</v>
       </c>
       <c r="H39" s="10" t="s">
-        <v>115</v>
+        <v>105</v>
       </c>
       <c r="I39" s="10" t="s">
-        <v>74</v>
-      </c>
-      <c r="J39" s="11" t="s">
-        <v>150</v>
-      </c>
-      <c r="K39" s="12" t="s">
-        <v>60</v>
-      </c>
-      <c r="L39" s="13">
-        <v>0</v>
-      </c>
-      <c r="M39" s="14" t="s">
-        <v>121</v>
-      </c>
-      <c r="N39" s="10" t="s">
-        <v>185</v>
-      </c>
-      <c r="O39" s="9">
+        <v>105</v>
+      </c>
+      <c r="J39" s="10" t="s">
+        <v>64</v>
+      </c>
+      <c r="K39" s="11" t="s">
+        <v>137</v>
+      </c>
+      <c r="L39" s="12" t="s">
+        <v>50</v>
+      </c>
+      <c r="M39" s="13">
+        <v>0</v>
+      </c>
+      <c r="N39" s="14" t="s">
+        <v>109</v>
+      </c>
+      <c r="O39" s="10" t="s">
+        <v>172</v>
+      </c>
+      <c r="P39" s="9">
         <v>5</v>
       </c>
-      <c r="P39" s="18" t="s">
-        <v>120</v>
-      </c>
-      <c r="Q39" s="9"/>
-    </row>
-    <row r="40" spans="1:17">
+      <c r="Q39" s="18" t="s">
+        <v>108</v>
+      </c>
+      <c r="R39" s="9"/>
+    </row>
+    <row r="40" spans="1:18">
       <c r="A40" s="24">
         <v>40</v>
       </c>
@@ -3326,44 +3447,47 @@
         <v>1</v>
       </c>
       <c r="E40" s="10" t="s">
-        <v>75</v>
+        <v>65</v>
       </c>
       <c r="F40" s="10" t="s">
-        <v>215</v>
+        <v>202</v>
       </c>
       <c r="G40" s="10" t="s">
-        <v>194</v>
+        <v>181</v>
       </c>
       <c r="H40" s="10" t="s">
-        <v>115</v>
+        <v>105</v>
       </c>
       <c r="I40" s="10" t="s">
-        <v>76</v>
-      </c>
-      <c r="J40" s="11" t="s">
-        <v>151</v>
-      </c>
-      <c r="K40" s="12" t="s">
-        <v>60</v>
-      </c>
-      <c r="L40" s="13">
-        <v>0</v>
-      </c>
-      <c r="M40" s="14" t="s">
-        <v>121</v>
-      </c>
-      <c r="N40" s="10" t="s">
-        <v>185</v>
-      </c>
-      <c r="O40" s="9">
+        <v>105</v>
+      </c>
+      <c r="J40" s="10" t="s">
+        <v>66</v>
+      </c>
+      <c r="K40" s="11" t="s">
+        <v>138</v>
+      </c>
+      <c r="L40" s="12" t="s">
+        <v>50</v>
+      </c>
+      <c r="M40" s="13">
+        <v>0</v>
+      </c>
+      <c r="N40" s="14" t="s">
+        <v>109</v>
+      </c>
+      <c r="O40" s="10" t="s">
+        <v>172</v>
+      </c>
+      <c r="P40" s="9">
         <v>8</v>
       </c>
-      <c r="P40" s="18" t="s">
-        <v>120</v>
-      </c>
-      <c r="Q40" s="9"/>
-    </row>
-    <row r="41" spans="1:17">
+      <c r="Q40" s="18" t="s">
+        <v>108</v>
+      </c>
+      <c r="R40" s="9"/>
+    </row>
+    <row r="41" spans="1:18">
       <c r="A41" s="24">
         <v>41</v>
       </c>
@@ -3377,44 +3501,47 @@
         <v>1</v>
       </c>
       <c r="E41" s="10" t="s">
-        <v>77</v>
+        <v>67</v>
       </c>
       <c r="F41" s="10" t="s">
-        <v>215</v>
+        <v>202</v>
       </c>
       <c r="G41" s="10" t="s">
-        <v>194</v>
+        <v>181</v>
       </c>
       <c r="H41" s="10" t="s">
-        <v>115</v>
+        <v>105</v>
       </c>
       <c r="I41" s="10" t="s">
-        <v>78</v>
-      </c>
-      <c r="J41" s="11" t="s">
-        <v>152</v>
-      </c>
-      <c r="K41" s="12" t="s">
-        <v>60</v>
-      </c>
-      <c r="L41" s="13">
-        <v>0</v>
-      </c>
-      <c r="M41" s="14" t="s">
-        <v>121</v>
-      </c>
-      <c r="N41" s="10" t="s">
-        <v>185</v>
-      </c>
-      <c r="O41" s="9">
+        <v>105</v>
+      </c>
+      <c r="J41" s="10" t="s">
+        <v>68</v>
+      </c>
+      <c r="K41" s="11" t="s">
+        <v>139</v>
+      </c>
+      <c r="L41" s="12" t="s">
+        <v>50</v>
+      </c>
+      <c r="M41" s="13">
+        <v>0</v>
+      </c>
+      <c r="N41" s="14" t="s">
+        <v>109</v>
+      </c>
+      <c r="O41" s="10" t="s">
+        <v>172</v>
+      </c>
+      <c r="P41" s="9">
         <v>7</v>
       </c>
-      <c r="P41" s="18" t="s">
-        <v>120</v>
-      </c>
-      <c r="Q41" s="9"/>
-    </row>
-    <row r="42" spans="1:17">
+      <c r="Q41" s="18" t="s">
+        <v>108</v>
+      </c>
+      <c r="R41" s="9"/>
+    </row>
+    <row r="42" spans="1:18">
       <c r="A42" s="24">
         <v>42</v>
       </c>
@@ -3429,44 +3556,47 @@
         <v>1</v>
       </c>
       <c r="E42" s="10" t="s">
-        <v>207</v>
+        <v>194</v>
       </c>
       <c r="F42" s="10" t="s">
-        <v>215</v>
+        <v>202</v>
       </c>
       <c r="G42" s="10" t="s">
-        <v>194</v>
+        <v>181</v>
       </c>
       <c r="H42" s="10" t="s">
-        <v>115</v>
+        <v>105</v>
       </c>
       <c r="I42" s="10" t="s">
-        <v>211</v>
-      </c>
-      <c r="J42" s="11" t="s">
-        <v>149</v>
-      </c>
-      <c r="K42" s="12" t="s">
-        <v>60</v>
-      </c>
-      <c r="L42" s="13">
-        <v>0</v>
-      </c>
-      <c r="M42" s="14" t="s">
-        <v>121</v>
-      </c>
-      <c r="N42" s="29" t="s">
-        <v>189</v>
-      </c>
-      <c r="O42" s="9">
+        <v>105</v>
+      </c>
+      <c r="J42" s="10" t="s">
+        <v>198</v>
+      </c>
+      <c r="K42" s="11" t="s">
+        <v>136</v>
+      </c>
+      <c r="L42" s="12" t="s">
+        <v>50</v>
+      </c>
+      <c r="M42" s="13">
+        <v>0</v>
+      </c>
+      <c r="N42" s="14" t="s">
+        <v>109</v>
+      </c>
+      <c r="O42" s="29" t="s">
+        <v>176</v>
+      </c>
+      <c r="P42" s="9">
         <v>11</v>
       </c>
-      <c r="P42" s="18" t="s">
-        <v>120</v>
-      </c>
-      <c r="Q42" s="9"/>
-    </row>
-    <row r="43" spans="1:17">
+      <c r="Q42" s="18" t="s">
+        <v>108</v>
+      </c>
+      <c r="R42" s="9"/>
+    </row>
+    <row r="43" spans="1:18">
       <c r="A43" s="24">
         <v>43</v>
       </c>
@@ -3481,44 +3611,47 @@
         <v>1</v>
       </c>
       <c r="E43" s="10" t="s">
-        <v>208</v>
+        <v>195</v>
       </c>
       <c r="F43" s="10" t="s">
-        <v>215</v>
+        <v>202</v>
       </c>
       <c r="G43" s="10" t="s">
-        <v>194</v>
+        <v>181</v>
       </c>
       <c r="H43" s="10" t="s">
-        <v>115</v>
+        <v>105</v>
       </c>
       <c r="I43" s="10" t="s">
-        <v>212</v>
-      </c>
-      <c r="J43" s="11" t="s">
-        <v>150</v>
-      </c>
-      <c r="K43" s="12" t="s">
-        <v>60</v>
-      </c>
-      <c r="L43" s="13">
-        <v>0</v>
-      </c>
-      <c r="M43" s="14" t="s">
-        <v>121</v>
-      </c>
-      <c r="N43" s="29" t="s">
-        <v>189</v>
-      </c>
-      <c r="O43" s="9">
+        <v>105</v>
+      </c>
+      <c r="J43" s="10" t="s">
+        <v>199</v>
+      </c>
+      <c r="K43" s="11" t="s">
+        <v>137</v>
+      </c>
+      <c r="L43" s="12" t="s">
+        <v>50</v>
+      </c>
+      <c r="M43" s="13">
+        <v>0</v>
+      </c>
+      <c r="N43" s="14" t="s">
+        <v>109</v>
+      </c>
+      <c r="O43" s="29" t="s">
+        <v>176</v>
+      </c>
+      <c r="P43" s="9">
         <v>12</v>
       </c>
-      <c r="P43" s="18" t="s">
-        <v>120</v>
-      </c>
-      <c r="Q43" s="9"/>
-    </row>
-    <row r="44" spans="1:17">
+      <c r="Q43" s="18" t="s">
+        <v>108</v>
+      </c>
+      <c r="R43" s="9"/>
+    </row>
+    <row r="44" spans="1:18">
       <c r="A44" s="24">
         <v>44</v>
       </c>
@@ -3533,44 +3666,47 @@
         <v>1</v>
       </c>
       <c r="E44" s="10" t="s">
-        <v>209</v>
+        <v>196</v>
       </c>
       <c r="F44" s="10" t="s">
-        <v>215</v>
+        <v>202</v>
       </c>
       <c r="G44" s="10" t="s">
-        <v>194</v>
+        <v>181</v>
       </c>
       <c r="H44" s="10" t="s">
-        <v>115</v>
-      </c>
-      <c r="I44" s="12" t="s">
-        <v>214</v>
-      </c>
-      <c r="J44" s="11" t="s">
-        <v>151</v>
-      </c>
-      <c r="K44" s="12" t="s">
-        <v>60</v>
-      </c>
-      <c r="L44" s="13">
-        <v>0</v>
-      </c>
-      <c r="M44" s="14" t="s">
-        <v>121</v>
-      </c>
-      <c r="N44" s="33" t="s">
-        <v>136</v>
-      </c>
-      <c r="O44" s="9">
+        <v>105</v>
+      </c>
+      <c r="I44" s="10" t="s">
+        <v>105</v>
+      </c>
+      <c r="J44" s="12" t="s">
+        <v>201</v>
+      </c>
+      <c r="K44" s="11" t="s">
+        <v>138</v>
+      </c>
+      <c r="L44" s="12" t="s">
+        <v>50</v>
+      </c>
+      <c r="M44" s="13">
+        <v>0</v>
+      </c>
+      <c r="N44" s="14" t="s">
+        <v>109</v>
+      </c>
+      <c r="O44" s="33" t="s">
+        <v>123</v>
+      </c>
+      <c r="P44" s="9">
         <v>9</v>
       </c>
-      <c r="P44" s="18" t="s">
-        <v>120</v>
-      </c>
-      <c r="Q44" s="9"/>
-    </row>
-    <row r="45" spans="1:17">
+      <c r="Q44" s="18" t="s">
+        <v>108</v>
+      </c>
+      <c r="R44" s="9"/>
+    </row>
+    <row r="45" spans="1:18">
       <c r="A45" s="24">
         <v>45</v>
       </c>
@@ -3585,44 +3721,47 @@
         <v>1</v>
       </c>
       <c r="E45" s="10" t="s">
-        <v>210</v>
+        <v>197</v>
       </c>
       <c r="F45" s="10" t="s">
-        <v>215</v>
+        <v>202</v>
       </c>
       <c r="G45" s="10" t="s">
-        <v>194</v>
+        <v>181</v>
       </c>
       <c r="H45" s="10" t="s">
-        <v>115</v>
+        <v>105</v>
       </c>
       <c r="I45" s="10" t="s">
-        <v>213</v>
-      </c>
-      <c r="J45" s="11" t="s">
-        <v>152</v>
-      </c>
-      <c r="K45" s="12" t="s">
-        <v>60</v>
-      </c>
-      <c r="L45" s="13">
-        <v>0</v>
-      </c>
-      <c r="M45" s="14" t="s">
-        <v>121</v>
-      </c>
-      <c r="N45" s="34" t="s">
-        <v>136</v>
-      </c>
-      <c r="O45" s="9">
+        <v>105</v>
+      </c>
+      <c r="J45" s="10" t="s">
+        <v>200</v>
+      </c>
+      <c r="K45" s="11" t="s">
+        <v>139</v>
+      </c>
+      <c r="L45" s="12" t="s">
+        <v>50</v>
+      </c>
+      <c r="M45" s="13">
+        <v>0</v>
+      </c>
+      <c r="N45" s="14" t="s">
+        <v>109</v>
+      </c>
+      <c r="O45" s="34" t="s">
+        <v>123</v>
+      </c>
+      <c r="P45" s="9">
         <v>10</v>
       </c>
-      <c r="P45" s="18" t="s">
-        <v>120</v>
-      </c>
-      <c r="Q45" s="9"/>
-    </row>
-    <row r="46" spans="1:17" ht="19" customHeight="1">
+      <c r="Q45" s="18" t="s">
+        <v>108</v>
+      </c>
+      <c r="R45" s="9"/>
+    </row>
+    <row r="46" spans="1:18" ht="19" customHeight="1">
       <c r="A46" s="24">
         <v>46</v>
       </c>
@@ -3637,44 +3776,47 @@
         <v>1</v>
       </c>
       <c r="E46" s="25" t="s">
-        <v>79</v>
+        <v>69</v>
       </c>
       <c r="F46" s="25" t="s">
-        <v>216</v>
+        <v>203</v>
       </c>
       <c r="G46" s="25" t="s">
-        <v>193</v>
+        <v>180</v>
       </c>
       <c r="H46" s="25" t="s">
-        <v>115</v>
+        <v>105</v>
       </c>
       <c r="I46" s="25" t="s">
-        <v>80</v>
-      </c>
-      <c r="J46" s="26" t="s">
-        <v>153</v>
-      </c>
-      <c r="K46" s="24" t="s">
-        <v>110</v>
-      </c>
-      <c r="L46" s="27">
-        <v>0</v>
-      </c>
-      <c r="M46" s="32" t="s">
-        <v>121</v>
-      </c>
-      <c r="N46" s="35" t="s">
-        <v>186</v>
-      </c>
-      <c r="O46" s="30">
+        <v>105</v>
+      </c>
+      <c r="J46" s="25" t="s">
+        <v>70</v>
+      </c>
+      <c r="K46" s="26" t="s">
+        <v>140</v>
+      </c>
+      <c r="L46" s="24" t="s">
+        <v>100</v>
+      </c>
+      <c r="M46" s="27">
+        <v>0</v>
+      </c>
+      <c r="N46" s="32" t="s">
+        <v>109</v>
+      </c>
+      <c r="O46" s="35" t="s">
+        <v>173</v>
+      </c>
+      <c r="P46" s="30">
         <v>41</v>
       </c>
-      <c r="P46" s="31" t="s">
-        <v>120</v>
-      </c>
-      <c r="Q46" s="17"/>
-    </row>
-    <row r="47" spans="1:17">
+      <c r="Q46" s="31" t="s">
+        <v>108</v>
+      </c>
+      <c r="R46" s="17"/>
+    </row>
+    <row r="47" spans="1:18">
       <c r="A47" s="24">
         <v>47</v>
       </c>
@@ -3689,44 +3831,47 @@
         <v>1</v>
       </c>
       <c r="E47" s="25" t="s">
-        <v>81</v>
+        <v>71</v>
       </c>
       <c r="F47" s="25" t="s">
-        <v>198</v>
+        <v>185</v>
       </c>
       <c r="G47" s="25" t="s">
+        <v>106</v>
+      </c>
+      <c r="H47" s="25" t="s">
+        <v>106</v>
+      </c>
+      <c r="I47" s="25" t="s">
+        <v>106</v>
+      </c>
+      <c r="J47" s="25" t="s">
+        <v>72</v>
+      </c>
+      <c r="K47" s="26" t="s">
+        <v>156</v>
+      </c>
+      <c r="L47" s="24" t="s">
+        <v>100</v>
+      </c>
+      <c r="M47" s="27">
+        <v>0</v>
+      </c>
+      <c r="N47" s="32" t="s">
         <v>116</v>
       </c>
-      <c r="H47" s="25" t="s">
-        <v>116</v>
-      </c>
-      <c r="I47" s="25" t="s">
-        <v>82</v>
-      </c>
-      <c r="J47" s="26" t="s">
-        <v>169</v>
-      </c>
-      <c r="K47" s="24" t="s">
-        <v>110</v>
-      </c>
-      <c r="L47" s="27">
-        <v>0</v>
-      </c>
-      <c r="M47" s="32" t="s">
-        <v>129</v>
-      </c>
-      <c r="N47" s="35" t="s">
-        <v>186</v>
-      </c>
-      <c r="O47" s="30">
+      <c r="O47" s="35" t="s">
+        <v>173</v>
+      </c>
+      <c r="P47" s="30">
         <v>42</v>
       </c>
-      <c r="P47" s="31" t="s">
-        <v>120</v>
-      </c>
-      <c r="Q47" s="17"/>
-    </row>
-    <row r="48" spans="1:17">
+      <c r="Q47" s="31" t="s">
+        <v>108</v>
+      </c>
+      <c r="R47" s="17"/>
+    </row>
+    <row r="48" spans="1:18">
       <c r="A48" s="24">
         <v>48</v>
       </c>
@@ -3741,44 +3886,47 @@
         <v>1</v>
       </c>
       <c r="E48" s="25" t="s">
-        <v>83</v>
+        <v>73</v>
       </c>
       <c r="F48" s="25" t="s">
-        <v>216</v>
+        <v>203</v>
       </c>
       <c r="G48" s="25" t="s">
-        <v>193</v>
+        <v>180</v>
       </c>
       <c r="H48" s="25" t="s">
-        <v>115</v>
+        <v>105</v>
       </c>
       <c r="I48" s="25" t="s">
-        <v>84</v>
-      </c>
-      <c r="J48" s="26" t="s">
-        <v>154</v>
-      </c>
-      <c r="K48" s="24" t="s">
-        <v>110</v>
-      </c>
-      <c r="L48" s="27">
-        <v>0</v>
-      </c>
-      <c r="M48" s="32" t="s">
-        <v>121</v>
-      </c>
-      <c r="N48" s="36" t="s">
-        <v>187</v>
-      </c>
-      <c r="O48" s="30">
+        <v>105</v>
+      </c>
+      <c r="J48" s="25" t="s">
+        <v>74</v>
+      </c>
+      <c r="K48" s="26" t="s">
+        <v>141</v>
+      </c>
+      <c r="L48" s="24" t="s">
+        <v>100</v>
+      </c>
+      <c r="M48" s="27">
+        <v>0</v>
+      </c>
+      <c r="N48" s="32" t="s">
+        <v>109</v>
+      </c>
+      <c r="O48" s="36" t="s">
+        <v>174</v>
+      </c>
+      <c r="P48" s="30">
         <v>37</v>
       </c>
-      <c r="P48" s="31" t="s">
-        <v>120</v>
-      </c>
-      <c r="Q48" s="17"/>
-    </row>
-    <row r="49" spans="1:18">
+      <c r="Q48" s="31" t="s">
+        <v>108</v>
+      </c>
+      <c r="R48" s="17"/>
+    </row>
+    <row r="49" spans="1:19">
       <c r="A49" s="24">
         <v>49</v>
       </c>
@@ -3793,44 +3941,47 @@
         <v>1</v>
       </c>
       <c r="E49" s="25" t="s">
-        <v>85</v>
+        <v>75</v>
       </c>
       <c r="F49" s="25" t="s">
-        <v>198</v>
+        <v>185</v>
       </c>
       <c r="G49" s="25" t="s">
+        <v>106</v>
+      </c>
+      <c r="H49" s="25" t="s">
+        <v>106</v>
+      </c>
+      <c r="I49" s="25" t="s">
+        <v>106</v>
+      </c>
+      <c r="J49" s="25" t="s">
+        <v>76</v>
+      </c>
+      <c r="K49" s="26" t="s">
+        <v>157</v>
+      </c>
+      <c r="L49" s="24" t="s">
+        <v>100</v>
+      </c>
+      <c r="M49" s="27">
+        <v>1</v>
+      </c>
+      <c r="N49" s="32" t="s">
         <v>116</v>
       </c>
-      <c r="H49" s="25" t="s">
-        <v>116</v>
-      </c>
-      <c r="I49" s="25" t="s">
-        <v>86</v>
-      </c>
-      <c r="J49" s="26" t="s">
-        <v>170</v>
-      </c>
-      <c r="K49" s="24" t="s">
-        <v>110</v>
-      </c>
-      <c r="L49" s="27">
-        <v>1</v>
-      </c>
-      <c r="M49" s="32" t="s">
-        <v>129</v>
-      </c>
-      <c r="N49" s="36" t="s">
-        <v>187</v>
-      </c>
-      <c r="O49" s="30">
+      <c r="O49" s="36" t="s">
+        <v>174</v>
+      </c>
+      <c r="P49" s="30">
         <v>38</v>
       </c>
-      <c r="P49" s="31" t="s">
-        <v>120</v>
-      </c>
-      <c r="Q49" s="17"/>
-    </row>
-    <row r="50" spans="1:18" ht="17" customHeight="1">
+      <c r="Q49" s="31" t="s">
+        <v>108</v>
+      </c>
+      <c r="R49" s="17"/>
+    </row>
+    <row r="50" spans="1:19" ht="17" customHeight="1">
       <c r="A50" s="24">
         <v>50</v>
       </c>
@@ -3845,44 +3996,47 @@
         <v>1</v>
       </c>
       <c r="E50" s="10" t="s">
-        <v>88</v>
+        <v>78</v>
       </c>
       <c r="F50" s="10" t="s">
-        <v>200</v>
+        <v>187</v>
       </c>
       <c r="G50" s="10" t="s">
-        <v>196</v>
+        <v>183</v>
       </c>
       <c r="H50" s="10" t="s">
-        <v>114</v>
+        <v>104</v>
       </c>
       <c r="I50" s="10" t="s">
-        <v>89</v>
-      </c>
-      <c r="J50" s="11" t="s">
-        <v>206</v>
-      </c>
-      <c r="K50" s="12" t="s">
-        <v>87</v>
-      </c>
-      <c r="L50" s="13">
-        <v>0</v>
-      </c>
-      <c r="M50" s="14" t="s">
-        <v>123</v>
-      </c>
-      <c r="N50" s="35" t="s">
-        <v>186</v>
-      </c>
-      <c r="O50" s="9">
+        <v>104</v>
+      </c>
+      <c r="J50" s="10" t="s">
+        <v>79</v>
+      </c>
+      <c r="K50" s="11" t="s">
+        <v>193</v>
+      </c>
+      <c r="L50" s="12" t="s">
+        <v>77</v>
+      </c>
+      <c r="M50" s="13">
+        <v>0</v>
+      </c>
+      <c r="N50" s="14" t="s">
+        <v>111</v>
+      </c>
+      <c r="O50" s="35" t="s">
+        <v>173</v>
+      </c>
+      <c r="P50" s="9">
         <v>48</v>
       </c>
-      <c r="P50" s="18" t="s">
-        <v>120</v>
-      </c>
-      <c r="Q50" s="9"/>
-    </row>
-    <row r="51" spans="1:18">
+      <c r="Q50" s="18" t="s">
+        <v>108</v>
+      </c>
+      <c r="R50" s="9"/>
+    </row>
+    <row r="51" spans="1:19">
       <c r="A51" s="24">
         <v>51</v>
       </c>
@@ -3897,46 +4051,49 @@
         <v>1</v>
       </c>
       <c r="E51" s="10" t="s">
-        <v>90</v>
+        <v>80</v>
       </c>
       <c r="F51" s="10" t="s">
-        <v>200</v>
+        <v>187</v>
       </c>
       <c r="G51" s="10" t="s">
-        <v>196</v>
+        <v>183</v>
       </c>
       <c r="H51" s="10" t="s">
-        <v>114</v>
+        <v>104</v>
       </c>
       <c r="I51" s="10" t="s">
-        <v>91</v>
-      </c>
-      <c r="J51" s="11" t="s">
-        <v>180</v>
-      </c>
-      <c r="K51" s="12" t="s">
-        <v>87</v>
-      </c>
-      <c r="L51" s="13">
-        <v>0</v>
-      </c>
-      <c r="M51" s="14" t="s">
-        <v>123</v>
-      </c>
-      <c r="N51" s="35" t="s">
-        <v>186</v>
-      </c>
-      <c r="O51" s="9">
+        <v>104</v>
+      </c>
+      <c r="J51" s="10" t="s">
+        <v>81</v>
+      </c>
+      <c r="K51" s="11" t="s">
+        <v>167</v>
+      </c>
+      <c r="L51" s="12" t="s">
+        <v>77</v>
+      </c>
+      <c r="M51" s="13">
+        <v>0</v>
+      </c>
+      <c r="N51" s="14" t="s">
+        <v>111</v>
+      </c>
+      <c r="O51" s="35" t="s">
+        <v>173</v>
+      </c>
+      <c r="P51" s="9">
         <v>44</v>
       </c>
-      <c r="P51" s="18" t="s">
-        <v>120</v>
-      </c>
-      <c r="Q51" s="9" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="52" spans="1:18">
+      <c r="Q51" s="18" t="s">
+        <v>108</v>
+      </c>
+      <c r="R51" s="9" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="52" spans="1:19">
       <c r="A52" s="24">
         <v>52</v>
       </c>
@@ -3951,44 +4108,47 @@
         <v>1</v>
       </c>
       <c r="E52" s="10" t="s">
-        <v>92</v>
+        <v>82</v>
       </c>
       <c r="F52" s="10" t="s">
-        <v>200</v>
+        <v>187</v>
       </c>
       <c r="G52" s="10" t="s">
-        <v>196</v>
+        <v>183</v>
       </c>
       <c r="H52" s="10" t="s">
-        <v>114</v>
+        <v>104</v>
       </c>
       <c r="I52" s="10" t="s">
-        <v>93</v>
-      </c>
-      <c r="J52" s="11" t="s">
-        <v>155</v>
-      </c>
-      <c r="K52" s="12" t="s">
-        <v>87</v>
-      </c>
-      <c r="L52" s="13">
-        <v>0</v>
-      </c>
-      <c r="M52" s="14" t="s">
-        <v>123</v>
-      </c>
-      <c r="N52" s="36" t="s">
-        <v>187</v>
-      </c>
-      <c r="O52" s="9">
+        <v>104</v>
+      </c>
+      <c r="J52" s="10" t="s">
+        <v>83</v>
+      </c>
+      <c r="K52" s="11" t="s">
+        <v>142</v>
+      </c>
+      <c r="L52" s="12" t="s">
+        <v>77</v>
+      </c>
+      <c r="M52" s="13">
+        <v>0</v>
+      </c>
+      <c r="N52" s="14" t="s">
+        <v>111</v>
+      </c>
+      <c r="O52" s="36" t="s">
+        <v>174</v>
+      </c>
+      <c r="P52" s="9">
         <v>46</v>
       </c>
-      <c r="P52" s="18" t="s">
-        <v>120</v>
-      </c>
-      <c r="Q52" s="9"/>
-    </row>
-    <row r="53" spans="1:18">
+      <c r="Q52" s="18" t="s">
+        <v>108</v>
+      </c>
+      <c r="R52" s="9"/>
+    </row>
+    <row r="53" spans="1:19">
       <c r="A53" s="24">
         <v>53</v>
       </c>
@@ -4003,46 +4163,49 @@
         <v>1</v>
       </c>
       <c r="E53" s="10" t="s">
-        <v>94</v>
+        <v>84</v>
       </c>
       <c r="F53" s="10" t="s">
-        <v>200</v>
+        <v>187</v>
       </c>
       <c r="G53" s="10" t="s">
-        <v>196</v>
+        <v>183</v>
       </c>
       <c r="H53" s="10" t="s">
-        <v>114</v>
+        <v>104</v>
       </c>
       <c r="I53" s="10" t="s">
-        <v>95</v>
-      </c>
-      <c r="J53" s="11" t="s">
-        <v>181</v>
-      </c>
-      <c r="K53" s="12" t="s">
-        <v>87</v>
-      </c>
-      <c r="L53" s="13">
-        <v>0</v>
-      </c>
-      <c r="M53" s="14" t="s">
-        <v>123</v>
-      </c>
-      <c r="N53" s="36" t="s">
-        <v>187</v>
-      </c>
-      <c r="O53" s="9">
+        <v>104</v>
+      </c>
+      <c r="J53" s="10" t="s">
+        <v>85</v>
+      </c>
+      <c r="K53" s="11" t="s">
+        <v>168</v>
+      </c>
+      <c r="L53" s="12" t="s">
+        <v>77</v>
+      </c>
+      <c r="M53" s="13">
+        <v>0</v>
+      </c>
+      <c r="N53" s="14" t="s">
+        <v>111</v>
+      </c>
+      <c r="O53" s="36" t="s">
+        <v>174</v>
+      </c>
+      <c r="P53" s="9">
         <v>40</v>
       </c>
-      <c r="P53" s="18" t="s">
-        <v>120</v>
-      </c>
-      <c r="Q53" s="9" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="54" spans="1:18">
+      <c r="Q53" s="18" t="s">
+        <v>108</v>
+      </c>
+      <c r="R53" s="9" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="54" spans="1:19">
       <c r="A54" s="24">
         <v>54</v>
       </c>
@@ -4057,40 +4220,43 @@
         <v>1</v>
       </c>
       <c r="E54" s="10" t="s">
-        <v>96</v>
+        <v>86</v>
       </c>
       <c r="F54" s="10"/>
       <c r="G54" s="10"/>
       <c r="H54" s="10" t="s">
-        <v>115</v>
+        <v>105</v>
       </c>
       <c r="I54" s="10" t="s">
-        <v>97</v>
-      </c>
-      <c r="J54" s="11" t="s">
-        <v>182</v>
-      </c>
-      <c r="K54" s="12" t="s">
+        <v>105</v>
+      </c>
+      <c r="J54" s="10" t="s">
         <v>87</v>
       </c>
-      <c r="L54" s="13">
-        <v>0</v>
-      </c>
-      <c r="M54" s="14" t="s">
-        <v>121</v>
-      </c>
-      <c r="N54" s="36" t="s">
-        <v>187</v>
-      </c>
-      <c r="O54" s="9">
+      <c r="K54" s="11" t="s">
+        <v>169</v>
+      </c>
+      <c r="L54" s="12" t="s">
+        <v>77</v>
+      </c>
+      <c r="M54" s="13">
+        <v>0</v>
+      </c>
+      <c r="N54" s="14" t="s">
+        <v>109</v>
+      </c>
+      <c r="O54" s="36" t="s">
+        <v>174</v>
+      </c>
+      <c r="P54" s="9">
         <v>45</v>
       </c>
-      <c r="P54" s="18" t="s">
-        <v>120</v>
-      </c>
-      <c r="Q54" s="9"/>
-    </row>
-    <row r="55" spans="1:18">
+      <c r="Q54" s="18" t="s">
+        <v>108</v>
+      </c>
+      <c r="R54" s="9"/>
+    </row>
+    <row r="55" spans="1:19">
       <c r="A55" s="24">
         <v>55</v>
       </c>
@@ -4105,40 +4271,43 @@
         <v>1</v>
       </c>
       <c r="E55" s="10" t="s">
-        <v>98</v>
+        <v>88</v>
       </c>
       <c r="F55" s="10"/>
       <c r="G55" s="10"/>
       <c r="H55" s="10" t="s">
-        <v>115</v>
+        <v>105</v>
       </c>
       <c r="I55" s="10" t="s">
-        <v>99</v>
-      </c>
-      <c r="J55" s="11" t="s">
-        <v>203</v>
-      </c>
-      <c r="K55" s="12" t="s">
-        <v>87</v>
-      </c>
-      <c r="L55" s="13">
-        <v>0</v>
-      </c>
-      <c r="M55" s="14" t="s">
-        <v>121</v>
-      </c>
-      <c r="N55" s="35" t="s">
-        <v>186</v>
-      </c>
-      <c r="O55" s="9">
+        <v>105</v>
+      </c>
+      <c r="J55" s="10" t="s">
+        <v>89</v>
+      </c>
+      <c r="K55" s="11" t="s">
+        <v>190</v>
+      </c>
+      <c r="L55" s="12" t="s">
+        <v>77</v>
+      </c>
+      <c r="M55" s="13">
+        <v>0</v>
+      </c>
+      <c r="N55" s="14" t="s">
+        <v>109</v>
+      </c>
+      <c r="O55" s="35" t="s">
+        <v>173</v>
+      </c>
+      <c r="P55" s="9">
         <v>47</v>
       </c>
-      <c r="P55" s="18" t="s">
-        <v>120</v>
-      </c>
-      <c r="Q55" s="9"/>
-    </row>
-    <row r="56" spans="1:18">
+      <c r="Q55" s="18" t="s">
+        <v>108</v>
+      </c>
+      <c r="R55" s="9"/>
+    </row>
+    <row r="56" spans="1:19">
       <c r="A56" s="24">
         <v>56</v>
       </c>
@@ -4153,40 +4322,43 @@
         <v>1</v>
       </c>
       <c r="E56" s="10" t="s">
-        <v>100</v>
+        <v>90</v>
       </c>
       <c r="F56" s="10"/>
       <c r="G56" s="10"/>
       <c r="H56" s="10" t="s">
-        <v>114</v>
+        <v>104</v>
       </c>
       <c r="I56" s="10" t="s">
-        <v>101</v>
-      </c>
-      <c r="J56" s="11" t="s">
-        <v>183</v>
-      </c>
-      <c r="K56" s="12" t="s">
-        <v>87</v>
-      </c>
-      <c r="L56" s="13">
-        <v>0</v>
-      </c>
-      <c r="M56" s="14" t="s">
-        <v>123</v>
-      </c>
-      <c r="N56" s="35" t="s">
-        <v>186</v>
-      </c>
-      <c r="O56" s="9">
+        <v>104</v>
+      </c>
+      <c r="J56" s="10" t="s">
+        <v>91</v>
+      </c>
+      <c r="K56" s="11" t="s">
+        <v>170</v>
+      </c>
+      <c r="L56" s="12" t="s">
+        <v>77</v>
+      </c>
+      <c r="M56" s="13">
+        <v>0</v>
+      </c>
+      <c r="N56" s="14" t="s">
+        <v>111</v>
+      </c>
+      <c r="O56" s="35" t="s">
+        <v>173</v>
+      </c>
+      <c r="P56" s="9">
         <v>43</v>
       </c>
-      <c r="P56" s="18" t="s">
-        <v>120</v>
-      </c>
-      <c r="Q56" s="9"/>
-    </row>
-    <row r="57" spans="1:18">
+      <c r="Q56" s="18" t="s">
+        <v>108</v>
+      </c>
+      <c r="R56" s="9"/>
+    </row>
+    <row r="57" spans="1:19">
       <c r="A57" s="24">
         <v>57</v>
       </c>
@@ -4201,40 +4373,43 @@
         <v>1</v>
       </c>
       <c r="E57" s="10" t="s">
-        <v>102</v>
+        <v>92</v>
       </c>
       <c r="F57" s="10"/>
       <c r="G57" s="10"/>
       <c r="H57" s="10" t="s">
-        <v>114</v>
+        <v>104</v>
       </c>
       <c r="I57" s="10" t="s">
-        <v>103</v>
-      </c>
-      <c r="J57" s="11" t="s">
-        <v>184</v>
-      </c>
-      <c r="K57" s="12" t="s">
-        <v>87</v>
-      </c>
-      <c r="L57" s="13">
-        <v>0</v>
-      </c>
-      <c r="M57" s="14" t="s">
-        <v>123</v>
-      </c>
-      <c r="N57" s="36" t="s">
-        <v>187</v>
-      </c>
-      <c r="O57" s="9">
+        <v>104</v>
+      </c>
+      <c r="J57" s="10" t="s">
+        <v>93</v>
+      </c>
+      <c r="K57" s="11" t="s">
+        <v>171</v>
+      </c>
+      <c r="L57" s="12" t="s">
+        <v>77</v>
+      </c>
+      <c r="M57" s="13">
+        <v>0</v>
+      </c>
+      <c r="N57" s="14" t="s">
+        <v>111</v>
+      </c>
+      <c r="O57" s="36" t="s">
+        <v>174</v>
+      </c>
+      <c r="P57" s="9">
         <v>39</v>
       </c>
-      <c r="P57" s="18" t="s">
-        <v>120</v>
-      </c>
-      <c r="Q57" s="9"/>
-    </row>
-    <row r="58" spans="1:18" s="6" customFormat="1">
+      <c r="Q57" s="18" t="s">
+        <v>108</v>
+      </c>
+      <c r="R57" s="9"/>
+    </row>
+    <row r="58" spans="1:19" s="6" customFormat="1">
       <c r="A58" s="37">
         <v>9</v>
       </c>
@@ -4248,43 +4423,46 @@
         <v>0</v>
       </c>
       <c r="E58" s="38" t="s">
-        <v>134</v>
+        <v>121</v>
       </c>
       <c r="F58" s="38" t="s">
-        <v>200</v>
+        <v>187</v>
       </c>
       <c r="G58" s="38" t="s">
-        <v>196</v>
+        <v>183</v>
       </c>
       <c r="H58" s="38" t="s">
-        <v>114</v>
+        <v>104</v>
       </c>
       <c r="I58" s="38" t="s">
-        <v>132</v>
-      </c>
-      <c r="J58" s="7" t="s">
-        <v>205</v>
-      </c>
-      <c r="K58" s="37" t="s">
-        <v>108</v>
-      </c>
-      <c r="L58" s="3">
-        <v>1</v>
-      </c>
-      <c r="M58" s="4" t="s">
-        <v>123</v>
-      </c>
-      <c r="N58" s="39" t="s">
-        <v>188</v>
-      </c>
-      <c r="O58" s="38">
+        <v>104</v>
+      </c>
+      <c r="J58" s="38" t="s">
+        <v>119</v>
+      </c>
+      <c r="K58" s="7" t="s">
+        <v>192</v>
+      </c>
+      <c r="L58" s="37" t="s">
+        <v>98</v>
+      </c>
+      <c r="M58" s="3">
+        <v>1</v>
+      </c>
+      <c r="N58" s="4" t="s">
+        <v>111</v>
+      </c>
+      <c r="O58" s="39" t="s">
+        <v>175</v>
+      </c>
+      <c r="P58" s="38">
         <v>16</v>
       </c>
-      <c r="P58" s="40" t="s">
-        <v>120</v>
-      </c>
-      <c r="Q58" s="20"/>
-      <c r="R58"/>
+      <c r="Q58" s="40" t="s">
+        <v>108</v>
+      </c>
+      <c r="R58" s="20"/>
+      <c r="S58"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
add statistical tests to vignette
</commit_message>
<xml_diff>
--- a/data-raw/params_out.xlsx
+++ b/data-raw/params_out.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/Data/GitHub/grwat/data-raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{DCFA66C9-4920-FC44-B75F-00FAD6FAC267}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{3E7E914F-E12B-CA4A-981F-971799B3035C}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8000" yWindow="1660" windowWidth="28300" windowHeight="14680" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="500" yWindow="1660" windowWidth="28300" windowHeight="14680" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="639" uniqueCount="219">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="640" uniqueCount="220">
   <si>
     <t>year_number</t>
   </si>
@@ -685,6 +685,9 @@
   </si>
   <si>
     <t>Readtype</t>
+  </si>
+  <si>
+    <t>Test</t>
   </si>
 </sst>
 </file>
@@ -893,7 +896,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="42">
+  <cellXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1006,6 +1009,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -1296,10 +1302,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:S58"/>
+  <dimension ref="A1:T58"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="81" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="J3" sqref="J3"/>
+      <selection activeCell="K30" sqref="K30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16"/>
@@ -1313,18 +1319,19 @@
     <col min="7" max="7" width="8.1640625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="10.5" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="7.5" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="75.6640625" customWidth="1"/>
-    <col min="11" max="11" width="61.6640625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="34.33203125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="7.5" style="2" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="6.5" style="2" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="14.1640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="6.83203125" style="2" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="11.6640625" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="50.83203125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="7.5" customWidth="1"/>
+    <col min="11" max="11" width="75.6640625" customWidth="1"/>
+    <col min="12" max="12" width="61.6640625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="34.33203125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="7.5" style="2" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="6.5" style="2" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="14.1640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="6.83203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="50.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" s="1" customFormat="1" ht="19" customHeight="1">
+    <row r="1" spans="1:20" s="1" customFormat="1" ht="19" customHeight="1">
       <c r="A1" s="15" t="s">
         <v>95</v>
       </c>
@@ -1353,34 +1360,37 @@
         <v>103</v>
       </c>
       <c r="J1" s="15" t="s">
+        <v>219</v>
+      </c>
+      <c r="K1" s="15" t="s">
         <v>177</v>
       </c>
-      <c r="K1" s="15" t="s">
+      <c r="L1" s="15" t="s">
         <v>143</v>
       </c>
-      <c r="L1" s="15" t="s">
+      <c r="M1" s="15" t="s">
         <v>94</v>
       </c>
-      <c r="M1" s="15" t="s">
+      <c r="N1" s="15" t="s">
         <v>107</v>
       </c>
-      <c r="N1" s="15" t="s">
+      <c r="O1" s="15" t="s">
         <v>110</v>
       </c>
-      <c r="O1" s="15" t="s">
+      <c r="P1" s="15" t="s">
         <v>118</v>
       </c>
-      <c r="P1" s="15" t="s">
+      <c r="Q1" s="15" t="s">
         <v>117</v>
       </c>
-      <c r="Q1" s="16" t="s">
+      <c r="R1" s="16" t="s">
         <v>217</v>
       </c>
-      <c r="R1" s="8" t="s">
+      <c r="S1" s="8" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="2" spans="1:19" ht="17" customHeight="1">
+    <row r="2" spans="1:20" ht="17" customHeight="1">
       <c r="A2" s="12">
         <v>1</v>
       </c>
@@ -1404,33 +1414,36 @@
       <c r="I2" s="10" t="s">
         <v>104</v>
       </c>
-      <c r="J2" s="10" t="s">
-        <v>1</v>
-      </c>
-      <c r="K2" s="11" t="s">
+      <c r="J2" s="10">
+        <v>0</v>
+      </c>
+      <c r="K2" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="L2" s="11" t="s">
         <v>153</v>
       </c>
-      <c r="L2" s="12" t="s">
+      <c r="M2" s="12" t="s">
         <v>98</v>
       </c>
-      <c r="M2" s="13">
-        <v>0</v>
-      </c>
-      <c r="N2" s="14" t="s">
+      <c r="N2" s="13">
+        <v>0</v>
+      </c>
+      <c r="O2" s="14" t="s">
         <v>112</v>
       </c>
-      <c r="O2" s="17" t="s">
+      <c r="P2" s="17" t="s">
         <v>122</v>
       </c>
-      <c r="P2" s="9">
-        <v>0</v>
-      </c>
-      <c r="Q2" s="18" t="s">
-        <v>108</v>
-      </c>
-      <c r="R2" s="9"/>
-    </row>
-    <row r="3" spans="1:19">
+      <c r="Q2" s="9">
+        <v>0</v>
+      </c>
+      <c r="R2" s="18" t="s">
+        <v>108</v>
+      </c>
+      <c r="S2" s="9"/>
+    </row>
+    <row r="3" spans="1:20">
       <c r="A3" s="12">
         <v>2</v>
       </c>
@@ -1458,33 +1471,36 @@
       <c r="I3" s="10" t="s">
         <v>104</v>
       </c>
-      <c r="J3" s="10" t="s">
+      <c r="J3" s="10">
+        <v>0</v>
+      </c>
+      <c r="K3" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="K3" s="11" t="s">
+      <c r="L3" s="11" t="s">
         <v>188</v>
       </c>
-      <c r="L3" s="12" t="s">
+      <c r="M3" s="12" t="s">
         <v>98</v>
       </c>
-      <c r="M3" s="13">
-        <v>0</v>
-      </c>
-      <c r="N3" s="14" t="s">
+      <c r="N3" s="13">
+        <v>0</v>
+      </c>
+      <c r="O3" s="14" t="s">
         <v>112</v>
       </c>
-      <c r="O3" s="17" t="s">
+      <c r="P3" s="17" t="s">
         <v>122</v>
       </c>
-      <c r="P3" s="9">
-        <v>0</v>
-      </c>
-      <c r="Q3" s="18" t="s">
-        <v>108</v>
-      </c>
-      <c r="R3" s="9"/>
-    </row>
-    <row r="4" spans="1:19">
+      <c r="Q3" s="9">
+        <v>0</v>
+      </c>
+      <c r="R3" s="18" t="s">
+        <v>108</v>
+      </c>
+      <c r="S3" s="9"/>
+    </row>
+    <row r="4" spans="1:20">
       <c r="A4" s="12">
         <v>3</v>
       </c>
@@ -1512,33 +1528,36 @@
       <c r="I4" s="10" t="s">
         <v>104</v>
       </c>
-      <c r="J4" s="10" t="s">
+      <c r="J4" s="10">
+        <v>0</v>
+      </c>
+      <c r="K4" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="K4" s="11" t="s">
+      <c r="L4" s="11" t="s">
         <v>189</v>
       </c>
-      <c r="L4" s="12" t="s">
+      <c r="M4" s="12" t="s">
         <v>98</v>
       </c>
-      <c r="M4" s="13">
-        <v>0</v>
-      </c>
-      <c r="N4" s="14" t="s">
+      <c r="N4" s="13">
+        <v>0</v>
+      </c>
+      <c r="O4" s="14" t="s">
         <v>112</v>
       </c>
-      <c r="O4" s="17" t="s">
+      <c r="P4" s="17" t="s">
         <v>122</v>
       </c>
-      <c r="P4" s="9">
-        <v>0</v>
-      </c>
-      <c r="Q4" s="18" t="s">
-        <v>108</v>
-      </c>
-      <c r="R4" s="9"/>
-    </row>
-    <row r="5" spans="1:19">
+      <c r="Q4" s="9">
+        <v>0</v>
+      </c>
+      <c r="R4" s="18" t="s">
+        <v>108</v>
+      </c>
+      <c r="S4" s="9"/>
+    </row>
+    <row r="5" spans="1:20">
       <c r="A5" s="12">
         <v>4</v>
       </c>
@@ -1566,33 +1585,36 @@
       <c r="I5" s="10" t="s">
         <v>106</v>
       </c>
-      <c r="J5" s="10" t="s">
+      <c r="J5" s="10">
+        <v>1</v>
+      </c>
+      <c r="K5" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="K5" s="11" t="s">
+      <c r="L5" s="11" t="s">
         <v>154</v>
       </c>
-      <c r="L5" s="12" t="s">
+      <c r="M5" s="12" t="s">
         <v>98</v>
       </c>
-      <c r="M5" s="13">
+      <c r="N5" s="13">
         <v>2</v>
       </c>
-      <c r="N5" s="14" t="s">
+      <c r="O5" s="14" t="s">
         <v>116</v>
       </c>
-      <c r="O5" s="19" t="s">
+      <c r="P5" s="19" t="s">
         <v>175</v>
       </c>
-      <c r="P5" s="9">
+      <c r="Q5" s="9">
         <v>14</v>
       </c>
-      <c r="Q5" s="18" t="s">
-        <v>108</v>
-      </c>
-      <c r="R5" s="9"/>
-    </row>
-    <row r="6" spans="1:19">
+      <c r="R5" s="18" t="s">
+        <v>108</v>
+      </c>
+      <c r="S5" s="9"/>
+    </row>
+    <row r="6" spans="1:20">
       <c r="A6" s="12">
         <v>5</v>
       </c>
@@ -1620,33 +1642,36 @@
       <c r="I6" s="10" t="s">
         <v>106</v>
       </c>
-      <c r="J6" s="10" t="s">
+      <c r="J6" s="10">
+        <v>1</v>
+      </c>
+      <c r="K6" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="K6" s="11" t="s">
+      <c r="L6" s="11" t="s">
         <v>155</v>
       </c>
-      <c r="L6" s="12" t="s">
+      <c r="M6" s="12" t="s">
         <v>98</v>
       </c>
-      <c r="M6" s="13">
+      <c r="N6" s="13">
         <v>2</v>
       </c>
-      <c r="N6" s="14" t="s">
+      <c r="O6" s="14" t="s">
         <v>116</v>
       </c>
-      <c r="O6" s="19" t="s">
+      <c r="P6" s="19" t="s">
         <v>175</v>
       </c>
-      <c r="P6" s="9">
+      <c r="Q6" s="9">
         <v>16</v>
       </c>
-      <c r="Q6" s="18" t="s">
-        <v>108</v>
-      </c>
-      <c r="R6" s="9"/>
-    </row>
-    <row r="7" spans="1:19">
+      <c r="R6" s="18" t="s">
+        <v>108</v>
+      </c>
+      <c r="S6" s="9"/>
+    </row>
+    <row r="7" spans="1:20">
       <c r="A7" s="12">
         <v>6</v>
       </c>
@@ -1674,33 +1699,36 @@
       <c r="I7" s="10" t="s">
         <v>105</v>
       </c>
-      <c r="J7" s="10" t="s">
+      <c r="J7" s="10">
+        <v>1</v>
+      </c>
+      <c r="K7" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="K7" s="11" t="s">
+      <c r="L7" s="11" t="s">
         <v>124</v>
       </c>
-      <c r="L7" s="12" t="s">
+      <c r="M7" s="12" t="s">
         <v>98</v>
       </c>
-      <c r="M7" s="13">
-        <v>0</v>
-      </c>
-      <c r="N7" s="14" t="s">
+      <c r="N7" s="13">
+        <v>0</v>
+      </c>
+      <c r="O7" s="14" t="s">
         <v>109</v>
       </c>
-      <c r="O7" s="10" t="s">
+      <c r="P7" s="10" t="s">
         <v>172</v>
       </c>
-      <c r="P7" s="9">
+      <c r="Q7" s="9">
         <v>13</v>
       </c>
-      <c r="Q7" s="18" t="s">
-        <v>108</v>
-      </c>
-      <c r="R7" s="9"/>
-    </row>
-    <row r="8" spans="1:19">
+      <c r="R7" s="18" t="s">
+        <v>108</v>
+      </c>
+      <c r="S7" s="9"/>
+    </row>
+    <row r="8" spans="1:20">
       <c r="A8" s="12">
         <v>7</v>
       </c>
@@ -1728,33 +1756,36 @@
       <c r="I8" s="10" t="s">
         <v>105</v>
       </c>
-      <c r="J8" s="10" t="s">
+      <c r="J8" s="10">
+        <v>1</v>
+      </c>
+      <c r="K8" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="K8" s="11" t="s">
+      <c r="L8" s="11" t="s">
         <v>125</v>
       </c>
-      <c r="L8" s="12" t="s">
+      <c r="M8" s="12" t="s">
         <v>98</v>
       </c>
-      <c r="M8" s="13">
-        <v>0</v>
-      </c>
-      <c r="N8" s="14" t="s">
+      <c r="N8" s="13">
+        <v>0</v>
+      </c>
+      <c r="O8" s="14" t="s">
         <v>109</v>
       </c>
-      <c r="O8" s="19" t="s">
+      <c r="P8" s="19" t="s">
         <v>175</v>
       </c>
-      <c r="P8" s="9">
+      <c r="Q8" s="9">
         <v>17</v>
       </c>
-      <c r="Q8" s="18" t="s">
-        <v>108</v>
-      </c>
-      <c r="R8" s="9"/>
-    </row>
-    <row r="9" spans="1:19">
+      <c r="R8" s="18" t="s">
+        <v>108</v>
+      </c>
+      <c r="S8" s="9"/>
+    </row>
+    <row r="9" spans="1:20">
       <c r="A9" s="12">
         <v>8</v>
       </c>
@@ -1782,33 +1813,36 @@
       <c r="I9" s="10" t="s">
         <v>106</v>
       </c>
-      <c r="J9" s="10" t="s">
+      <c r="J9" s="10">
+        <v>1</v>
+      </c>
+      <c r="K9" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="K9" s="11" t="s">
+      <c r="L9" s="11" t="s">
         <v>152</v>
       </c>
-      <c r="L9" s="12" t="s">
+      <c r="M9" s="12" t="s">
         <v>98</v>
       </c>
-      <c r="M9" s="13">
+      <c r="N9" s="13">
         <v>2</v>
       </c>
-      <c r="N9" s="14" t="s">
+      <c r="O9" s="14" t="s">
         <v>116</v>
       </c>
-      <c r="O9" s="19" t="s">
+      <c r="P9" s="19" t="s">
         <v>175</v>
       </c>
-      <c r="P9" s="9">
+      <c r="Q9" s="9">
         <v>18</v>
       </c>
-      <c r="Q9" s="18" t="s">
-        <v>108</v>
-      </c>
-      <c r="R9" s="9"/>
-    </row>
-    <row r="10" spans="1:19" s="6" customFormat="1" ht="19" customHeight="1">
+      <c r="R9" s="18" t="s">
+        <v>108</v>
+      </c>
+      <c r="S9" s="9"/>
+    </row>
+    <row r="10" spans="1:20" s="6" customFormat="1" ht="19" customHeight="1">
       <c r="A10" s="12">
         <v>10</v>
       </c>
@@ -1836,34 +1870,37 @@
       <c r="I10" s="10" t="s">
         <v>105</v>
       </c>
-      <c r="J10" s="10" t="s">
+      <c r="J10" s="10">
+        <v>1</v>
+      </c>
+      <c r="K10" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="K10" s="21" t="s">
+      <c r="L10" s="21" t="s">
         <v>191</v>
       </c>
-      <c r="L10" s="12" t="s">
+      <c r="M10" s="12" t="s">
         <v>98</v>
       </c>
-      <c r="M10" s="22">
-        <v>0</v>
-      </c>
-      <c r="N10" s="23" t="s">
+      <c r="N10" s="22">
+        <v>0</v>
+      </c>
+      <c r="O10" s="23" t="s">
         <v>109</v>
       </c>
-      <c r="O10" s="10" t="s">
+      <c r="P10" s="10" t="s">
         <v>172</v>
       </c>
-      <c r="P10" s="20">
+      <c r="Q10" s="20">
         <v>15</v>
       </c>
-      <c r="Q10" s="18" t="s">
-        <v>108</v>
-      </c>
-      <c r="R10" s="20"/>
-      <c r="S10"/>
-    </row>
-    <row r="11" spans="1:19">
+      <c r="R10" s="18" t="s">
+        <v>108</v>
+      </c>
+      <c r="S10" s="20"/>
+      <c r="T10"/>
+    </row>
+    <row r="11" spans="1:20">
       <c r="A11" s="24">
         <v>11</v>
       </c>
@@ -1891,33 +1928,36 @@
       <c r="I11" s="25" t="s">
         <v>105</v>
       </c>
-      <c r="J11" s="25" t="s">
+      <c r="J11" s="42">
+        <v>1</v>
+      </c>
+      <c r="K11" s="25" t="s">
         <v>19</v>
       </c>
-      <c r="K11" s="26" t="s">
+      <c r="L11" s="26" t="s">
         <v>126</v>
       </c>
-      <c r="L11" s="24" t="s">
+      <c r="M11" s="24" t="s">
         <v>99</v>
       </c>
-      <c r="M11" s="27">
-        <v>0</v>
-      </c>
-      <c r="N11" s="28" t="s">
+      <c r="N11" s="27">
+        <v>0</v>
+      </c>
+      <c r="O11" s="28" t="s">
         <v>109</v>
       </c>
-      <c r="O11" s="29" t="s">
+      <c r="P11" s="29" t="s">
         <v>176</v>
       </c>
-      <c r="P11" s="30">
+      <c r="Q11" s="30">
         <v>23</v>
       </c>
-      <c r="Q11" s="31" t="s">
-        <v>108</v>
-      </c>
-      <c r="R11" s="17"/>
-    </row>
-    <row r="12" spans="1:19">
+      <c r="R11" s="31" t="s">
+        <v>108</v>
+      </c>
+      <c r="S11" s="17"/>
+    </row>
+    <row r="12" spans="1:20">
       <c r="A12" s="24">
         <v>12</v>
       </c>
@@ -1945,35 +1985,38 @@
       <c r="I12" s="41" t="s">
         <v>106</v>
       </c>
-      <c r="J12" s="25" t="s">
+      <c r="J12" s="42">
+        <v>1</v>
+      </c>
+      <c r="K12" s="25" t="s">
         <v>21</v>
       </c>
-      <c r="K12" s="26" t="s">
+      <c r="L12" s="26" t="s">
         <v>149</v>
       </c>
-      <c r="L12" s="24" t="s">
+      <c r="M12" s="24" t="s">
         <v>99</v>
       </c>
-      <c r="M12" s="27">
-        <v>0</v>
-      </c>
-      <c r="N12" s="32" t="s">
+      <c r="N12" s="27">
+        <v>0</v>
+      </c>
+      <c r="O12" s="32" t="s">
         <v>204</v>
       </c>
-      <c r="O12" s="29" t="s">
+      <c r="P12" s="29" t="s">
         <v>176</v>
       </c>
-      <c r="P12" s="30">
+      <c r="Q12" s="30">
         <v>24</v>
       </c>
-      <c r="Q12" s="31" t="s">
-        <v>108</v>
-      </c>
-      <c r="R12" s="17" t="s">
+      <c r="R12" s="31" t="s">
+        <v>108</v>
+      </c>
+      <c r="S12" s="17" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="13" spans="1:19">
+    <row r="13" spans="1:20">
       <c r="A13" s="24">
         <v>13</v>
       </c>
@@ -2001,33 +2044,36 @@
       <c r="I13" s="25" t="s">
         <v>105</v>
       </c>
-      <c r="J13" s="25" t="s">
+      <c r="J13" s="42">
+        <v>1</v>
+      </c>
+      <c r="K13" s="25" t="s">
         <v>23</v>
       </c>
-      <c r="K13" s="26" t="s">
+      <c r="L13" s="26" t="s">
         <v>127</v>
       </c>
-      <c r="L13" s="24" t="s">
+      <c r="M13" s="24" t="s">
         <v>99</v>
       </c>
-      <c r="M13" s="27">
-        <v>0</v>
-      </c>
-      <c r="N13" s="32" t="s">
+      <c r="N13" s="27">
+        <v>0</v>
+      </c>
+      <c r="O13" s="32" t="s">
         <v>109</v>
       </c>
-      <c r="O13" s="33" t="s">
+      <c r="P13" s="33" t="s">
         <v>123</v>
       </c>
-      <c r="P13" s="30">
+      <c r="Q13" s="30">
         <v>21</v>
       </c>
-      <c r="Q13" s="31" t="s">
-        <v>108</v>
-      </c>
-      <c r="R13" s="17"/>
-    </row>
-    <row r="14" spans="1:19">
+      <c r="R13" s="31" t="s">
+        <v>108</v>
+      </c>
+      <c r="S13" s="17"/>
+    </row>
+    <row r="14" spans="1:20">
       <c r="A14" s="24">
         <v>14</v>
       </c>
@@ -2055,35 +2101,38 @@
       <c r="I14" s="41" t="s">
         <v>106</v>
       </c>
-      <c r="J14" s="25" t="s">
+      <c r="J14" s="42">
+        <v>1</v>
+      </c>
+      <c r="K14" s="25" t="s">
         <v>25</v>
       </c>
-      <c r="K14" s="26" t="s">
+      <c r="L14" s="26" t="s">
         <v>150</v>
       </c>
-      <c r="L14" s="24" t="s">
+      <c r="M14" s="24" t="s">
         <v>99</v>
       </c>
-      <c r="M14" s="27">
-        <v>1</v>
-      </c>
-      <c r="N14" s="32" t="s">
+      <c r="N14" s="27">
+        <v>1</v>
+      </c>
+      <c r="O14" s="32" t="s">
         <v>204</v>
       </c>
-      <c r="O14" s="34" t="s">
+      <c r="P14" s="34" t="s">
         <v>123</v>
       </c>
-      <c r="P14" s="30">
+      <c r="Q14" s="30">
         <v>22</v>
       </c>
-      <c r="Q14" s="31" t="s">
-        <v>108</v>
-      </c>
-      <c r="R14" s="17" t="s">
+      <c r="R14" s="31" t="s">
+        <v>108</v>
+      </c>
+      <c r="S14" s="17" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="15" spans="1:19">
+    <row r="15" spans="1:20">
       <c r="A15" s="24">
         <v>15</v>
       </c>
@@ -2111,33 +2160,36 @@
       <c r="I15" s="25" t="s">
         <v>105</v>
       </c>
-      <c r="J15" s="25" t="s">
+      <c r="J15" s="42">
+        <v>1</v>
+      </c>
+      <c r="K15" s="25" t="s">
         <v>27</v>
       </c>
-      <c r="K15" s="26" t="s">
+      <c r="L15" s="26" t="s">
         <v>128</v>
       </c>
-      <c r="L15" s="24" t="s">
+      <c r="M15" s="24" t="s">
         <v>99</v>
       </c>
-      <c r="M15" s="27">
-        <v>0</v>
-      </c>
-      <c r="N15" s="32" t="s">
+      <c r="N15" s="27">
+        <v>0</v>
+      </c>
+      <c r="O15" s="32" t="s">
         <v>109</v>
       </c>
-      <c r="O15" s="29" t="s">
+      <c r="P15" s="29" t="s">
         <v>176</v>
       </c>
-      <c r="P15" s="30">
+      <c r="Q15" s="30">
         <v>27</v>
       </c>
-      <c r="Q15" s="31" t="s">
-        <v>108</v>
-      </c>
-      <c r="R15" s="17"/>
-    </row>
-    <row r="16" spans="1:19">
+      <c r="R15" s="31" t="s">
+        <v>108</v>
+      </c>
+      <c r="S15" s="17"/>
+    </row>
+    <row r="16" spans="1:20">
       <c r="A16" s="24">
         <v>16</v>
       </c>
@@ -2165,33 +2217,36 @@
       <c r="I16" s="25" t="s">
         <v>106</v>
       </c>
-      <c r="J16" s="25" t="s">
+      <c r="J16" s="42">
+        <v>1</v>
+      </c>
+      <c r="K16" s="25" t="s">
         <v>28</v>
       </c>
-      <c r="K16" s="26" t="s">
+      <c r="L16" s="26" t="s">
         <v>144</v>
       </c>
-      <c r="L16" s="24" t="s">
+      <c r="M16" s="24" t="s">
         <v>99</v>
       </c>
-      <c r="M16" s="27">
-        <v>0</v>
-      </c>
-      <c r="N16" s="32" t="s">
+      <c r="N16" s="27">
+        <v>0</v>
+      </c>
+      <c r="O16" s="32" t="s">
         <v>116</v>
       </c>
-      <c r="O16" s="29" t="s">
+      <c r="P16" s="29" t="s">
         <v>176</v>
       </c>
-      <c r="P16" s="30">
+      <c r="Q16" s="30">
         <v>28</v>
       </c>
-      <c r="Q16" s="31" t="s">
-        <v>108</v>
-      </c>
-      <c r="R16" s="17"/>
-    </row>
-    <row r="17" spans="1:18">
+      <c r="R16" s="31" t="s">
+        <v>108</v>
+      </c>
+      <c r="S16" s="17"/>
+    </row>
+    <row r="17" spans="1:19">
       <c r="A17" s="24">
         <v>17</v>
       </c>
@@ -2219,33 +2274,36 @@
       <c r="I17" s="25" t="s">
         <v>106</v>
       </c>
-      <c r="J17" s="25" t="s">
+      <c r="J17" s="42">
+        <v>1</v>
+      </c>
+      <c r="K17" s="25" t="s">
         <v>29</v>
       </c>
-      <c r="K17" s="26" t="s">
+      <c r="L17" s="26" t="s">
         <v>145</v>
       </c>
-      <c r="L17" s="24" t="s">
+      <c r="M17" s="24" t="s">
         <v>99</v>
       </c>
-      <c r="M17" s="27">
-        <v>0</v>
-      </c>
-      <c r="N17" s="32" t="s">
+      <c r="N17" s="27">
+        <v>0</v>
+      </c>
+      <c r="O17" s="32" t="s">
         <v>116</v>
       </c>
-      <c r="O17" s="17" t="s">
+      <c r="P17" s="17" t="s">
         <v>122</v>
       </c>
-      <c r="P17" s="30">
-        <v>0</v>
-      </c>
-      <c r="Q17" s="31" t="s">
-        <v>108</v>
-      </c>
-      <c r="R17" s="17"/>
-    </row>
-    <row r="18" spans="1:18">
+      <c r="Q17" s="30">
+        <v>0</v>
+      </c>
+      <c r="R17" s="31" t="s">
+        <v>108</v>
+      </c>
+      <c r="S17" s="17"/>
+    </row>
+    <row r="18" spans="1:19">
       <c r="A18" s="24">
         <v>18</v>
       </c>
@@ -2273,33 +2331,36 @@
       <c r="I18" s="25" t="s">
         <v>105</v>
       </c>
-      <c r="J18" s="25" t="s">
+      <c r="J18" s="42">
+        <v>1</v>
+      </c>
+      <c r="K18" s="25" t="s">
         <v>31</v>
       </c>
-      <c r="K18" s="26" t="s">
+      <c r="L18" s="26" t="s">
         <v>129</v>
       </c>
-      <c r="L18" s="24" t="s">
+      <c r="M18" s="24" t="s">
         <v>99</v>
       </c>
-      <c r="M18" s="27">
-        <v>0</v>
-      </c>
-      <c r="N18" s="32" t="s">
+      <c r="N18" s="27">
+        <v>0</v>
+      </c>
+      <c r="O18" s="32" t="s">
         <v>109</v>
       </c>
-      <c r="O18" s="33" t="s">
+      <c r="P18" s="33" t="s">
         <v>123</v>
       </c>
-      <c r="P18" s="30">
+      <c r="Q18" s="30">
         <v>25</v>
       </c>
-      <c r="Q18" s="31" t="s">
-        <v>108</v>
-      </c>
-      <c r="R18" s="17"/>
-    </row>
-    <row r="19" spans="1:18">
+      <c r="R18" s="31" t="s">
+        <v>108</v>
+      </c>
+      <c r="S18" s="17"/>
+    </row>
+    <row r="19" spans="1:19">
       <c r="A19" s="24">
         <v>19</v>
       </c>
@@ -2327,33 +2388,36 @@
       <c r="I19" s="25" t="s">
         <v>106</v>
       </c>
-      <c r="J19" s="25" t="s">
+      <c r="J19" s="42">
+        <v>1</v>
+      </c>
+      <c r="K19" s="25" t="s">
         <v>32</v>
       </c>
-      <c r="K19" s="26" t="s">
+      <c r="L19" s="26" t="s">
         <v>151</v>
       </c>
-      <c r="L19" s="24" t="s">
+      <c r="M19" s="24" t="s">
         <v>99</v>
       </c>
-      <c r="M19" s="27">
-        <v>1</v>
-      </c>
-      <c r="N19" s="32" t="s">
+      <c r="N19" s="27">
+        <v>1</v>
+      </c>
+      <c r="O19" s="32" t="s">
         <v>116</v>
       </c>
-      <c r="O19" s="34" t="s">
+      <c r="P19" s="34" t="s">
         <v>123</v>
       </c>
-      <c r="P19" s="30">
+      <c r="Q19" s="30">
         <v>26</v>
       </c>
-      <c r="Q19" s="31" t="s">
-        <v>108</v>
-      </c>
-      <c r="R19" s="17"/>
-    </row>
-    <row r="20" spans="1:18">
+      <c r="R19" s="31" t="s">
+        <v>108</v>
+      </c>
+      <c r="S19" s="17"/>
+    </row>
+    <row r="20" spans="1:19">
       <c r="A20" s="24">
         <v>20</v>
       </c>
@@ -2381,33 +2445,36 @@
       <c r="I20" s="25" t="s">
         <v>106</v>
       </c>
-      <c r="J20" s="25" t="s">
+      <c r="J20" s="42">
+        <v>1</v>
+      </c>
+      <c r="K20" s="25" t="s">
         <v>33</v>
       </c>
-      <c r="K20" s="26" t="s">
+      <c r="L20" s="26" t="s">
         <v>146</v>
       </c>
-      <c r="L20" s="24" t="s">
+      <c r="M20" s="24" t="s">
         <v>99</v>
       </c>
-      <c r="M20" s="27">
-        <v>1</v>
-      </c>
-      <c r="N20" s="32" t="s">
+      <c r="N20" s="27">
+        <v>1</v>
+      </c>
+      <c r="O20" s="32" t="s">
         <v>116</v>
       </c>
-      <c r="O20" s="17" t="s">
+      <c r="P20" s="17" t="s">
         <v>122</v>
       </c>
-      <c r="P20" s="30">
-        <v>0</v>
-      </c>
-      <c r="Q20" s="31" t="s">
-        <v>108</v>
-      </c>
-      <c r="R20" s="17"/>
-    </row>
-    <row r="21" spans="1:18">
+      <c r="Q20" s="30">
+        <v>0</v>
+      </c>
+      <c r="R20" s="31" t="s">
+        <v>108</v>
+      </c>
+      <c r="S20" s="17"/>
+    </row>
+    <row r="21" spans="1:19">
       <c r="A21" s="24">
         <v>21</v>
       </c>
@@ -2435,33 +2502,36 @@
       <c r="I21" s="25" t="s">
         <v>105</v>
       </c>
-      <c r="J21" s="25" t="s">
+      <c r="J21" s="42">
+        <v>1</v>
+      </c>
+      <c r="K21" s="25" t="s">
         <v>35</v>
       </c>
-      <c r="K21" s="26" t="s">
+      <c r="L21" s="26" t="s">
         <v>130</v>
       </c>
-      <c r="L21" s="24" t="s">
+      <c r="M21" s="24" t="s">
         <v>99</v>
       </c>
-      <c r="M21" s="27">
-        <v>0</v>
-      </c>
-      <c r="N21" s="32" t="s">
+      <c r="N21" s="27">
+        <v>0</v>
+      </c>
+      <c r="O21" s="32" t="s">
         <v>109</v>
       </c>
-      <c r="O21" s="29" t="s">
+      <c r="P21" s="29" t="s">
         <v>176</v>
       </c>
-      <c r="P21" s="30">
+      <c r="Q21" s="30">
         <v>31</v>
       </c>
-      <c r="Q21" s="31" t="s">
-        <v>108</v>
-      </c>
-      <c r="R21" s="17"/>
-    </row>
-    <row r="22" spans="1:18">
+      <c r="R21" s="31" t="s">
+        <v>108</v>
+      </c>
+      <c r="S21" s="17"/>
+    </row>
+    <row r="22" spans="1:19">
       <c r="A22" s="24">
         <v>22</v>
       </c>
@@ -2489,33 +2559,36 @@
       <c r="I22" s="25" t="s">
         <v>106</v>
       </c>
-      <c r="J22" s="25" t="s">
+      <c r="J22" s="42">
+        <v>1</v>
+      </c>
+      <c r="K22" s="25" t="s">
         <v>36</v>
       </c>
-      <c r="K22" s="26" t="s">
+      <c r="L22" s="26" t="s">
         <v>147</v>
       </c>
-      <c r="L22" s="24" t="s">
+      <c r="M22" s="24" t="s">
         <v>99</v>
       </c>
-      <c r="M22" s="27">
-        <v>0</v>
-      </c>
-      <c r="N22" s="32" t="s">
+      <c r="N22" s="27">
+        <v>0</v>
+      </c>
+      <c r="O22" s="32" t="s">
         <v>116</v>
       </c>
-      <c r="O22" s="29" t="s">
+      <c r="P22" s="29" t="s">
         <v>176</v>
       </c>
-      <c r="P22" s="30">
+      <c r="Q22" s="30">
         <v>32</v>
       </c>
-      <c r="Q22" s="31" t="s">
-        <v>108</v>
-      </c>
-      <c r="R22" s="17"/>
-    </row>
-    <row r="23" spans="1:18">
+      <c r="R22" s="31" t="s">
+        <v>108</v>
+      </c>
+      <c r="S22" s="17"/>
+    </row>
+    <row r="23" spans="1:19">
       <c r="A23" s="24">
         <v>23</v>
       </c>
@@ -2543,33 +2616,36 @@
       <c r="I23" s="25" t="s">
         <v>106</v>
       </c>
-      <c r="J23" s="25" t="s">
+      <c r="J23" s="42">
+        <v>1</v>
+      </c>
+      <c r="K23" s="25" t="s">
         <v>37</v>
       </c>
-      <c r="K23" s="26" t="s">
+      <c r="L23" s="26" t="s">
         <v>148</v>
       </c>
-      <c r="L23" s="24" t="s">
+      <c r="M23" s="24" t="s">
         <v>99</v>
       </c>
-      <c r="M23" s="27">
-        <v>0</v>
-      </c>
-      <c r="N23" s="32" t="s">
+      <c r="N23" s="27">
+        <v>0</v>
+      </c>
+      <c r="O23" s="32" t="s">
         <v>116</v>
       </c>
-      <c r="O23" s="17" t="s">
+      <c r="P23" s="17" t="s">
         <v>122</v>
       </c>
-      <c r="P23" s="30">
-        <v>0</v>
-      </c>
-      <c r="Q23" s="31" t="s">
-        <v>108</v>
-      </c>
-      <c r="R23" s="17"/>
-    </row>
-    <row r="24" spans="1:18">
+      <c r="Q23" s="30">
+        <v>0</v>
+      </c>
+      <c r="R23" s="31" t="s">
+        <v>108</v>
+      </c>
+      <c r="S23" s="17"/>
+    </row>
+    <row r="24" spans="1:19">
       <c r="A24" s="24">
         <v>24</v>
       </c>
@@ -2597,33 +2673,36 @@
       <c r="I24" s="25" t="s">
         <v>105</v>
       </c>
-      <c r="J24" s="25" t="s">
+      <c r="J24" s="42">
+        <v>1</v>
+      </c>
+      <c r="K24" s="25" t="s">
         <v>39</v>
       </c>
-      <c r="K24" s="26" t="s">
+      <c r="L24" s="26" t="s">
         <v>131</v>
       </c>
-      <c r="L24" s="24" t="s">
+      <c r="M24" s="24" t="s">
         <v>99</v>
       </c>
-      <c r="M24" s="27">
-        <v>0</v>
-      </c>
-      <c r="N24" s="32" t="s">
+      <c r="N24" s="27">
+        <v>0</v>
+      </c>
+      <c r="O24" s="32" t="s">
         <v>109</v>
       </c>
-      <c r="O24" s="33" t="s">
+      <c r="P24" s="33" t="s">
         <v>123</v>
       </c>
-      <c r="P24" s="30">
+      <c r="Q24" s="30">
         <v>29</v>
       </c>
-      <c r="Q24" s="31" t="s">
-        <v>108</v>
-      </c>
-      <c r="R24" s="17"/>
-    </row>
-    <row r="25" spans="1:18">
+      <c r="R24" s="31" t="s">
+        <v>108</v>
+      </c>
+      <c r="S24" s="17"/>
+    </row>
+    <row r="25" spans="1:19">
       <c r="A25" s="24">
         <v>25</v>
       </c>
@@ -2651,33 +2730,36 @@
       <c r="I25" s="25" t="s">
         <v>106</v>
       </c>
-      <c r="J25" s="25" t="s">
+      <c r="J25" s="42">
+        <v>1</v>
+      </c>
+      <c r="K25" s="25" t="s">
         <v>40</v>
       </c>
-      <c r="K25" s="26" t="s">
+      <c r="L25" s="26" t="s">
         <v>158</v>
       </c>
-      <c r="L25" s="24" t="s">
+      <c r="M25" s="24" t="s">
         <v>99</v>
       </c>
-      <c r="M25" s="27">
-        <v>1</v>
-      </c>
-      <c r="N25" s="32" t="s">
+      <c r="N25" s="27">
+        <v>1</v>
+      </c>
+      <c r="O25" s="32" t="s">
         <v>116</v>
       </c>
-      <c r="O25" s="34" t="s">
+      <c r="P25" s="34" t="s">
         <v>123</v>
       </c>
-      <c r="P25" s="30">
+      <c r="Q25" s="30">
         <v>30</v>
       </c>
-      <c r="Q25" s="31" t="s">
-        <v>108</v>
-      </c>
-      <c r="R25" s="17"/>
-    </row>
-    <row r="26" spans="1:18">
+      <c r="R25" s="31" t="s">
+        <v>108</v>
+      </c>
+      <c r="S25" s="17"/>
+    </row>
+    <row r="26" spans="1:19">
       <c r="A26" s="24">
         <v>26</v>
       </c>
@@ -2705,33 +2787,36 @@
       <c r="I26" s="25" t="s">
         <v>106</v>
       </c>
-      <c r="J26" s="25" t="s">
+      <c r="J26" s="42">
+        <v>1</v>
+      </c>
+      <c r="K26" s="25" t="s">
         <v>41</v>
       </c>
-      <c r="K26" s="26" t="s">
+      <c r="L26" s="26" t="s">
         <v>159</v>
       </c>
-      <c r="L26" s="24" t="s">
+      <c r="M26" s="24" t="s">
         <v>99</v>
       </c>
-      <c r="M26" s="27">
-        <v>1</v>
-      </c>
-      <c r="N26" s="32" t="s">
+      <c r="N26" s="27">
+        <v>1</v>
+      </c>
+      <c r="O26" s="32" t="s">
         <v>116</v>
       </c>
-      <c r="O26" s="17" t="s">
+      <c r="P26" s="17" t="s">
         <v>122</v>
       </c>
-      <c r="P26" s="30">
-        <v>0</v>
-      </c>
-      <c r="Q26" s="31" t="s">
-        <v>108</v>
-      </c>
-      <c r="R26" s="17"/>
-    </row>
-    <row r="27" spans="1:18">
+      <c r="Q26" s="30">
+        <v>0</v>
+      </c>
+      <c r="R26" s="31" t="s">
+        <v>108</v>
+      </c>
+      <c r="S26" s="17"/>
+    </row>
+    <row r="27" spans="1:19">
       <c r="A27" s="24">
         <v>27</v>
       </c>
@@ -2759,33 +2844,36 @@
       <c r="I27" s="25" t="s">
         <v>105</v>
       </c>
-      <c r="J27" s="25" t="s">
+      <c r="J27" s="42">
+        <v>1</v>
+      </c>
+      <c r="K27" s="25" t="s">
         <v>43</v>
       </c>
-      <c r="K27" s="26" t="s">
+      <c r="L27" s="26" t="s">
         <v>132</v>
       </c>
-      <c r="L27" s="24" t="s">
+      <c r="M27" s="24" t="s">
         <v>99</v>
       </c>
-      <c r="M27" s="27">
-        <v>0</v>
-      </c>
-      <c r="N27" s="32" t="s">
+      <c r="N27" s="27">
+        <v>0</v>
+      </c>
+      <c r="O27" s="32" t="s">
         <v>109</v>
       </c>
-      <c r="O27" s="29" t="s">
+      <c r="P27" s="29" t="s">
         <v>176</v>
       </c>
-      <c r="P27" s="30">
+      <c r="Q27" s="30">
         <v>35</v>
       </c>
-      <c r="Q27" s="31" t="s">
-        <v>108</v>
-      </c>
-      <c r="R27" s="17"/>
-    </row>
-    <row r="28" spans="1:18">
+      <c r="R27" s="31" t="s">
+        <v>108</v>
+      </c>
+      <c r="S27" s="17"/>
+    </row>
+    <row r="28" spans="1:19">
       <c r="A28" s="24">
         <v>28</v>
       </c>
@@ -2813,33 +2901,36 @@
       <c r="I28" s="25" t="s">
         <v>106</v>
       </c>
-      <c r="J28" s="25" t="s">
+      <c r="J28" s="42">
+        <v>1</v>
+      </c>
+      <c r="K28" s="25" t="s">
         <v>44</v>
       </c>
-      <c r="K28" s="26" t="s">
+      <c r="L28" s="26" t="s">
         <v>160</v>
       </c>
-      <c r="L28" s="24" t="s">
+      <c r="M28" s="24" t="s">
         <v>99</v>
       </c>
-      <c r="M28" s="27">
-        <v>0</v>
-      </c>
-      <c r="N28" s="32" t="s">
+      <c r="N28" s="27">
+        <v>0</v>
+      </c>
+      <c r="O28" s="32" t="s">
         <v>116</v>
       </c>
-      <c r="O28" s="29" t="s">
+      <c r="P28" s="29" t="s">
         <v>176</v>
       </c>
-      <c r="P28" s="30">
+      <c r="Q28" s="30">
         <v>36</v>
       </c>
-      <c r="Q28" s="31" t="s">
-        <v>108</v>
-      </c>
-      <c r="R28" s="17"/>
-    </row>
-    <row r="29" spans="1:18">
+      <c r="R28" s="31" t="s">
+        <v>108</v>
+      </c>
+      <c r="S28" s="17"/>
+    </row>
+    <row r="29" spans="1:19">
       <c r="A29" s="24">
         <v>29</v>
       </c>
@@ -2867,33 +2958,36 @@
       <c r="I29" s="25" t="s">
         <v>106</v>
       </c>
-      <c r="J29" s="25" t="s">
+      <c r="J29" s="42">
+        <v>1</v>
+      </c>
+      <c r="K29" s="25" t="s">
         <v>45</v>
       </c>
-      <c r="K29" s="26" t="s">
+      <c r="L29" s="26" t="s">
         <v>161</v>
       </c>
-      <c r="L29" s="24" t="s">
+      <c r="M29" s="24" t="s">
         <v>99</v>
       </c>
-      <c r="M29" s="27">
-        <v>0</v>
-      </c>
-      <c r="N29" s="32" t="s">
+      <c r="N29" s="27">
+        <v>0</v>
+      </c>
+      <c r="O29" s="32" t="s">
         <v>116</v>
       </c>
-      <c r="O29" s="17" t="s">
+      <c r="P29" s="17" t="s">
         <v>122</v>
       </c>
-      <c r="P29" s="30">
-        <v>0</v>
-      </c>
-      <c r="Q29" s="31" t="s">
-        <v>108</v>
-      </c>
-      <c r="R29" s="17"/>
-    </row>
-    <row r="30" spans="1:18">
+      <c r="Q29" s="30">
+        <v>0</v>
+      </c>
+      <c r="R29" s="31" t="s">
+        <v>108</v>
+      </c>
+      <c r="S29" s="17"/>
+    </row>
+    <row r="30" spans="1:19">
       <c r="A30" s="24">
         <v>30</v>
       </c>
@@ -2921,33 +3015,36 @@
       <c r="I30" s="25" t="s">
         <v>105</v>
       </c>
-      <c r="J30" s="25" t="s">
+      <c r="J30" s="42">
+        <v>1</v>
+      </c>
+      <c r="K30" s="25" t="s">
         <v>47</v>
       </c>
-      <c r="K30" s="26" t="s">
+      <c r="L30" s="26" t="s">
         <v>133</v>
       </c>
-      <c r="L30" s="24" t="s">
+      <c r="M30" s="24" t="s">
         <v>99</v>
       </c>
-      <c r="M30" s="27">
-        <v>0</v>
-      </c>
-      <c r="N30" s="32" t="s">
+      <c r="N30" s="27">
+        <v>0</v>
+      </c>
+      <c r="O30" s="32" t="s">
         <v>109</v>
       </c>
-      <c r="O30" s="33" t="s">
+      <c r="P30" s="33" t="s">
         <v>123</v>
       </c>
-      <c r="P30" s="30">
+      <c r="Q30" s="30">
         <v>33</v>
       </c>
-      <c r="Q30" s="31" t="s">
-        <v>108</v>
-      </c>
-      <c r="R30" s="17"/>
-    </row>
-    <row r="31" spans="1:18">
+      <c r="R30" s="31" t="s">
+        <v>108</v>
+      </c>
+      <c r="S30" s="17"/>
+    </row>
+    <row r="31" spans="1:19">
       <c r="A31" s="24">
         <v>31</v>
       </c>
@@ -2975,33 +3072,36 @@
       <c r="I31" s="25" t="s">
         <v>106</v>
       </c>
-      <c r="J31" s="25" t="s">
+      <c r="J31" s="42">
+        <v>1</v>
+      </c>
+      <c r="K31" s="25" t="s">
         <v>48</v>
       </c>
-      <c r="K31" s="26" t="s">
+      <c r="L31" s="26" t="s">
         <v>162</v>
       </c>
-      <c r="L31" s="24" t="s">
+      <c r="M31" s="24" t="s">
         <v>99</v>
       </c>
-      <c r="M31" s="27">
-        <v>1</v>
-      </c>
-      <c r="N31" s="32" t="s">
+      <c r="N31" s="27">
+        <v>1</v>
+      </c>
+      <c r="O31" s="32" t="s">
         <v>116</v>
       </c>
-      <c r="O31" s="34" t="s">
+      <c r="P31" s="34" t="s">
         <v>123</v>
       </c>
-      <c r="P31" s="30">
+      <c r="Q31" s="30">
         <v>34</v>
       </c>
-      <c r="Q31" s="31" t="s">
-        <v>108</v>
-      </c>
-      <c r="R31" s="17"/>
-    </row>
-    <row r="32" spans="1:18">
+      <c r="R31" s="31" t="s">
+        <v>108</v>
+      </c>
+      <c r="S31" s="17"/>
+    </row>
+    <row r="32" spans="1:19">
       <c r="A32" s="24">
         <v>32</v>
       </c>
@@ -3029,33 +3129,36 @@
       <c r="I32" s="25" t="s">
         <v>106</v>
       </c>
-      <c r="J32" s="25" t="s">
+      <c r="J32" s="42">
+        <v>1</v>
+      </c>
+      <c r="K32" s="25" t="s">
         <v>49</v>
       </c>
-      <c r="K32" s="26" t="s">
+      <c r="L32" s="26" t="s">
         <v>163</v>
       </c>
-      <c r="L32" s="24" t="s">
+      <c r="M32" s="24" t="s">
         <v>99</v>
       </c>
-      <c r="M32" s="27">
-        <v>1</v>
-      </c>
-      <c r="N32" s="32" t="s">
+      <c r="N32" s="27">
+        <v>1</v>
+      </c>
+      <c r="O32" s="32" t="s">
         <v>116</v>
       </c>
-      <c r="O32" s="17" t="s">
+      <c r="P32" s="17" t="s">
         <v>122</v>
       </c>
-      <c r="P32" s="30">
-        <v>0</v>
-      </c>
-      <c r="Q32" s="31" t="s">
-        <v>108</v>
-      </c>
-      <c r="R32" s="17"/>
-    </row>
-    <row r="33" spans="1:18" ht="19" customHeight="1">
+      <c r="Q32" s="30">
+        <v>0</v>
+      </c>
+      <c r="R32" s="31" t="s">
+        <v>108</v>
+      </c>
+      <c r="S32" s="17"/>
+    </row>
+    <row r="33" spans="1:19" ht="19" customHeight="1">
       <c r="A33" s="24">
         <v>33</v>
       </c>
@@ -3083,33 +3186,36 @@
       <c r="I33" s="10" t="s">
         <v>105</v>
       </c>
-      <c r="J33" s="10" t="s">
+      <c r="J33" s="10">
+        <v>1</v>
+      </c>
+      <c r="K33" s="10" t="s">
         <v>52</v>
       </c>
-      <c r="K33" s="11" t="s">
+      <c r="L33" s="11" t="s">
         <v>134</v>
       </c>
-      <c r="L33" s="12" t="s">
+      <c r="M33" s="12" t="s">
         <v>50</v>
       </c>
-      <c r="M33" s="13">
-        <v>0</v>
-      </c>
-      <c r="N33" s="14" t="s">
+      <c r="N33" s="13">
+        <v>0</v>
+      </c>
+      <c r="O33" s="14" t="s">
         <v>109</v>
       </c>
-      <c r="O33" s="10" t="s">
+      <c r="P33" s="10" t="s">
         <v>172</v>
       </c>
-      <c r="P33" s="9">
-        <v>1</v>
-      </c>
-      <c r="Q33" s="18" t="s">
-        <v>108</v>
-      </c>
-      <c r="R33" s="9"/>
-    </row>
-    <row r="34" spans="1:18">
+      <c r="Q33" s="9">
+        <v>1</v>
+      </c>
+      <c r="R33" s="18" t="s">
+        <v>108</v>
+      </c>
+      <c r="S33" s="9"/>
+    </row>
+    <row r="34" spans="1:19">
       <c r="A34" s="24">
         <v>34</v>
       </c>
@@ -3137,33 +3243,36 @@
       <c r="I34" s="10" t="s">
         <v>105</v>
       </c>
-      <c r="J34" s="10" t="s">
+      <c r="J34" s="10">
+        <v>1</v>
+      </c>
+      <c r="K34" s="10" t="s">
         <v>54</v>
       </c>
-      <c r="K34" s="11" t="s">
+      <c r="L34" s="11" t="s">
         <v>135</v>
       </c>
-      <c r="L34" s="12" t="s">
+      <c r="M34" s="12" t="s">
         <v>50</v>
       </c>
-      <c r="M34" s="13">
-        <v>0</v>
-      </c>
-      <c r="N34" s="14" t="s">
+      <c r="N34" s="13">
+        <v>0</v>
+      </c>
+      <c r="O34" s="14" t="s">
         <v>109</v>
       </c>
-      <c r="O34" s="10" t="s">
+      <c r="P34" s="10" t="s">
         <v>172</v>
       </c>
-      <c r="P34" s="9">
+      <c r="Q34" s="9">
         <v>3</v>
       </c>
-      <c r="Q34" s="18" t="s">
-        <v>108</v>
-      </c>
-      <c r="R34" s="9"/>
-    </row>
-    <row r="35" spans="1:18">
+      <c r="R34" s="18" t="s">
+        <v>108</v>
+      </c>
+      <c r="S34" s="9"/>
+    </row>
+    <row r="35" spans="1:19">
       <c r="A35" s="24">
         <v>35</v>
       </c>
@@ -3191,33 +3300,36 @@
       <c r="I35" s="10" t="s">
         <v>105</v>
       </c>
-      <c r="J35" s="10" t="s">
+      <c r="J35" s="10">
+        <v>1</v>
+      </c>
+      <c r="K35" s="10" t="s">
         <v>56</v>
       </c>
-      <c r="K35" s="11" t="s">
+      <c r="L35" s="11" t="s">
         <v>164</v>
       </c>
-      <c r="L35" s="12" t="s">
+      <c r="M35" s="12" t="s">
         <v>50</v>
       </c>
-      <c r="M35" s="13">
-        <v>0</v>
-      </c>
-      <c r="N35" s="14" t="s">
+      <c r="N35" s="13">
+        <v>0</v>
+      </c>
+      <c r="O35" s="14" t="s">
         <v>109</v>
       </c>
-      <c r="O35" s="10" t="s">
+      <c r="P35" s="10" t="s">
         <v>172</v>
       </c>
-      <c r="P35" s="9">
+      <c r="Q35" s="9">
         <v>4</v>
       </c>
-      <c r="Q35" s="18" t="s">
-        <v>108</v>
-      </c>
-      <c r="R35" s="9"/>
-    </row>
-    <row r="36" spans="1:18">
+      <c r="R35" s="18" t="s">
+        <v>108</v>
+      </c>
+      <c r="S35" s="9"/>
+    </row>
+    <row r="36" spans="1:19">
       <c r="A36" s="24">
         <v>36</v>
       </c>
@@ -3245,33 +3357,36 @@
       <c r="I36" s="10" t="s">
         <v>105</v>
       </c>
-      <c r="J36" s="10" t="s">
+      <c r="J36" s="10">
+        <v>1</v>
+      </c>
+      <c r="K36" s="10" t="s">
         <v>58</v>
       </c>
-      <c r="K36" s="11" t="s">
+      <c r="L36" s="11" t="s">
         <v>165</v>
       </c>
-      <c r="L36" s="12" t="s">
+      <c r="M36" s="12" t="s">
         <v>50</v>
       </c>
-      <c r="M36" s="13">
-        <v>0</v>
-      </c>
-      <c r="N36" s="14" t="s">
+      <c r="N36" s="13">
+        <v>0</v>
+      </c>
+      <c r="O36" s="14" t="s">
         <v>109</v>
       </c>
-      <c r="O36" s="10" t="s">
+      <c r="P36" s="10" t="s">
         <v>172</v>
       </c>
-      <c r="P36" s="9">
+      <c r="Q36" s="9">
         <v>2</v>
       </c>
-      <c r="Q36" s="18" t="s">
-        <v>108</v>
-      </c>
-      <c r="R36" s="9"/>
-    </row>
-    <row r="37" spans="1:18">
+      <c r="R36" s="18" t="s">
+        <v>108</v>
+      </c>
+      <c r="S36" s="9"/>
+    </row>
+    <row r="37" spans="1:19">
       <c r="A37" s="24">
         <v>37</v>
       </c>
@@ -3299,33 +3414,36 @@
       <c r="I37" s="10" t="s">
         <v>105</v>
       </c>
-      <c r="J37" s="10" t="s">
+      <c r="J37" s="10">
+        <v>1</v>
+      </c>
+      <c r="K37" s="10" t="s">
         <v>60</v>
       </c>
-      <c r="K37" s="11" t="s">
+      <c r="L37" s="11" t="s">
         <v>166</v>
       </c>
-      <c r="L37" s="12" t="s">
+      <c r="M37" s="12" t="s">
         <v>50</v>
       </c>
-      <c r="M37" s="13">
-        <v>0</v>
-      </c>
-      <c r="N37" s="14" t="s">
+      <c r="N37" s="13">
+        <v>0</v>
+      </c>
+      <c r="O37" s="14" t="s">
         <v>109</v>
       </c>
-      <c r="O37" s="19" t="s">
+      <c r="P37" s="19" t="s">
         <v>175</v>
       </c>
-      <c r="P37" s="9">
+      <c r="Q37" s="9">
         <v>19</v>
       </c>
-      <c r="Q37" s="18" t="s">
-        <v>108</v>
-      </c>
-      <c r="R37" s="9"/>
-    </row>
-    <row r="38" spans="1:18">
+      <c r="R37" s="18" t="s">
+        <v>108</v>
+      </c>
+      <c r="S37" s="9"/>
+    </row>
+    <row r="38" spans="1:19">
       <c r="A38" s="24">
         <v>38</v>
       </c>
@@ -3353,33 +3471,36 @@
       <c r="I38" s="10" t="s">
         <v>105</v>
       </c>
-      <c r="J38" s="10" t="s">
+      <c r="J38" s="10">
+        <v>1</v>
+      </c>
+      <c r="K38" s="10" t="s">
         <v>62</v>
       </c>
-      <c r="K38" s="11" t="s">
+      <c r="L38" s="11" t="s">
         <v>136</v>
       </c>
-      <c r="L38" s="12" t="s">
+      <c r="M38" s="12" t="s">
         <v>50</v>
       </c>
-      <c r="M38" s="13">
-        <v>0</v>
-      </c>
-      <c r="N38" s="14" t="s">
+      <c r="N38" s="13">
+        <v>0</v>
+      </c>
+      <c r="O38" s="14" t="s">
         <v>109</v>
       </c>
-      <c r="O38" s="10" t="s">
+      <c r="P38" s="10" t="s">
         <v>172</v>
       </c>
-      <c r="P38" s="9">
+      <c r="Q38" s="9">
         <v>6</v>
       </c>
-      <c r="Q38" s="18" t="s">
-        <v>108</v>
-      </c>
-      <c r="R38" s="9"/>
-    </row>
-    <row r="39" spans="1:18">
+      <c r="R38" s="18" t="s">
+        <v>108</v>
+      </c>
+      <c r="S38" s="9"/>
+    </row>
+    <row r="39" spans="1:19">
       <c r="A39" s="24">
         <v>39</v>
       </c>
@@ -3407,33 +3528,36 @@
       <c r="I39" s="10" t="s">
         <v>105</v>
       </c>
-      <c r="J39" s="10" t="s">
+      <c r="J39" s="10">
+        <v>1</v>
+      </c>
+      <c r="K39" s="10" t="s">
         <v>64</v>
       </c>
-      <c r="K39" s="11" t="s">
+      <c r="L39" s="11" t="s">
         <v>137</v>
       </c>
-      <c r="L39" s="12" t="s">
+      <c r="M39" s="12" t="s">
         <v>50</v>
       </c>
-      <c r="M39" s="13">
-        <v>0</v>
-      </c>
-      <c r="N39" s="14" t="s">
+      <c r="N39" s="13">
+        <v>0</v>
+      </c>
+      <c r="O39" s="14" t="s">
         <v>109</v>
       </c>
-      <c r="O39" s="10" t="s">
+      <c r="P39" s="10" t="s">
         <v>172</v>
       </c>
-      <c r="P39" s="9">
+      <c r="Q39" s="9">
         <v>5</v>
       </c>
-      <c r="Q39" s="18" t="s">
-        <v>108</v>
-      </c>
-      <c r="R39" s="9"/>
-    </row>
-    <row r="40" spans="1:18">
+      <c r="R39" s="18" t="s">
+        <v>108</v>
+      </c>
+      <c r="S39" s="9"/>
+    </row>
+    <row r="40" spans="1:19">
       <c r="A40" s="24">
         <v>40</v>
       </c>
@@ -3461,33 +3585,36 @@
       <c r="I40" s="10" t="s">
         <v>105</v>
       </c>
-      <c r="J40" s="10" t="s">
+      <c r="J40" s="10">
+        <v>1</v>
+      </c>
+      <c r="K40" s="10" t="s">
         <v>66</v>
       </c>
-      <c r="K40" s="11" t="s">
+      <c r="L40" s="11" t="s">
         <v>138</v>
       </c>
-      <c r="L40" s="12" t="s">
+      <c r="M40" s="12" t="s">
         <v>50</v>
       </c>
-      <c r="M40" s="13">
-        <v>0</v>
-      </c>
-      <c r="N40" s="14" t="s">
+      <c r="N40" s="13">
+        <v>0</v>
+      </c>
+      <c r="O40" s="14" t="s">
         <v>109</v>
       </c>
-      <c r="O40" s="10" t="s">
+      <c r="P40" s="10" t="s">
         <v>172</v>
       </c>
-      <c r="P40" s="9">
+      <c r="Q40" s="9">
         <v>8</v>
       </c>
-      <c r="Q40" s="18" t="s">
-        <v>108</v>
-      </c>
-      <c r="R40" s="9"/>
-    </row>
-    <row r="41" spans="1:18">
+      <c r="R40" s="18" t="s">
+        <v>108</v>
+      </c>
+      <c r="S40" s="9"/>
+    </row>
+    <row r="41" spans="1:19">
       <c r="A41" s="24">
         <v>41</v>
       </c>
@@ -3515,33 +3642,36 @@
       <c r="I41" s="10" t="s">
         <v>105</v>
       </c>
-      <c r="J41" s="10" t="s">
+      <c r="J41" s="10">
+        <v>1</v>
+      </c>
+      <c r="K41" s="10" t="s">
         <v>68</v>
       </c>
-      <c r="K41" s="11" t="s">
+      <c r="L41" s="11" t="s">
         <v>139</v>
       </c>
-      <c r="L41" s="12" t="s">
+      <c r="M41" s="12" t="s">
         <v>50</v>
       </c>
-      <c r="M41" s="13">
-        <v>0</v>
-      </c>
-      <c r="N41" s="14" t="s">
+      <c r="N41" s="13">
+        <v>0</v>
+      </c>
+      <c r="O41" s="14" t="s">
         <v>109</v>
       </c>
-      <c r="O41" s="10" t="s">
+      <c r="P41" s="10" t="s">
         <v>172</v>
       </c>
-      <c r="P41" s="9">
+      <c r="Q41" s="9">
         <v>7</v>
       </c>
-      <c r="Q41" s="18" t="s">
-        <v>108</v>
-      </c>
-      <c r="R41" s="9"/>
-    </row>
-    <row r="42" spans="1:18">
+      <c r="R41" s="18" t="s">
+        <v>108</v>
+      </c>
+      <c r="S41" s="9"/>
+    </row>
+    <row r="42" spans="1:19">
       <c r="A42" s="24">
         <v>42</v>
       </c>
@@ -3570,33 +3700,36 @@
       <c r="I42" s="10" t="s">
         <v>105</v>
       </c>
-      <c r="J42" s="10" t="s">
+      <c r="J42" s="10">
+        <v>1</v>
+      </c>
+      <c r="K42" s="10" t="s">
         <v>198</v>
       </c>
-      <c r="K42" s="11" t="s">
+      <c r="L42" s="11" t="s">
         <v>136</v>
       </c>
-      <c r="L42" s="12" t="s">
+      <c r="M42" s="12" t="s">
         <v>50</v>
       </c>
-      <c r="M42" s="13">
-        <v>0</v>
-      </c>
-      <c r="N42" s="14" t="s">
+      <c r="N42" s="13">
+        <v>0</v>
+      </c>
+      <c r="O42" s="14" t="s">
         <v>109</v>
       </c>
-      <c r="O42" s="29" t="s">
+      <c r="P42" s="29" t="s">
         <v>176</v>
       </c>
-      <c r="P42" s="9">
+      <c r="Q42" s="9">
         <v>11</v>
       </c>
-      <c r="Q42" s="18" t="s">
-        <v>108</v>
-      </c>
-      <c r="R42" s="9"/>
-    </row>
-    <row r="43" spans="1:18">
+      <c r="R42" s="18" t="s">
+        <v>108</v>
+      </c>
+      <c r="S42" s="9"/>
+    </row>
+    <row r="43" spans="1:19">
       <c r="A43" s="24">
         <v>43</v>
       </c>
@@ -3625,33 +3758,36 @@
       <c r="I43" s="10" t="s">
         <v>105</v>
       </c>
-      <c r="J43" s="10" t="s">
+      <c r="J43" s="10">
+        <v>1</v>
+      </c>
+      <c r="K43" s="10" t="s">
         <v>199</v>
       </c>
-      <c r="K43" s="11" t="s">
+      <c r="L43" s="11" t="s">
         <v>137</v>
       </c>
-      <c r="L43" s="12" t="s">
+      <c r="M43" s="12" t="s">
         <v>50</v>
       </c>
-      <c r="M43" s="13">
-        <v>0</v>
-      </c>
-      <c r="N43" s="14" t="s">
+      <c r="N43" s="13">
+        <v>0</v>
+      </c>
+      <c r="O43" s="14" t="s">
         <v>109</v>
       </c>
-      <c r="O43" s="29" t="s">
+      <c r="P43" s="29" t="s">
         <v>176</v>
       </c>
-      <c r="P43" s="9">
+      <c r="Q43" s="9">
         <v>12</v>
       </c>
-      <c r="Q43" s="18" t="s">
-        <v>108</v>
-      </c>
-      <c r="R43" s="9"/>
-    </row>
-    <row r="44" spans="1:18">
+      <c r="R43" s="18" t="s">
+        <v>108</v>
+      </c>
+      <c r="S43" s="9"/>
+    </row>
+    <row r="44" spans="1:19">
       <c r="A44" s="24">
         <v>44</v>
       </c>
@@ -3680,33 +3816,36 @@
       <c r="I44" s="10" t="s">
         <v>105</v>
       </c>
-      <c r="J44" s="12" t="s">
+      <c r="J44" s="10">
+        <v>1</v>
+      </c>
+      <c r="K44" s="12" t="s">
         <v>201</v>
       </c>
-      <c r="K44" s="11" t="s">
+      <c r="L44" s="11" t="s">
         <v>138</v>
       </c>
-      <c r="L44" s="12" t="s">
+      <c r="M44" s="12" t="s">
         <v>50</v>
       </c>
-      <c r="M44" s="13">
-        <v>0</v>
-      </c>
-      <c r="N44" s="14" t="s">
+      <c r="N44" s="13">
+        <v>0</v>
+      </c>
+      <c r="O44" s="14" t="s">
         <v>109</v>
       </c>
-      <c r="O44" s="33" t="s">
+      <c r="P44" s="33" t="s">
         <v>123</v>
       </c>
-      <c r="P44" s="9">
+      <c r="Q44" s="9">
         <v>9</v>
       </c>
-      <c r="Q44" s="18" t="s">
-        <v>108</v>
-      </c>
-      <c r="R44" s="9"/>
-    </row>
-    <row r="45" spans="1:18">
+      <c r="R44" s="18" t="s">
+        <v>108</v>
+      </c>
+      <c r="S44" s="9"/>
+    </row>
+    <row r="45" spans="1:19">
       <c r="A45" s="24">
         <v>45</v>
       </c>
@@ -3735,33 +3874,36 @@
       <c r="I45" s="10" t="s">
         <v>105</v>
       </c>
-      <c r="J45" s="10" t="s">
+      <c r="J45" s="10">
+        <v>1</v>
+      </c>
+      <c r="K45" s="10" t="s">
         <v>200</v>
       </c>
-      <c r="K45" s="11" t="s">
+      <c r="L45" s="11" t="s">
         <v>139</v>
       </c>
-      <c r="L45" s="12" t="s">
+      <c r="M45" s="12" t="s">
         <v>50</v>
       </c>
-      <c r="M45" s="13">
-        <v>0</v>
-      </c>
-      <c r="N45" s="14" t="s">
+      <c r="N45" s="13">
+        <v>0</v>
+      </c>
+      <c r="O45" s="14" t="s">
         <v>109</v>
       </c>
-      <c r="O45" s="34" t="s">
+      <c r="P45" s="34" t="s">
         <v>123</v>
       </c>
-      <c r="P45" s="9">
+      <c r="Q45" s="9">
         <v>10</v>
       </c>
-      <c r="Q45" s="18" t="s">
-        <v>108</v>
-      </c>
-      <c r="R45" s="9"/>
-    </row>
-    <row r="46" spans="1:18" ht="19" customHeight="1">
+      <c r="R45" s="18" t="s">
+        <v>108</v>
+      </c>
+      <c r="S45" s="9"/>
+    </row>
+    <row r="46" spans="1:19" ht="19" customHeight="1">
       <c r="A46" s="24">
         <v>46</v>
       </c>
@@ -3790,33 +3932,36 @@
       <c r="I46" s="25" t="s">
         <v>105</v>
       </c>
-      <c r="J46" s="25" t="s">
+      <c r="J46" s="10">
+        <v>1</v>
+      </c>
+      <c r="K46" s="25" t="s">
         <v>70</v>
       </c>
-      <c r="K46" s="26" t="s">
+      <c r="L46" s="26" t="s">
         <v>140</v>
       </c>
-      <c r="L46" s="24" t="s">
+      <c r="M46" s="24" t="s">
         <v>100</v>
       </c>
-      <c r="M46" s="27">
-        <v>0</v>
-      </c>
-      <c r="N46" s="32" t="s">
+      <c r="N46" s="27">
+        <v>0</v>
+      </c>
+      <c r="O46" s="32" t="s">
         <v>109</v>
       </c>
-      <c r="O46" s="35" t="s">
+      <c r="P46" s="35" t="s">
         <v>173</v>
       </c>
-      <c r="P46" s="30">
+      <c r="Q46" s="30">
         <v>41</v>
       </c>
-      <c r="Q46" s="31" t="s">
-        <v>108</v>
-      </c>
-      <c r="R46" s="17"/>
-    </row>
-    <row r="47" spans="1:18">
+      <c r="R46" s="31" t="s">
+        <v>108</v>
+      </c>
+      <c r="S46" s="17"/>
+    </row>
+    <row r="47" spans="1:19">
       <c r="A47" s="24">
         <v>47</v>
       </c>
@@ -3845,33 +3990,36 @@
       <c r="I47" s="25" t="s">
         <v>106</v>
       </c>
-      <c r="J47" s="25" t="s">
+      <c r="J47" s="10">
+        <v>1</v>
+      </c>
+      <c r="K47" s="25" t="s">
         <v>72</v>
       </c>
-      <c r="K47" s="26" t="s">
+      <c r="L47" s="26" t="s">
         <v>156</v>
       </c>
-      <c r="L47" s="24" t="s">
+      <c r="M47" s="24" t="s">
         <v>100</v>
       </c>
-      <c r="M47" s="27">
-        <v>0</v>
-      </c>
-      <c r="N47" s="32" t="s">
+      <c r="N47" s="27">
+        <v>0</v>
+      </c>
+      <c r="O47" s="32" t="s">
         <v>116</v>
       </c>
-      <c r="O47" s="35" t="s">
+      <c r="P47" s="35" t="s">
         <v>173</v>
       </c>
-      <c r="P47" s="30">
+      <c r="Q47" s="30">
         <v>42</v>
       </c>
-      <c r="Q47" s="31" t="s">
-        <v>108</v>
-      </c>
-      <c r="R47" s="17"/>
-    </row>
-    <row r="48" spans="1:18">
+      <c r="R47" s="31" t="s">
+        <v>108</v>
+      </c>
+      <c r="S47" s="17"/>
+    </row>
+    <row r="48" spans="1:19">
       <c r="A48" s="24">
         <v>48</v>
       </c>
@@ -3900,33 +4048,36 @@
       <c r="I48" s="25" t="s">
         <v>105</v>
       </c>
-      <c r="J48" s="25" t="s">
+      <c r="J48" s="10">
+        <v>1</v>
+      </c>
+      <c r="K48" s="25" t="s">
         <v>74</v>
       </c>
-      <c r="K48" s="26" t="s">
+      <c r="L48" s="26" t="s">
         <v>141</v>
       </c>
-      <c r="L48" s="24" t="s">
+      <c r="M48" s="24" t="s">
         <v>100</v>
       </c>
-      <c r="M48" s="27">
-        <v>0</v>
-      </c>
-      <c r="N48" s="32" t="s">
+      <c r="N48" s="27">
+        <v>0</v>
+      </c>
+      <c r="O48" s="32" t="s">
         <v>109</v>
       </c>
-      <c r="O48" s="36" t="s">
+      <c r="P48" s="36" t="s">
         <v>174</v>
       </c>
-      <c r="P48" s="30">
+      <c r="Q48" s="30">
         <v>37</v>
       </c>
-      <c r="Q48" s="31" t="s">
-        <v>108</v>
-      </c>
-      <c r="R48" s="17"/>
-    </row>
-    <row r="49" spans="1:19">
+      <c r="R48" s="31" t="s">
+        <v>108</v>
+      </c>
+      <c r="S48" s="17"/>
+    </row>
+    <row r="49" spans="1:20">
       <c r="A49" s="24">
         <v>49</v>
       </c>
@@ -3955,33 +4106,36 @@
       <c r="I49" s="25" t="s">
         <v>106</v>
       </c>
-      <c r="J49" s="25" t="s">
+      <c r="J49" s="10">
+        <v>1</v>
+      </c>
+      <c r="K49" s="25" t="s">
         <v>76</v>
       </c>
-      <c r="K49" s="26" t="s">
+      <c r="L49" s="26" t="s">
         <v>157</v>
       </c>
-      <c r="L49" s="24" t="s">
+      <c r="M49" s="24" t="s">
         <v>100</v>
       </c>
-      <c r="M49" s="27">
-        <v>1</v>
-      </c>
-      <c r="N49" s="32" t="s">
+      <c r="N49" s="27">
+        <v>1</v>
+      </c>
+      <c r="O49" s="32" t="s">
         <v>116</v>
       </c>
-      <c r="O49" s="36" t="s">
+      <c r="P49" s="36" t="s">
         <v>174</v>
       </c>
-      <c r="P49" s="30">
+      <c r="Q49" s="30">
         <v>38</v>
       </c>
-      <c r="Q49" s="31" t="s">
-        <v>108</v>
-      </c>
-      <c r="R49" s="17"/>
-    </row>
-    <row r="50" spans="1:19" ht="17" customHeight="1">
+      <c r="R49" s="31" t="s">
+        <v>108</v>
+      </c>
+      <c r="S49" s="17"/>
+    </row>
+    <row r="50" spans="1:20" ht="17" customHeight="1">
       <c r="A50" s="24">
         <v>50</v>
       </c>
@@ -4010,33 +4164,36 @@
       <c r="I50" s="10" t="s">
         <v>104</v>
       </c>
-      <c r="J50" s="10" t="s">
+      <c r="J50" s="10">
+        <v>1</v>
+      </c>
+      <c r="K50" s="10" t="s">
         <v>79</v>
       </c>
-      <c r="K50" s="11" t="s">
+      <c r="L50" s="11" t="s">
         <v>193</v>
       </c>
-      <c r="L50" s="12" t="s">
+      <c r="M50" s="12" t="s">
         <v>77</v>
       </c>
-      <c r="M50" s="13">
-        <v>0</v>
-      </c>
-      <c r="N50" s="14" t="s">
+      <c r="N50" s="13">
+        <v>0</v>
+      </c>
+      <c r="O50" s="14" t="s">
         <v>111</v>
       </c>
-      <c r="O50" s="35" t="s">
+      <c r="P50" s="35" t="s">
         <v>173</v>
       </c>
-      <c r="P50" s="9">
+      <c r="Q50" s="9">
         <v>48</v>
       </c>
-      <c r="Q50" s="18" t="s">
-        <v>108</v>
-      </c>
-      <c r="R50" s="9"/>
-    </row>
-    <row r="51" spans="1:19">
+      <c r="R50" s="18" t="s">
+        <v>108</v>
+      </c>
+      <c r="S50" s="9"/>
+    </row>
+    <row r="51" spans="1:20">
       <c r="A51" s="24">
         <v>51</v>
       </c>
@@ -4065,35 +4222,38 @@
       <c r="I51" s="10" t="s">
         <v>104</v>
       </c>
-      <c r="J51" s="10" t="s">
+      <c r="J51" s="10">
+        <v>1</v>
+      </c>
+      <c r="K51" s="10" t="s">
         <v>81</v>
       </c>
-      <c r="K51" s="11" t="s">
+      <c r="L51" s="11" t="s">
         <v>167</v>
       </c>
-      <c r="L51" s="12" t="s">
+      <c r="M51" s="12" t="s">
         <v>77</v>
       </c>
-      <c r="M51" s="13">
-        <v>0</v>
-      </c>
-      <c r="N51" s="14" t="s">
+      <c r="N51" s="13">
+        <v>0</v>
+      </c>
+      <c r="O51" s="14" t="s">
         <v>111</v>
       </c>
-      <c r="O51" s="35" t="s">
+      <c r="P51" s="35" t="s">
         <v>173</v>
       </c>
-      <c r="P51" s="9">
+      <c r="Q51" s="9">
         <v>44</v>
       </c>
-      <c r="Q51" s="18" t="s">
-        <v>108</v>
-      </c>
-      <c r="R51" s="9" t="s">
+      <c r="R51" s="18" t="s">
+        <v>108</v>
+      </c>
+      <c r="S51" s="9" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="52" spans="1:19">
+    <row r="52" spans="1:20">
       <c r="A52" s="24">
         <v>52</v>
       </c>
@@ -4122,33 +4282,36 @@
       <c r="I52" s="10" t="s">
         <v>104</v>
       </c>
-      <c r="J52" s="10" t="s">
+      <c r="J52" s="10">
+        <v>1</v>
+      </c>
+      <c r="K52" s="10" t="s">
         <v>83</v>
       </c>
-      <c r="K52" s="11" t="s">
+      <c r="L52" s="11" t="s">
         <v>142</v>
       </c>
-      <c r="L52" s="12" t="s">
+      <c r="M52" s="12" t="s">
         <v>77</v>
       </c>
-      <c r="M52" s="13">
-        <v>0</v>
-      </c>
-      <c r="N52" s="14" t="s">
+      <c r="N52" s="13">
+        <v>0</v>
+      </c>
+      <c r="O52" s="14" t="s">
         <v>111</v>
       </c>
-      <c r="O52" s="36" t="s">
+      <c r="P52" s="36" t="s">
         <v>174</v>
       </c>
-      <c r="P52" s="9">
+      <c r="Q52" s="9">
         <v>46</v>
       </c>
-      <c r="Q52" s="18" t="s">
-        <v>108</v>
-      </c>
-      <c r="R52" s="9"/>
-    </row>
-    <row r="53" spans="1:19">
+      <c r="R52" s="18" t="s">
+        <v>108</v>
+      </c>
+      <c r="S52" s="9"/>
+    </row>
+    <row r="53" spans="1:20">
       <c r="A53" s="24">
         <v>53</v>
       </c>
@@ -4177,35 +4340,38 @@
       <c r="I53" s="10" t="s">
         <v>104</v>
       </c>
-      <c r="J53" s="10" t="s">
+      <c r="J53" s="10">
+        <v>1</v>
+      </c>
+      <c r="K53" s="10" t="s">
         <v>85</v>
       </c>
-      <c r="K53" s="11" t="s">
+      <c r="L53" s="11" t="s">
         <v>168</v>
       </c>
-      <c r="L53" s="12" t="s">
+      <c r="M53" s="12" t="s">
         <v>77</v>
       </c>
-      <c r="M53" s="13">
-        <v>0</v>
-      </c>
-      <c r="N53" s="14" t="s">
+      <c r="N53" s="13">
+        <v>0</v>
+      </c>
+      <c r="O53" s="14" t="s">
         <v>111</v>
       </c>
-      <c r="O53" s="36" t="s">
+      <c r="P53" s="36" t="s">
         <v>174</v>
       </c>
-      <c r="P53" s="9">
+      <c r="Q53" s="9">
         <v>40</v>
       </c>
-      <c r="Q53" s="18" t="s">
-        <v>108</v>
-      </c>
-      <c r="R53" s="9" t="s">
+      <c r="R53" s="18" t="s">
+        <v>108</v>
+      </c>
+      <c r="S53" s="9" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="54" spans="1:19">
+    <row r="54" spans="1:20">
       <c r="A54" s="24">
         <v>54</v>
       </c>
@@ -4230,33 +4396,36 @@
       <c r="I54" s="10" t="s">
         <v>105</v>
       </c>
-      <c r="J54" s="10" t="s">
+      <c r="J54" s="10">
+        <v>1</v>
+      </c>
+      <c r="K54" s="10" t="s">
         <v>87</v>
       </c>
-      <c r="K54" s="11" t="s">
+      <c r="L54" s="11" t="s">
         <v>169</v>
       </c>
-      <c r="L54" s="12" t="s">
+      <c r="M54" s="12" t="s">
         <v>77</v>
       </c>
-      <c r="M54" s="13">
-        <v>0</v>
-      </c>
-      <c r="N54" s="14" t="s">
+      <c r="N54" s="13">
+        <v>0</v>
+      </c>
+      <c r="O54" s="14" t="s">
         <v>109</v>
       </c>
-      <c r="O54" s="36" t="s">
+      <c r="P54" s="36" t="s">
         <v>174</v>
       </c>
-      <c r="P54" s="9">
+      <c r="Q54" s="9">
         <v>45</v>
       </c>
-      <c r="Q54" s="18" t="s">
-        <v>108</v>
-      </c>
-      <c r="R54" s="9"/>
-    </row>
-    <row r="55" spans="1:19">
+      <c r="R54" s="18" t="s">
+        <v>108</v>
+      </c>
+      <c r="S54" s="9"/>
+    </row>
+    <row r="55" spans="1:20">
       <c r="A55" s="24">
         <v>55</v>
       </c>
@@ -4281,33 +4450,36 @@
       <c r="I55" s="10" t="s">
         <v>105</v>
       </c>
-      <c r="J55" s="10" t="s">
+      <c r="J55" s="10">
+        <v>1</v>
+      </c>
+      <c r="K55" s="10" t="s">
         <v>89</v>
       </c>
-      <c r="K55" s="11" t="s">
+      <c r="L55" s="11" t="s">
         <v>190</v>
       </c>
-      <c r="L55" s="12" t="s">
+      <c r="M55" s="12" t="s">
         <v>77</v>
       </c>
-      <c r="M55" s="13">
-        <v>0</v>
-      </c>
-      <c r="N55" s="14" t="s">
+      <c r="N55" s="13">
+        <v>0</v>
+      </c>
+      <c r="O55" s="14" t="s">
         <v>109</v>
       </c>
-      <c r="O55" s="35" t="s">
+      <c r="P55" s="35" t="s">
         <v>173</v>
       </c>
-      <c r="P55" s="9">
+      <c r="Q55" s="9">
         <v>47</v>
       </c>
-      <c r="Q55" s="18" t="s">
-        <v>108</v>
-      </c>
-      <c r="R55" s="9"/>
-    </row>
-    <row r="56" spans="1:19">
+      <c r="R55" s="18" t="s">
+        <v>108</v>
+      </c>
+      <c r="S55" s="9"/>
+    </row>
+    <row r="56" spans="1:20">
       <c r="A56" s="24">
         <v>56</v>
       </c>
@@ -4332,33 +4504,36 @@
       <c r="I56" s="10" t="s">
         <v>104</v>
       </c>
-      <c r="J56" s="10" t="s">
+      <c r="J56" s="10">
+        <v>1</v>
+      </c>
+      <c r="K56" s="10" t="s">
         <v>91</v>
       </c>
-      <c r="K56" s="11" t="s">
+      <c r="L56" s="11" t="s">
         <v>170</v>
       </c>
-      <c r="L56" s="12" t="s">
+      <c r="M56" s="12" t="s">
         <v>77</v>
       </c>
-      <c r="M56" s="13">
-        <v>0</v>
-      </c>
-      <c r="N56" s="14" t="s">
+      <c r="N56" s="13">
+        <v>0</v>
+      </c>
+      <c r="O56" s="14" t="s">
         <v>111</v>
       </c>
-      <c r="O56" s="35" t="s">
+      <c r="P56" s="35" t="s">
         <v>173</v>
       </c>
-      <c r="P56" s="9">
+      <c r="Q56" s="9">
         <v>43</v>
       </c>
-      <c r="Q56" s="18" t="s">
-        <v>108</v>
-      </c>
-      <c r="R56" s="9"/>
-    </row>
-    <row r="57" spans="1:19">
+      <c r="R56" s="18" t="s">
+        <v>108</v>
+      </c>
+      <c r="S56" s="9"/>
+    </row>
+    <row r="57" spans="1:20">
       <c r="A57" s="24">
         <v>57</v>
       </c>
@@ -4383,33 +4558,36 @@
       <c r="I57" s="10" t="s">
         <v>104</v>
       </c>
-      <c r="J57" s="10" t="s">
+      <c r="J57" s="10">
+        <v>1</v>
+      </c>
+      <c r="K57" s="10" t="s">
         <v>93</v>
       </c>
-      <c r="K57" s="11" t="s">
+      <c r="L57" s="11" t="s">
         <v>171</v>
       </c>
-      <c r="L57" s="12" t="s">
+      <c r="M57" s="12" t="s">
         <v>77</v>
       </c>
-      <c r="M57" s="13">
-        <v>0</v>
-      </c>
-      <c r="N57" s="14" t="s">
+      <c r="N57" s="13">
+        <v>0</v>
+      </c>
+      <c r="O57" s="14" t="s">
         <v>111</v>
       </c>
-      <c r="O57" s="36" t="s">
+      <c r="P57" s="36" t="s">
         <v>174</v>
       </c>
-      <c r="P57" s="9">
+      <c r="Q57" s="9">
         <v>39</v>
       </c>
-      <c r="Q57" s="18" t="s">
-        <v>108</v>
-      </c>
-      <c r="R57" s="9"/>
-    </row>
-    <row r="58" spans="1:19" s="6" customFormat="1">
+      <c r="R57" s="18" t="s">
+        <v>108</v>
+      </c>
+      <c r="S57" s="9"/>
+    </row>
+    <row r="58" spans="1:20" s="6" customFormat="1">
       <c r="A58" s="37">
         <v>9</v>
       </c>
@@ -4437,32 +4615,35 @@
       <c r="I58" s="38" t="s">
         <v>104</v>
       </c>
-      <c r="J58" s="38" t="s">
+      <c r="J58" s="10">
+        <v>1</v>
+      </c>
+      <c r="K58" s="38" t="s">
         <v>119</v>
       </c>
-      <c r="K58" s="7" t="s">
+      <c r="L58" s="7" t="s">
         <v>192</v>
       </c>
-      <c r="L58" s="37" t="s">
+      <c r="M58" s="37" t="s">
         <v>98</v>
       </c>
-      <c r="M58" s="3">
-        <v>1</v>
-      </c>
-      <c r="N58" s="4" t="s">
+      <c r="N58" s="3">
+        <v>1</v>
+      </c>
+      <c r="O58" s="4" t="s">
         <v>111</v>
       </c>
-      <c r="O58" s="39" t="s">
+      <c r="P58" s="39" t="s">
         <v>175</v>
       </c>
-      <c r="P58" s="38">
+      <c r="Q58" s="38">
         <v>16</v>
       </c>
-      <c r="Q58" s="40" t="s">
-        <v>108</v>
-      </c>
-      <c r="R58" s="20"/>
-      <c r="S58"/>
+      <c r="R58" s="40" t="s">
+        <v>108</v>
+      </c>
+      <c r="S58" s="20"/>
+      <c r="T58"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
repair wrong ordering of plots
</commit_message>
<xml_diff>
--- a/data-raw/params_out.xlsx
+++ b/data-raw/params_out.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tsamsonov/GitHub/grwat/data-raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4520BCBE-5D90-9A42-BD06-6083DD975144}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9697C57-5983-6A4A-87ED-C60D5C57F876}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="500" yWindow="1660" windowWidth="28300" windowHeight="14680" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-20" yWindow="460" windowWidth="51200" windowHeight="27220" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="640" uniqueCount="220">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="640" uniqueCount="224">
   <si>
     <t>year_number</t>
   </si>
@@ -688,6 +688,18 @@
   </si>
   <si>
     <t>Test</t>
+  </si>
+  <si>
+    <t>Groundwater runoff during summer</t>
+  </si>
+  <si>
+    <t>Groundwater runoff during winter</t>
+  </si>
+  <si>
+    <t>Summer low flow runoff</t>
+  </si>
+  <si>
+    <t>Winter low flow runoff</t>
   </si>
 </sst>
 </file>
@@ -1304,8 +1316,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:T58"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I42" zoomScale="81" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="N59" sqref="N59"/>
+    <sheetView tabSelected="1" zoomScale="81" zoomScaleNormal="70" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G34" sqref="G34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16"/>
@@ -1778,7 +1791,7 @@
         <v>175</v>
       </c>
       <c r="Q8" s="9">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="R8" s="18" t="s">
         <v>108</v>
@@ -1835,7 +1848,7 @@
         <v>175</v>
       </c>
       <c r="Q9" s="9">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="R9" s="18" t="s">
         <v>108</v>
@@ -1844,7 +1857,7 @@
     </row>
     <row r="10" spans="1:20" s="6" customFormat="1" ht="19" customHeight="1">
       <c r="A10" s="12">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B10" s="20">
         <v>93</v>
@@ -1902,7 +1915,7 @@
     </row>
     <row r="11" spans="1:20" ht="17">
       <c r="A11" s="24">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B11" s="17">
         <v>103</v>
@@ -1959,7 +1972,7 @@
     </row>
     <row r="12" spans="1:20" ht="17">
       <c r="A12" s="24">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B12" s="17">
         <v>113</v>
@@ -2018,7 +2031,7 @@
     </row>
     <row r="13" spans="1:20" ht="17">
       <c r="A13" s="24">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B13" s="17">
         <v>123</v>
@@ -2075,7 +2088,7 @@
     </row>
     <row r="14" spans="1:20" ht="17">
       <c r="A14" s="24">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B14" s="17">
         <v>133</v>
@@ -2134,7 +2147,7 @@
     </row>
     <row r="15" spans="1:20" ht="17">
       <c r="A15" s="24">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B15" s="17">
         <v>143</v>
@@ -2191,7 +2204,7 @@
     </row>
     <row r="16" spans="1:20" ht="17">
       <c r="A16" s="24">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B16" s="17">
         <v>153</v>
@@ -2248,7 +2261,7 @@
     </row>
     <row r="17" spans="1:19" ht="17">
       <c r="A17" s="24">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B17" s="17">
         <v>168</v>
@@ -2292,8 +2305,8 @@
       <c r="O17" s="32" t="s">
         <v>116</v>
       </c>
-      <c r="P17" s="17" t="s">
-        <v>122</v>
+      <c r="P17" s="29" t="s">
+        <v>176</v>
       </c>
       <c r="Q17" s="30">
         <v>0</v>
@@ -2305,7 +2318,7 @@
     </row>
     <row r="18" spans="1:19" ht="17">
       <c r="A18" s="24">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B18" s="17">
         <v>183</v>
@@ -2362,7 +2375,7 @@
     </row>
     <row r="19" spans="1:19" ht="17">
       <c r="A19" s="24">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B19" s="17">
         <v>193</v>
@@ -2419,7 +2432,7 @@
     </row>
     <row r="20" spans="1:19" ht="17">
       <c r="A20" s="24">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B20" s="17">
         <v>208</v>
@@ -2463,8 +2476,8 @@
       <c r="O20" s="32" t="s">
         <v>116</v>
       </c>
-      <c r="P20" s="17" t="s">
-        <v>122</v>
+      <c r="P20" s="34" t="s">
+        <v>123</v>
       </c>
       <c r="Q20" s="30">
         <v>0</v>
@@ -2476,7 +2489,7 @@
     </row>
     <row r="21" spans="1:19" ht="17">
       <c r="A21" s="24">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B21" s="17">
         <v>223</v>
@@ -2533,7 +2546,7 @@
     </row>
     <row r="22" spans="1:19" ht="17">
       <c r="A22" s="24">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B22" s="17">
         <v>233</v>
@@ -2590,7 +2603,7 @@
     </row>
     <row r="23" spans="1:19" ht="17">
       <c r="A23" s="24">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B23" s="17">
         <v>248</v>
@@ -2634,8 +2647,8 @@
       <c r="O23" s="32" t="s">
         <v>116</v>
       </c>
-      <c r="P23" s="17" t="s">
-        <v>122</v>
+      <c r="P23" s="29" t="s">
+        <v>176</v>
       </c>
       <c r="Q23" s="30">
         <v>0</v>
@@ -2647,7 +2660,7 @@
     </row>
     <row r="24" spans="1:19" ht="17">
       <c r="A24" s="24">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B24" s="17">
         <v>263</v>
@@ -2704,7 +2717,7 @@
     </row>
     <row r="25" spans="1:19" ht="17">
       <c r="A25" s="24">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B25" s="17">
         <v>273</v>
@@ -2761,7 +2774,7 @@
     </row>
     <row r="26" spans="1:19" ht="17">
       <c r="A26" s="24">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B26" s="17">
         <v>288</v>
@@ -2805,8 +2818,8 @@
       <c r="O26" s="32" t="s">
         <v>116</v>
       </c>
-      <c r="P26" s="17" t="s">
-        <v>122</v>
+      <c r="P26" s="34" t="s">
+        <v>123</v>
       </c>
       <c r="Q26" s="30">
         <v>0</v>
@@ -2818,7 +2831,7 @@
     </row>
     <row r="27" spans="1:19" ht="17">
       <c r="A27" s="24">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B27" s="17">
         <v>303</v>
@@ -2875,7 +2888,7 @@
     </row>
     <row r="28" spans="1:19" ht="17">
       <c r="A28" s="24">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B28" s="17">
         <v>313</v>
@@ -2932,7 +2945,7 @@
     </row>
     <row r="29" spans="1:19" ht="17">
       <c r="A29" s="24">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B29" s="17">
         <v>328</v>
@@ -2976,8 +2989,8 @@
       <c r="O29" s="32" t="s">
         <v>116</v>
       </c>
-      <c r="P29" s="17" t="s">
-        <v>122</v>
+      <c r="P29" s="29" t="s">
+        <v>176</v>
       </c>
       <c r="Q29" s="30">
         <v>0</v>
@@ -2989,7 +3002,7 @@
     </row>
     <row r="30" spans="1:19" ht="17">
       <c r="A30" s="24">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B30" s="17">
         <v>343</v>
@@ -3046,7 +3059,7 @@
     </row>
     <row r="31" spans="1:19" ht="17">
       <c r="A31" s="24">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B31" s="17">
         <v>353</v>
@@ -3103,7 +3116,7 @@
     </row>
     <row r="32" spans="1:19" ht="17">
       <c r="A32" s="24">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B32" s="17">
         <v>368</v>
@@ -3147,8 +3160,8 @@
       <c r="O32" s="32" t="s">
         <v>116</v>
       </c>
-      <c r="P32" s="17" t="s">
-        <v>122</v>
+      <c r="P32" s="34" t="s">
+        <v>123</v>
       </c>
       <c r="Q32" s="30">
         <v>0</v>
@@ -3159,8 +3172,8 @@
       <c r="S32" s="17"/>
     </row>
     <row r="33" spans="1:19" ht="19" customHeight="1">
-      <c r="A33" s="24">
-        <v>33</v>
+      <c r="A33" s="12">
+        <v>32</v>
       </c>
       <c r="B33" s="9">
         <v>383</v>
@@ -3216,8 +3229,8 @@
       <c r="S33" s="9"/>
     </row>
     <row r="34" spans="1:19" ht="17">
-      <c r="A34" s="24">
-        <v>34</v>
+      <c r="A34" s="12">
+        <v>33</v>
       </c>
       <c r="B34" s="9">
         <v>396</v>
@@ -3273,8 +3286,8 @@
       <c r="S34" s="9"/>
     </row>
     <row r="35" spans="1:19" ht="17">
-      <c r="A35" s="24">
-        <v>35</v>
+      <c r="A35" s="12">
+        <v>34</v>
       </c>
       <c r="B35" s="9">
         <v>409</v>
@@ -3318,8 +3331,8 @@
       <c r="O35" s="14" t="s">
         <v>109</v>
       </c>
-      <c r="P35" s="10" t="s">
-        <v>172</v>
+      <c r="P35" s="19" t="s">
+        <v>175</v>
       </c>
       <c r="Q35" s="9">
         <v>4</v>
@@ -3330,8 +3343,8 @@
       <c r="S35" s="9"/>
     </row>
     <row r="36" spans="1:19" ht="17">
-      <c r="A36" s="24">
-        <v>36</v>
+      <c r="A36" s="12">
+        <v>35</v>
       </c>
       <c r="B36" s="9">
         <v>422</v>
@@ -3375,8 +3388,8 @@
       <c r="O36" s="14" t="s">
         <v>109</v>
       </c>
-      <c r="P36" s="10" t="s">
-        <v>172</v>
+      <c r="P36" s="19" t="s">
+        <v>175</v>
       </c>
       <c r="Q36" s="9">
         <v>2</v>
@@ -3387,8 +3400,8 @@
       <c r="S36" s="9"/>
     </row>
     <row r="37" spans="1:19" ht="17">
-      <c r="A37" s="24">
-        <v>37</v>
+      <c r="A37" s="12">
+        <v>36</v>
       </c>
       <c r="B37" s="9">
         <v>435</v>
@@ -3436,7 +3449,7 @@
         <v>175</v>
       </c>
       <c r="Q37" s="9">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="R37" s="18" t="s">
         <v>108</v>
@@ -3444,8 +3457,8 @@
       <c r="S37" s="9"/>
     </row>
     <row r="38" spans="1:19" ht="17">
-      <c r="A38" s="24">
-        <v>38</v>
+      <c r="A38" s="12">
+        <v>37</v>
       </c>
       <c r="B38" s="9">
         <v>448</v>
@@ -3489,8 +3502,8 @@
       <c r="O38" s="14" t="s">
         <v>109</v>
       </c>
-      <c r="P38" s="10" t="s">
-        <v>172</v>
+      <c r="P38" s="35" t="s">
+        <v>173</v>
       </c>
       <c r="Q38" s="9">
         <v>6</v>
@@ -3501,8 +3514,8 @@
       <c r="S38" s="9"/>
     </row>
     <row r="39" spans="1:19" ht="17">
-      <c r="A39" s="24">
-        <v>39</v>
+      <c r="A39" s="12">
+        <v>38</v>
       </c>
       <c r="B39" s="9">
         <v>461</v>
@@ -3546,8 +3559,8 @@
       <c r="O39" s="14" t="s">
         <v>109</v>
       </c>
-      <c r="P39" s="10" t="s">
-        <v>172</v>
+      <c r="P39" s="35" t="s">
+        <v>173</v>
       </c>
       <c r="Q39" s="9">
         <v>5</v>
@@ -3558,8 +3571,8 @@
       <c r="S39" s="9"/>
     </row>
     <row r="40" spans="1:19" ht="17">
-      <c r="A40" s="24">
-        <v>40</v>
+      <c r="A40" s="12">
+        <v>39</v>
       </c>
       <c r="B40" s="9">
         <v>474</v>
@@ -3603,8 +3616,8 @@
       <c r="O40" s="14" t="s">
         <v>109</v>
       </c>
-      <c r="P40" s="10" t="s">
-        <v>172</v>
+      <c r="P40" s="36" t="s">
+        <v>174</v>
       </c>
       <c r="Q40" s="9">
         <v>8</v>
@@ -3615,8 +3628,8 @@
       <c r="S40" s="9"/>
     </row>
     <row r="41" spans="1:19" ht="17">
-      <c r="A41" s="24">
-        <v>41</v>
+      <c r="A41" s="12">
+        <v>40</v>
       </c>
       <c r="B41" s="9">
         <v>487</v>
@@ -3660,8 +3673,8 @@
       <c r="O41" s="14" t="s">
         <v>109</v>
       </c>
-      <c r="P41" s="10" t="s">
-        <v>172</v>
+      <c r="P41" s="36" t="s">
+        <v>174</v>
       </c>
       <c r="Q41" s="9">
         <v>7</v>
@@ -3672,8 +3685,8 @@
       <c r="S41" s="9"/>
     </row>
     <row r="42" spans="1:19" ht="17">
-      <c r="A42" s="24">
-        <v>42</v>
+      <c r="A42" s="12">
+        <v>41</v>
       </c>
       <c r="B42" s="9">
         <f>B41+C41</f>
@@ -3685,7 +3698,7 @@
       <c r="D42" s="9">
         <v>1</v>
       </c>
-      <c r="E42" s="10" t="s">
+      <c r="E42" s="35" t="s">
         <v>194</v>
       </c>
       <c r="F42" s="10" t="s">
@@ -3707,7 +3720,7 @@
         <v>198</v>
       </c>
       <c r="L42" s="11" t="s">
-        <v>136</v>
+        <v>220</v>
       </c>
       <c r="M42" s="12" t="s">
         <v>50</v>
@@ -3730,11 +3743,11 @@
       <c r="S42" s="9"/>
     </row>
     <row r="43" spans="1:19" ht="17">
-      <c r="A43" s="24">
-        <v>43</v>
+      <c r="A43" s="12">
+        <v>42</v>
       </c>
       <c r="B43" s="9">
-        <f t="shared" ref="B43:B45" si="0">B42+C42</f>
+        <f>B42+C42</f>
         <v>513</v>
       </c>
       <c r="C43" s="9">
@@ -3743,7 +3756,7 @@
       <c r="D43" s="9">
         <v>1</v>
       </c>
-      <c r="E43" s="10" t="s">
+      <c r="E43" s="35" t="s">
         <v>195</v>
       </c>
       <c r="F43" s="10" t="s">
@@ -3765,7 +3778,7 @@
         <v>199</v>
       </c>
       <c r="L43" s="11" t="s">
-        <v>137</v>
+        <v>222</v>
       </c>
       <c r="M43" s="12" t="s">
         <v>50</v>
@@ -3788,11 +3801,11 @@
       <c r="S43" s="9"/>
     </row>
     <row r="44" spans="1:19" ht="17">
-      <c r="A44" s="24">
-        <v>44</v>
+      <c r="A44" s="12">
+        <v>43</v>
       </c>
       <c r="B44" s="9">
-        <f t="shared" si="0"/>
+        <f>B43+C43</f>
         <v>526</v>
       </c>
       <c r="C44" s="9">
@@ -3801,7 +3814,7 @@
       <c r="D44" s="9">
         <v>1</v>
       </c>
-      <c r="E44" s="10" t="s">
+      <c r="E44" s="35" t="s">
         <v>196</v>
       </c>
       <c r="F44" s="10" t="s">
@@ -3823,7 +3836,7 @@
         <v>201</v>
       </c>
       <c r="L44" s="11" t="s">
-        <v>138</v>
+        <v>221</v>
       </c>
       <c r="M44" s="12" t="s">
         <v>50</v>
@@ -3846,11 +3859,11 @@
       <c r="S44" s="9"/>
     </row>
     <row r="45" spans="1:19" ht="17">
-      <c r="A45" s="24">
-        <v>45</v>
+      <c r="A45" s="12">
+        <v>44</v>
       </c>
       <c r="B45" s="9">
-        <f t="shared" si="0"/>
+        <f>B44+C44</f>
         <v>539</v>
       </c>
       <c r="C45" s="9">
@@ -3859,7 +3872,7 @@
       <c r="D45" s="9">
         <v>1</v>
       </c>
-      <c r="E45" s="10" t="s">
+      <c r="E45" s="35" t="s">
         <v>197</v>
       </c>
       <c r="F45" s="10" t="s">
@@ -3881,7 +3894,7 @@
         <v>200</v>
       </c>
       <c r="L45" s="11" t="s">
-        <v>139</v>
+        <v>223</v>
       </c>
       <c r="M45" s="12" t="s">
         <v>50</v>
@@ -3905,7 +3918,7 @@
     </row>
     <row r="46" spans="1:19" ht="19" customHeight="1">
       <c r="A46" s="24">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B46" s="17">
         <f>B45+C45</f>
@@ -3963,10 +3976,10 @@
     </row>
     <row r="47" spans="1:19" ht="17">
       <c r="A47" s="24">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B47" s="17">
-        <f t="shared" ref="B47:B49" si="1">B46+C46</f>
+        <f>B46+C46</f>
         <v>562</v>
       </c>
       <c r="C47" s="17">
@@ -4021,10 +4034,10 @@
     </row>
     <row r="48" spans="1:19" ht="17">
       <c r="A48" s="24">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B48" s="17">
-        <f t="shared" si="1"/>
+        <f>B47+C47</f>
         <v>577</v>
       </c>
       <c r="C48" s="17">
@@ -4079,10 +4092,10 @@
     </row>
     <row r="49" spans="1:20" ht="17">
       <c r="A49" s="24">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B49" s="17">
-        <f t="shared" si="1"/>
+        <f>B48+C48</f>
         <v>587</v>
       </c>
       <c r="C49" s="17">
@@ -4136,8 +4149,8 @@
       <c r="S49" s="17"/>
     </row>
     <row r="50" spans="1:20" ht="17" customHeight="1">
-      <c r="A50" s="24">
-        <v>50</v>
+      <c r="A50" s="12">
+        <v>49</v>
       </c>
       <c r="B50" s="9">
         <f>B49+C49</f>
@@ -4182,8 +4195,8 @@
       <c r="O50" s="14" t="s">
         <v>111</v>
       </c>
-      <c r="P50" s="35" t="s">
-        <v>173</v>
+      <c r="P50" s="29" t="s">
+        <v>176</v>
       </c>
       <c r="Q50" s="9">
         <v>48</v>
@@ -4194,11 +4207,11 @@
       <c r="S50" s="9"/>
     </row>
     <row r="51" spans="1:20" ht="17">
-      <c r="A51" s="24">
-        <v>51</v>
+      <c r="A51" s="12">
+        <v>50</v>
       </c>
       <c r="B51" s="9">
-        <f t="shared" ref="B51:B57" si="2">B50+C50</f>
+        <f>B50+C50</f>
         <v>612</v>
       </c>
       <c r="C51" s="9">
@@ -4254,11 +4267,11 @@
       </c>
     </row>
     <row r="52" spans="1:20" ht="17">
-      <c r="A52" s="24">
-        <v>52</v>
+      <c r="A52" s="12">
+        <v>51</v>
       </c>
       <c r="B52" s="9">
-        <f t="shared" si="2"/>
+        <f>B51+C51</f>
         <v>622</v>
       </c>
       <c r="C52" s="9">
@@ -4300,8 +4313,8 @@
       <c r="O52" s="14" t="s">
         <v>111</v>
       </c>
-      <c r="P52" s="36" t="s">
-        <v>174</v>
+      <c r="P52" s="34" t="s">
+        <v>123</v>
       </c>
       <c r="Q52" s="9">
         <v>46</v>
@@ -4312,11 +4325,11 @@
       <c r="S52" s="9"/>
     </row>
     <row r="53" spans="1:20" ht="17">
-      <c r="A53" s="24">
-        <v>53</v>
+      <c r="A53" s="12">
+        <v>52</v>
       </c>
       <c r="B53" s="9">
-        <f t="shared" si="2"/>
+        <f>B52+C52</f>
         <v>632</v>
       </c>
       <c r="C53" s="9">
@@ -4372,11 +4385,11 @@
       </c>
     </row>
     <row r="54" spans="1:20" ht="17">
-      <c r="A54" s="24">
-        <v>54</v>
+      <c r="A54" s="12">
+        <v>53</v>
       </c>
       <c r="B54" s="9">
-        <f t="shared" si="2"/>
+        <f>B53+C53</f>
         <v>642</v>
       </c>
       <c r="C54" s="9">
@@ -4414,8 +4427,8 @@
       <c r="O54" s="14" t="s">
         <v>109</v>
       </c>
-      <c r="P54" s="36" t="s">
-        <v>174</v>
+      <c r="P54" s="34" t="s">
+        <v>123</v>
       </c>
       <c r="Q54" s="9">
         <v>45</v>
@@ -4426,11 +4439,11 @@
       <c r="S54" s="9"/>
     </row>
     <row r="55" spans="1:20" ht="17">
-      <c r="A55" s="24">
-        <v>55</v>
+      <c r="A55" s="12">
+        <v>54</v>
       </c>
       <c r="B55" s="9">
-        <f t="shared" si="2"/>
+        <f>B54+C54</f>
         <v>649</v>
       </c>
       <c r="C55" s="9">
@@ -4468,8 +4481,8 @@
       <c r="O55" s="14" t="s">
         <v>109</v>
       </c>
-      <c r="P55" s="35" t="s">
-        <v>173</v>
+      <c r="P55" s="29" t="s">
+        <v>176</v>
       </c>
       <c r="Q55" s="9">
         <v>47</v>
@@ -4480,11 +4493,11 @@
       <c r="S55" s="9"/>
     </row>
     <row r="56" spans="1:20" ht="17">
-      <c r="A56" s="24">
-        <v>56</v>
+      <c r="A56" s="12">
+        <v>55</v>
       </c>
       <c r="B56" s="9">
-        <f t="shared" si="2"/>
+        <f>B55+C55</f>
         <v>656</v>
       </c>
       <c r="C56" s="9">
@@ -4534,11 +4547,11 @@
       <c r="S56" s="9"/>
     </row>
     <row r="57" spans="1:20" ht="17">
-      <c r="A57" s="24">
-        <v>57</v>
+      <c r="A57" s="12">
+        <v>56</v>
       </c>
       <c r="B57" s="9">
-        <f t="shared" si="2"/>
+        <f>B56+C56</f>
         <v>666</v>
       </c>
       <c r="C57" s="9">
@@ -4588,8 +4601,8 @@
       <c r="S57" s="9"/>
     </row>
     <row r="58" spans="1:20" s="6" customFormat="1" ht="17">
-      <c r="A58" s="37">
-        <v>9</v>
+      <c r="A58" s="12">
+        <v>57</v>
       </c>
       <c r="B58" s="5">
         <v>0</v>
@@ -4637,7 +4650,7 @@
         <v>175</v>
       </c>
       <c r="Q58" s="38">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="R58" s="40" t="s">
         <v>108</v>
@@ -4646,6 +4659,9 @@
       <c r="T58"/>
     </row>
   </sheetData>
+  <sortState ref="A2:S58">
+    <sortCondition ref="A2:A58"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="0" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
add support for Ukrainian language
</commit_message>
<xml_diff>
--- a/data-raw/params_out.xlsx
+++ b/data-raw/params_out.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10411"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10410"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tsamsonov/GitHub/grwat/data-raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A2A6560-1C18-0D4F-9B3C-449B9B81372D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C006B90D-54B6-B84D-9A82-8B350920839F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="13500" yWindow="560" windowWidth="51200" windowHeight="26860" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="560" windowWidth="51200" windowHeight="26860" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
@@ -20,6 +20,14 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
     </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
     </ext>
@@ -28,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="640" uniqueCount="224">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="751" uniqueCount="286">
   <si>
     <t>year_number</t>
   </si>
@@ -700,6 +708,192 @@
   </si>
   <si>
     <t>Winter low flow runoff</t>
+  </si>
+  <si>
+    <t>Номер водогосподарського року в ряду спостережень</t>
+  </si>
+  <si>
+    <t>Рік, коли починається водогосподарський рік</t>
+  </si>
+  <si>
+    <t>Рік, коли закінчується водогосподарський рік</t>
+  </si>
+  <si>
+    <t>Дата початку повені</t>
+  </si>
+  <si>
+    <t>Дата закінчення повені</t>
+  </si>
+  <si>
+    <t>Тривалість повені</t>
+  </si>
+  <si>
+    <t>Середня витрата за водохозяйственнй рік</t>
+  </si>
+  <si>
+    <t>Максимальна витрата за водогосподарський рік</t>
+  </si>
+  <si>
+    <t>Дата максимальної витрати за водогосподарський рік</t>
+  </si>
+  <si>
+    <t>Середня витрата грунтових вод за водогосподарський рік</t>
+  </si>
+  <si>
+    <t>Мінімальний місячний витрата за літо</t>
+  </si>
+  <si>
+    <t>Місяць мінімального місячного витрати за літо</t>
+  </si>
+  <si>
+    <t>Мінімальний місячний витрата за зиму</t>
+  </si>
+  <si>
+    <t>Місяць мінімального місячного витрати за зиму</t>
+  </si>
+  <si>
+    <t>Мінімальний 30-добовий витрата за літо</t>
+  </si>
+  <si>
+    <t>Дата початку мінімальної 30-добової витрати за літо</t>
+  </si>
+  <si>
+    <t>Дата закінчення мінімальної 30-добової витрати за літо</t>
+  </si>
+  <si>
+    <t>Мінімальний 30-добовий витрата за зиму</t>
+  </si>
+  <si>
+    <t>Дата початку мінімальної 30-добової витрати за зиму</t>
+  </si>
+  <si>
+    <t>Дата закінчення мінімальної 30-добової витрати за зиму</t>
+  </si>
+  <si>
+    <t>Мінімальна 10-добова витрата за літо</t>
+  </si>
+  <si>
+    <t>Дата початку мінімальної 10-добової витрати за літо</t>
+  </si>
+  <si>
+    <t>Дата закінчення мінімальної 10-добової витрати за літо</t>
+  </si>
+  <si>
+    <t>Мінімальний 10-добовий витрата за зиму</t>
+  </si>
+  <si>
+    <t>Дата початку мінімальної 10-добової витрати за зиму</t>
+  </si>
+  <si>
+    <t>Дата закінчення мінімальної 10-добової витрати за зиму</t>
+  </si>
+  <si>
+    <t>Мінімальний 5-добовий витрата за літо</t>
+  </si>
+  <si>
+    <t>Дата початку мінімальної 5-добової витрати за літо</t>
+  </si>
+  <si>
+    <t>Дата закінчення мінімальної 5-добової витрати за літо</t>
+  </si>
+  <si>
+    <t>Мінімальний 5-добовий витрата за зиму</t>
+  </si>
+  <si>
+    <t>Дата початку мінімальної 5-добової витрати за зиму</t>
+  </si>
+  <si>
+    <t>Дата закінчення мінімальної 5-добової витрати за зиму</t>
+  </si>
+  <si>
+    <t>Обсяг річного стоку</t>
+  </si>
+  <si>
+    <t>Обсяг грунтового стоку</t>
+  </si>
+  <si>
+    <t>Обсяг повені без грунтової складової</t>
+  </si>
+  <si>
+    <t>Обсяг повені разом з об'ємом грунтової складової стоку</t>
+  </si>
+  <si>
+    <t>Обсяг повені разом з накладеними дощовими паводками і грунтовим стоком</t>
+  </si>
+  <si>
+    <t>Обсяг дощового стоку без грунтової складової</t>
+  </si>
+  <si>
+    <t>Обсяг дощового стоку разом з об'ємом грунтової складової стоку</t>
+  </si>
+  <si>
+    <t>Обсяг відлигового стоку без грунтової складової</t>
+  </si>
+  <si>
+    <t>Обсяг відлигового стоку разом з об'ємом грунтової складової стоку</t>
+  </si>
+  <si>
+    <t>Обсяг грунтового стоку влітку</t>
+  </si>
+  <si>
+    <t>Обсяг стоку літньої межені</t>
+  </si>
+  <si>
+    <t>Обсяг грунтового стоку взимку</t>
+  </si>
+  <si>
+    <t>Обсяг стоку зимової межені</t>
+  </si>
+  <si>
+    <t>Максимальна витрата дощових паводків</t>
+  </si>
+  <si>
+    <t>Максимальна витрата відлигових паводків</t>
+  </si>
+  <si>
+    <t>Дата максимальної витрати дощових паводків</t>
+  </si>
+  <si>
+    <t>Дата максимальної витрати відлигових паводків</t>
+  </si>
+  <si>
+    <t>Тривалість літньо-осінньої межені</t>
+  </si>
+  <si>
+    <t>Кількість днів з паводками в літньо-осінній межені</t>
+  </si>
+  <si>
+    <t>Тривалість зимової межені</t>
+  </si>
+  <si>
+    <t>Кількість днів з паводками в зимовій межені</t>
+  </si>
+  <si>
+    <t>Відносна мінливість витрати води в зимову межень</t>
+  </si>
+  <si>
+    <t>Відносна мінливість витрати води в літню межень</t>
+  </si>
+  <si>
+    <t>Кількість дощових паводків</t>
+  </si>
+  <si>
+    <t>Кількість оттепельных паводків</t>
+  </si>
+  <si>
+    <t>Descua</t>
+  </si>
+  <si>
+    <t>Unitsua</t>
+  </si>
+  <si>
+    <t>Рок</t>
+  </si>
+  <si>
+    <t>Місяць</t>
+  </si>
+  <si>
+    <t>Днів</t>
   </si>
 </sst>
 </file>
@@ -1296,11 +1490,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:T58"/>
+  <dimension ref="A1:V58"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="81" zoomScaleNormal="70" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G27" sqref="G27"/>
+      <selection pane="bottomLeft" activeCell="G55" sqref="G55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.85546875" defaultRowHeight="16"/>
@@ -1311,22 +1505,23 @@
     <col min="4" max="4" width="7.28515625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="15" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="7" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="8.140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.42578125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="7.42578125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="7.42578125" customWidth="1"/>
-    <col min="11" max="11" width="75.7109375" customWidth="1"/>
-    <col min="12" max="12" width="61.7109375" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="34.28515625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="7.42578125" style="2" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="6.42578125" style="2" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="14.140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="6.85546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="11.7109375" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="50.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="7" customWidth="1"/>
+    <col min="8" max="8" width="8.140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="7.42578125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="7.42578125" customWidth="1"/>
+    <col min="12" max="13" width="75.7109375" customWidth="1"/>
+    <col min="14" max="14" width="61.7109375" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="34.28515625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="7.42578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="6.42578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="14.140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="6.85546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="50.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" s="1" customFormat="1" ht="19" customHeight="1">
+    <row r="1" spans="1:22" s="1" customFormat="1" ht="19" customHeight="1">
       <c r="A1" s="11" t="s">
         <v>95</v>
       </c>
@@ -1346,46 +1541,52 @@
         <v>97</v>
       </c>
       <c r="G1" s="11" t="s">
+        <v>282</v>
+      </c>
+      <c r="H1" s="11" t="s">
         <v>178</v>
       </c>
-      <c r="H1" s="11" t="s">
+      <c r="I1" s="11" t="s">
         <v>218</v>
       </c>
-      <c r="I1" s="11" t="s">
+      <c r="J1" s="11" t="s">
         <v>103</v>
       </c>
-      <c r="J1" s="11" t="s">
+      <c r="K1" s="11" t="s">
         <v>219</v>
       </c>
-      <c r="K1" s="11" t="s">
+      <c r="L1" s="11" t="s">
         <v>177</v>
       </c>
-      <c r="L1" s="11" t="s">
+      <c r="M1" s="11" t="s">
+        <v>281</v>
+      </c>
+      <c r="N1" s="11" t="s">
         <v>143</v>
       </c>
-      <c r="M1" s="11" t="s">
+      <c r="O1" s="11" t="s">
         <v>94</v>
       </c>
-      <c r="N1" s="11" t="s">
+      <c r="P1" s="11" t="s">
         <v>107</v>
       </c>
-      <c r="O1" s="11" t="s">
+      <c r="Q1" s="11" t="s">
         <v>110</v>
       </c>
-      <c r="P1" s="11" t="s">
+      <c r="R1" s="11" t="s">
         <v>118</v>
       </c>
-      <c r="Q1" s="11" t="s">
+      <c r="S1" s="11" t="s">
         <v>117</v>
       </c>
-      <c r="R1" s="12" t="s">
+      <c r="T1" s="12" t="s">
         <v>217</v>
       </c>
-      <c r="S1" s="4" t="s">
+      <c r="U1" s="4" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="2" spans="1:20" ht="17" customHeight="1">
+    <row r="2" spans="1:22" ht="17" customHeight="1">
       <c r="A2" s="8">
         <v>1</v>
       </c>
@@ -1403,42 +1604,46 @@
       </c>
       <c r="F2" s="6"/>
       <c r="G2" s="6"/>
-      <c r="H2" s="6" t="s">
-        <v>104</v>
-      </c>
+      <c r="H2" s="6"/>
       <c r="I2" s="6" t="s">
         <v>104</v>
       </c>
-      <c r="J2" s="6">
-        <v>0</v>
-      </c>
-      <c r="K2" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="L2" s="7" t="s">
+      <c r="J2" s="6" t="s">
+        <v>104</v>
+      </c>
+      <c r="K2" s="6">
+        <v>0</v>
+      </c>
+      <c r="L2" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="M2" s="6" t="s">
+        <v>224</v>
+      </c>
+      <c r="N2" s="7" t="s">
         <v>153</v>
       </c>
-      <c r="M2" s="8" t="s">
+      <c r="O2" s="8" t="s">
         <v>98</v>
       </c>
-      <c r="N2" s="9">
-        <v>0</v>
-      </c>
-      <c r="O2" s="10" t="s">
+      <c r="P2" s="9">
+        <v>0</v>
+      </c>
+      <c r="Q2" s="10" t="s">
         <v>112</v>
       </c>
-      <c r="P2" s="13" t="s">
+      <c r="R2" s="13" t="s">
         <v>122</v>
       </c>
-      <c r="Q2" s="5">
-        <v>0</v>
-      </c>
-      <c r="R2" s="14" t="s">
-        <v>108</v>
-      </c>
-      <c r="S2" s="5"/>
-    </row>
-    <row r="3" spans="1:20" ht="17">
+      <c r="S2" s="5">
+        <v>0</v>
+      </c>
+      <c r="T2" s="14" t="s">
+        <v>108</v>
+      </c>
+      <c r="U2" s="5"/>
+    </row>
+    <row r="3" spans="1:22" ht="17">
       <c r="A3" s="8">
         <v>2</v>
       </c>
@@ -1458,44 +1663,50 @@
         <v>184</v>
       </c>
       <c r="G3" s="6" t="s">
+        <v>283</v>
+      </c>
+      <c r="H3" s="6" t="s">
         <v>179</v>
-      </c>
-      <c r="H3" s="6" t="s">
-        <v>104</v>
       </c>
       <c r="I3" s="6" t="s">
         <v>104</v>
       </c>
-      <c r="J3" s="6">
-        <v>0</v>
-      </c>
-      <c r="K3" s="6" t="s">
+      <c r="J3" s="6" t="s">
+        <v>104</v>
+      </c>
+      <c r="K3" s="6">
+        <v>0</v>
+      </c>
+      <c r="L3" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="L3" s="7" t="s">
+      <c r="M3" s="6" t="s">
+        <v>225</v>
+      </c>
+      <c r="N3" s="7" t="s">
         <v>188</v>
       </c>
-      <c r="M3" s="8" t="s">
+      <c r="O3" s="8" t="s">
         <v>98</v>
       </c>
-      <c r="N3" s="9">
-        <v>0</v>
-      </c>
-      <c r="O3" s="10" t="s">
+      <c r="P3" s="9">
+        <v>0</v>
+      </c>
+      <c r="Q3" s="10" t="s">
         <v>112</v>
       </c>
-      <c r="P3" s="13" t="s">
+      <c r="R3" s="13" t="s">
         <v>122</v>
       </c>
-      <c r="Q3" s="5">
-        <v>0</v>
-      </c>
-      <c r="R3" s="14" t="s">
-        <v>108</v>
-      </c>
-      <c r="S3" s="5"/>
-    </row>
-    <row r="4" spans="1:20" ht="17">
+      <c r="S3" s="5">
+        <v>0</v>
+      </c>
+      <c r="T3" s="14" t="s">
+        <v>108</v>
+      </c>
+      <c r="U3" s="5"/>
+    </row>
+    <row r="4" spans="1:22" ht="17">
       <c r="A4" s="8">
         <v>3</v>
       </c>
@@ -1515,44 +1726,50 @@
         <v>184</v>
       </c>
       <c r="G4" s="6" t="s">
+        <v>283</v>
+      </c>
+      <c r="H4" s="6" t="s">
         <v>179</v>
-      </c>
-      <c r="H4" s="6" t="s">
-        <v>104</v>
       </c>
       <c r="I4" s="6" t="s">
         <v>104</v>
       </c>
-      <c r="J4" s="6">
-        <v>0</v>
-      </c>
-      <c r="K4" s="6" t="s">
+      <c r="J4" s="6" t="s">
+        <v>104</v>
+      </c>
+      <c r="K4" s="6">
+        <v>0</v>
+      </c>
+      <c r="L4" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="L4" s="7" t="s">
+      <c r="M4" s="6" t="s">
+        <v>226</v>
+      </c>
+      <c r="N4" s="7" t="s">
         <v>189</v>
       </c>
-      <c r="M4" s="8" t="s">
+      <c r="O4" s="8" t="s">
         <v>98</v>
       </c>
-      <c r="N4" s="9">
-        <v>0</v>
-      </c>
-      <c r="O4" s="10" t="s">
+      <c r="P4" s="9">
+        <v>0</v>
+      </c>
+      <c r="Q4" s="10" t="s">
         <v>112</v>
       </c>
-      <c r="P4" s="13" t="s">
+      <c r="R4" s="13" t="s">
         <v>122</v>
       </c>
-      <c r="Q4" s="5">
-        <v>0</v>
-      </c>
-      <c r="R4" s="14" t="s">
-        <v>108</v>
-      </c>
-      <c r="S4" s="5"/>
-    </row>
-    <row r="5" spans="1:20" ht="17">
+      <c r="S4" s="5">
+        <v>0</v>
+      </c>
+      <c r="T4" s="14" t="s">
+        <v>108</v>
+      </c>
+      <c r="U4" s="5"/>
+    </row>
+    <row r="5" spans="1:22" ht="17">
       <c r="A5" s="8">
         <v>4</v>
       </c>
@@ -1572,7 +1789,7 @@
         <v>185</v>
       </c>
       <c r="G5" s="6" t="s">
-        <v>106</v>
+        <v>185</v>
       </c>
       <c r="H5" s="6" t="s">
         <v>106</v>
@@ -1580,36 +1797,42 @@
       <c r="I5" s="6" t="s">
         <v>106</v>
       </c>
-      <c r="J5" s="6">
-        <v>1</v>
-      </c>
-      <c r="K5" s="6" t="s">
+      <c r="J5" s="6" t="s">
+        <v>106</v>
+      </c>
+      <c r="K5" s="6">
+        <v>1</v>
+      </c>
+      <c r="L5" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="L5" s="7" t="s">
+      <c r="M5" s="6" t="s">
+        <v>227</v>
+      </c>
+      <c r="N5" s="7" t="s">
         <v>154</v>
       </c>
-      <c r="M5" s="8" t="s">
+      <c r="O5" s="8" t="s">
         <v>98</v>
       </c>
-      <c r="N5" s="9">
+      <c r="P5" s="9">
         <v>2</v>
       </c>
-      <c r="O5" s="10" t="s">
+      <c r="Q5" s="10" t="s">
         <v>116</v>
       </c>
-      <c r="P5" s="15" t="s">
+      <c r="R5" s="15" t="s">
         <v>175</v>
       </c>
-      <c r="Q5" s="5">
+      <c r="S5" s="5">
         <v>14</v>
       </c>
-      <c r="R5" s="14" t="s">
-        <v>108</v>
-      </c>
-      <c r="S5" s="5"/>
-    </row>
-    <row r="6" spans="1:20" ht="17">
+      <c r="T5" s="14" t="s">
+        <v>108</v>
+      </c>
+      <c r="U5" s="5"/>
+    </row>
+    <row r="6" spans="1:22" ht="17">
       <c r="A6" s="8">
         <v>5</v>
       </c>
@@ -1629,7 +1852,7 @@
         <v>185</v>
       </c>
       <c r="G6" s="6" t="s">
-        <v>106</v>
+        <v>185</v>
       </c>
       <c r="H6" s="6" t="s">
         <v>106</v>
@@ -1637,36 +1860,42 @@
       <c r="I6" s="6" t="s">
         <v>106</v>
       </c>
-      <c r="J6" s="6">
-        <v>1</v>
-      </c>
-      <c r="K6" s="6" t="s">
+      <c r="J6" s="6" t="s">
+        <v>106</v>
+      </c>
+      <c r="K6" s="6">
+        <v>1</v>
+      </c>
+      <c r="L6" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="L6" s="7" t="s">
+      <c r="M6" s="6" t="s">
+        <v>228</v>
+      </c>
+      <c r="N6" s="7" t="s">
         <v>155</v>
       </c>
-      <c r="M6" s="8" t="s">
+      <c r="O6" s="8" t="s">
         <v>98</v>
       </c>
-      <c r="N6" s="9">
+      <c r="P6" s="9">
         <v>2</v>
       </c>
-      <c r="O6" s="10" t="s">
+      <c r="Q6" s="10" t="s">
         <v>116</v>
       </c>
-      <c r="P6" s="15" t="s">
+      <c r="R6" s="15" t="s">
         <v>175</v>
       </c>
-      <c r="Q6" s="5">
+      <c r="S6" s="5">
         <v>16</v>
       </c>
-      <c r="R6" s="14" t="s">
-        <v>108</v>
-      </c>
-      <c r="S6" s="5"/>
-    </row>
-    <row r="7" spans="1:20" s="37" customFormat="1" ht="17">
+      <c r="T6" s="14" t="s">
+        <v>108</v>
+      </c>
+      <c r="U6" s="5"/>
+    </row>
+    <row r="7" spans="1:22" s="37" customFormat="1" ht="17">
       <c r="A7" s="8">
         <v>57</v>
       </c>
@@ -1686,45 +1915,51 @@
         <v>187</v>
       </c>
       <c r="G7" s="6" t="s">
+        <v>187</v>
+      </c>
+      <c r="H7" s="6" t="s">
         <v>183</v>
-      </c>
-      <c r="H7" s="6" t="s">
-        <v>104</v>
       </c>
       <c r="I7" s="6" t="s">
         <v>104</v>
       </c>
-      <c r="J7" s="6">
-        <v>1</v>
-      </c>
-      <c r="K7" s="6" t="s">
+      <c r="J7" s="6" t="s">
+        <v>104</v>
+      </c>
+      <c r="K7" s="6">
+        <v>1</v>
+      </c>
+      <c r="L7" s="6" t="s">
         <v>119</v>
       </c>
-      <c r="L7" s="35" t="s">
+      <c r="M7" s="6" t="s">
+        <v>229</v>
+      </c>
+      <c r="N7" s="35" t="s">
         <v>192</v>
       </c>
-      <c r="M7" s="8" t="s">
+      <c r="O7" s="8" t="s">
         <v>98</v>
       </c>
-      <c r="N7" s="18">
+      <c r="P7" s="18">
         <v>2</v>
       </c>
-      <c r="O7" s="19" t="s">
+      <c r="Q7" s="19" t="s">
         <v>111</v>
       </c>
-      <c r="P7" s="15" t="s">
+      <c r="R7" s="15" t="s">
         <v>175</v>
       </c>
-      <c r="Q7" s="6">
+      <c r="S7" s="6">
         <v>17</v>
       </c>
-      <c r="R7" s="14" t="s">
-        <v>108</v>
-      </c>
-      <c r="S7" s="16"/>
-      <c r="T7" s="36"/>
-    </row>
-    <row r="8" spans="1:20" ht="17">
+      <c r="T7" s="14" t="s">
+        <v>108</v>
+      </c>
+      <c r="U7" s="16"/>
+      <c r="V7" s="36"/>
+    </row>
+    <row r="8" spans="1:22" ht="17">
       <c r="A8" s="8">
         <v>6</v>
       </c>
@@ -1744,44 +1979,50 @@
         <v>203</v>
       </c>
       <c r="G8" s="6" t="s">
+        <v>203</v>
+      </c>
+      <c r="H8" s="6" t="s">
         <v>180</v>
       </c>
-      <c r="H8" s="6" t="s">
-        <v>105</v>
-      </c>
       <c r="I8" s="6" t="s">
         <v>105</v>
       </c>
-      <c r="J8" s="6">
-        <v>1</v>
-      </c>
-      <c r="K8" s="6" t="s">
+      <c r="J8" s="6" t="s">
+        <v>105</v>
+      </c>
+      <c r="K8" s="6">
+        <v>1</v>
+      </c>
+      <c r="L8" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="L8" s="7" t="s">
+      <c r="M8" s="6" t="s">
+        <v>230</v>
+      </c>
+      <c r="N8" s="7" t="s">
         <v>124</v>
       </c>
-      <c r="M8" s="8" t="s">
+      <c r="O8" s="8" t="s">
         <v>98</v>
       </c>
-      <c r="N8" s="9">
-        <v>0</v>
-      </c>
-      <c r="O8" s="10" t="s">
+      <c r="P8" s="9">
+        <v>0</v>
+      </c>
+      <c r="Q8" s="10" t="s">
         <v>109</v>
       </c>
-      <c r="P8" s="6" t="s">
+      <c r="R8" s="6" t="s">
         <v>172</v>
       </c>
-      <c r="Q8" s="5">
+      <c r="S8" s="5">
         <v>13</v>
       </c>
-      <c r="R8" s="14" t="s">
-        <v>108</v>
-      </c>
-      <c r="S8" s="5"/>
-    </row>
-    <row r="9" spans="1:20" ht="17">
+      <c r="T8" s="14" t="s">
+        <v>108</v>
+      </c>
+      <c r="U8" s="5"/>
+    </row>
+    <row r="9" spans="1:22" ht="17">
       <c r="A9" s="8">
         <v>7</v>
       </c>
@@ -1801,44 +2042,50 @@
         <v>203</v>
       </c>
       <c r="G9" s="6" t="s">
+        <v>203</v>
+      </c>
+      <c r="H9" s="6" t="s">
         <v>180</v>
       </c>
-      <c r="H9" s="6" t="s">
-        <v>105</v>
-      </c>
       <c r="I9" s="6" t="s">
         <v>105</v>
       </c>
-      <c r="J9" s="6">
-        <v>1</v>
-      </c>
-      <c r="K9" s="6" t="s">
+      <c r="J9" s="6" t="s">
+        <v>105</v>
+      </c>
+      <c r="K9" s="6">
+        <v>1</v>
+      </c>
+      <c r="L9" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="L9" s="7" t="s">
+      <c r="M9" s="6" t="s">
+        <v>231</v>
+      </c>
+      <c r="N9" s="7" t="s">
         <v>125</v>
       </c>
-      <c r="M9" s="8" t="s">
+      <c r="O9" s="8" t="s">
         <v>98</v>
       </c>
-      <c r="N9" s="9">
-        <v>0</v>
-      </c>
-      <c r="O9" s="10" t="s">
+      <c r="P9" s="9">
+        <v>0</v>
+      </c>
+      <c r="Q9" s="10" t="s">
         <v>109</v>
       </c>
-      <c r="P9" s="15" t="s">
+      <c r="R9" s="15" t="s">
         <v>175</v>
       </c>
-      <c r="Q9" s="5">
+      <c r="S9" s="5">
         <v>18</v>
       </c>
-      <c r="R9" s="14" t="s">
-        <v>108</v>
-      </c>
-      <c r="S9" s="5"/>
-    </row>
-    <row r="10" spans="1:20" ht="17">
+      <c r="T9" s="14" t="s">
+        <v>108</v>
+      </c>
+      <c r="U9" s="5"/>
+    </row>
+    <row r="10" spans="1:22" ht="17">
       <c r="A10" s="8">
         <v>8</v>
       </c>
@@ -1858,7 +2105,7 @@
         <v>185</v>
       </c>
       <c r="G10" s="6" t="s">
-        <v>106</v>
+        <v>185</v>
       </c>
       <c r="H10" s="6" t="s">
         <v>106</v>
@@ -1866,36 +2113,42 @@
       <c r="I10" s="6" t="s">
         <v>106</v>
       </c>
-      <c r="J10" s="6">
-        <v>1</v>
-      </c>
-      <c r="K10" s="6" t="s">
+      <c r="J10" s="6" t="s">
+        <v>106</v>
+      </c>
+      <c r="K10" s="6">
+        <v>1</v>
+      </c>
+      <c r="L10" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="L10" s="7" t="s">
+      <c r="M10" s="6" t="s">
+        <v>232</v>
+      </c>
+      <c r="N10" s="7" t="s">
         <v>152</v>
       </c>
-      <c r="M10" s="8" t="s">
+      <c r="O10" s="8" t="s">
         <v>98</v>
       </c>
-      <c r="N10" s="9">
+      <c r="P10" s="9">
         <v>2</v>
       </c>
-      <c r="O10" s="10" t="s">
+      <c r="Q10" s="10" t="s">
         <v>116</v>
       </c>
-      <c r="P10" s="15" t="s">
+      <c r="R10" s="15" t="s">
         <v>175</v>
       </c>
-      <c r="Q10" s="5">
+      <c r="S10" s="5">
         <v>19</v>
       </c>
-      <c r="R10" s="14" t="s">
-        <v>108</v>
-      </c>
-      <c r="S10" s="5"/>
-    </row>
-    <row r="11" spans="1:20" s="3" customFormat="1" ht="19" customHeight="1">
+      <c r="T10" s="14" t="s">
+        <v>108</v>
+      </c>
+      <c r="U10" s="5"/>
+    </row>
+    <row r="11" spans="1:22" s="3" customFormat="1" ht="19" customHeight="1">
       <c r="A11" s="8">
         <v>9</v>
       </c>
@@ -1915,45 +2168,51 @@
         <v>203</v>
       </c>
       <c r="G11" s="6" t="s">
+        <v>203</v>
+      </c>
+      <c r="H11" s="6" t="s">
         <v>180</v>
       </c>
-      <c r="H11" s="6" t="s">
-        <v>105</v>
-      </c>
       <c r="I11" s="6" t="s">
         <v>105</v>
       </c>
-      <c r="J11" s="6">
-        <v>1</v>
-      </c>
-      <c r="K11" s="6" t="s">
+      <c r="J11" s="6" t="s">
+        <v>105</v>
+      </c>
+      <c r="K11" s="6">
+        <v>1</v>
+      </c>
+      <c r="L11" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="L11" s="17" t="s">
+      <c r="M11" s="6" t="s">
+        <v>233</v>
+      </c>
+      <c r="N11" s="17" t="s">
         <v>191</v>
       </c>
-      <c r="M11" s="8" t="s">
+      <c r="O11" s="8" t="s">
         <v>98</v>
       </c>
-      <c r="N11" s="18">
-        <v>0</v>
-      </c>
-      <c r="O11" s="19" t="s">
+      <c r="P11" s="18">
+        <v>0</v>
+      </c>
+      <c r="Q11" s="19" t="s">
         <v>109</v>
       </c>
-      <c r="P11" s="6" t="s">
+      <c r="R11" s="6" t="s">
         <v>172</v>
       </c>
-      <c r="Q11" s="16">
+      <c r="S11" s="16">
         <v>15</v>
       </c>
-      <c r="R11" s="14" t="s">
-        <v>108</v>
-      </c>
-      <c r="S11" s="16"/>
-      <c r="T11"/>
-    </row>
-    <row r="12" spans="1:20" ht="17">
+      <c r="T11" s="14" t="s">
+        <v>108</v>
+      </c>
+      <c r="U11" s="16"/>
+      <c r="V11"/>
+    </row>
+    <row r="12" spans="1:22" ht="17">
       <c r="A12" s="20">
         <v>10</v>
       </c>
@@ -1973,44 +2232,50 @@
         <v>203</v>
       </c>
       <c r="G12" s="21" t="s">
+        <v>203</v>
+      </c>
+      <c r="H12" s="21" t="s">
         <v>180</v>
       </c>
-      <c r="H12" s="21" t="s">
-        <v>105</v>
-      </c>
       <c r="I12" s="21" t="s">
         <v>105</v>
       </c>
-      <c r="J12" s="34">
-        <v>1</v>
-      </c>
-      <c r="K12" s="21" t="s">
+      <c r="J12" s="21" t="s">
+        <v>105</v>
+      </c>
+      <c r="K12" s="34">
+        <v>1</v>
+      </c>
+      <c r="L12" s="21" t="s">
         <v>19</v>
       </c>
-      <c r="L12" s="22" t="s">
+      <c r="M12" s="21" t="s">
+        <v>234</v>
+      </c>
+      <c r="N12" s="22" t="s">
         <v>126</v>
       </c>
-      <c r="M12" s="20" t="s">
+      <c r="O12" s="20" t="s">
         <v>99</v>
       </c>
-      <c r="N12" s="23">
-        <v>0</v>
-      </c>
-      <c r="O12" s="24" t="s">
+      <c r="P12" s="23">
+        <v>0</v>
+      </c>
+      <c r="Q12" s="24" t="s">
         <v>109</v>
       </c>
-      <c r="P12" s="25" t="s">
+      <c r="R12" s="25" t="s">
         <v>176</v>
       </c>
-      <c r="Q12" s="26">
+      <c r="S12" s="26">
         <v>23</v>
       </c>
-      <c r="R12" s="27" t="s">
-        <v>108</v>
-      </c>
-      <c r="S12" s="13"/>
-    </row>
-    <row r="13" spans="1:20" ht="17">
+      <c r="T12" s="27" t="s">
+        <v>108</v>
+      </c>
+      <c r="U12" s="13"/>
+    </row>
+    <row r="13" spans="1:22" ht="17">
       <c r="A13" s="20">
         <v>11</v>
       </c>
@@ -2030,46 +2295,52 @@
         <v>186</v>
       </c>
       <c r="G13" s="21" t="s">
+        <v>284</v>
+      </c>
+      <c r="H13" s="21" t="s">
         <v>182</v>
       </c>
-      <c r="H13" s="33" t="s">
-        <v>105</v>
-      </c>
       <c r="I13" s="33" t="s">
-        <v>106</v>
-      </c>
-      <c r="J13" s="34">
-        <v>1</v>
-      </c>
-      <c r="K13" s="21" t="s">
+        <v>105</v>
+      </c>
+      <c r="J13" s="33" t="s">
+        <v>106</v>
+      </c>
+      <c r="K13" s="34">
+        <v>1</v>
+      </c>
+      <c r="L13" s="21" t="s">
         <v>21</v>
       </c>
-      <c r="L13" s="22" t="s">
+      <c r="M13" s="21" t="s">
+        <v>235</v>
+      </c>
+      <c r="N13" s="22" t="s">
         <v>149</v>
       </c>
-      <c r="M13" s="20" t="s">
+      <c r="O13" s="20" t="s">
         <v>99</v>
       </c>
-      <c r="N13" s="23">
-        <v>0</v>
-      </c>
-      <c r="O13" s="28" t="s">
+      <c r="P13" s="23">
+        <v>0</v>
+      </c>
+      <c r="Q13" s="28" t="s">
         <v>204</v>
       </c>
-      <c r="P13" s="25" t="s">
+      <c r="R13" s="25" t="s">
         <v>176</v>
       </c>
-      <c r="Q13" s="26">
+      <c r="S13" s="26">
         <v>24</v>
       </c>
-      <c r="R13" s="27" t="s">
-        <v>108</v>
-      </c>
-      <c r="S13" s="13" t="s">
+      <c r="T13" s="27" t="s">
+        <v>108</v>
+      </c>
+      <c r="U13" s="13" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="14" spans="1:20" ht="17">
+    <row r="14" spans="1:22" ht="17">
       <c r="A14" s="20">
         <v>12</v>
       </c>
@@ -2089,44 +2360,50 @@
         <v>203</v>
       </c>
       <c r="G14" s="21" t="s">
+        <v>203</v>
+      </c>
+      <c r="H14" s="21" t="s">
         <v>180</v>
       </c>
-      <c r="H14" s="21" t="s">
-        <v>105</v>
-      </c>
       <c r="I14" s="21" t="s">
         <v>105</v>
       </c>
-      <c r="J14" s="34">
-        <v>1</v>
-      </c>
-      <c r="K14" s="21" t="s">
+      <c r="J14" s="21" t="s">
+        <v>105</v>
+      </c>
+      <c r="K14" s="34">
+        <v>1</v>
+      </c>
+      <c r="L14" s="21" t="s">
         <v>23</v>
       </c>
-      <c r="L14" s="22" t="s">
+      <c r="M14" s="21" t="s">
+        <v>236</v>
+      </c>
+      <c r="N14" s="22" t="s">
         <v>127</v>
       </c>
-      <c r="M14" s="20" t="s">
+      <c r="O14" s="20" t="s">
         <v>99</v>
       </c>
-      <c r="N14" s="23">
-        <v>0</v>
-      </c>
-      <c r="O14" s="28" t="s">
+      <c r="P14" s="23">
+        <v>0</v>
+      </c>
+      <c r="Q14" s="28" t="s">
         <v>109</v>
       </c>
-      <c r="P14" s="29" t="s">
+      <c r="R14" s="29" t="s">
         <v>123</v>
       </c>
-      <c r="Q14" s="26">
+      <c r="S14" s="26">
         <v>21</v>
       </c>
-      <c r="R14" s="27" t="s">
-        <v>108</v>
-      </c>
-      <c r="S14" s="13"/>
-    </row>
-    <row r="15" spans="1:20" ht="17">
+      <c r="T14" s="27" t="s">
+        <v>108</v>
+      </c>
+      <c r="U14" s="13"/>
+    </row>
+    <row r="15" spans="1:22" ht="17">
       <c r="A15" s="20">
         <v>13</v>
       </c>
@@ -2146,46 +2423,52 @@
         <v>186</v>
       </c>
       <c r="G15" s="21" t="s">
+        <v>284</v>
+      </c>
+      <c r="H15" s="21" t="s">
         <v>182</v>
       </c>
-      <c r="H15" s="33" t="s">
-        <v>105</v>
-      </c>
       <c r="I15" s="33" t="s">
-        <v>106</v>
-      </c>
-      <c r="J15" s="34">
-        <v>1</v>
-      </c>
-      <c r="K15" s="21" t="s">
+        <v>105</v>
+      </c>
+      <c r="J15" s="33" t="s">
+        <v>106</v>
+      </c>
+      <c r="K15" s="34">
+        <v>1</v>
+      </c>
+      <c r="L15" s="21" t="s">
         <v>25</v>
       </c>
-      <c r="L15" s="22" t="s">
+      <c r="M15" s="21" t="s">
+        <v>237</v>
+      </c>
+      <c r="N15" s="22" t="s">
         <v>150</v>
       </c>
-      <c r="M15" s="20" t="s">
+      <c r="O15" s="20" t="s">
         <v>99</v>
       </c>
-      <c r="N15" s="23">
-        <v>1</v>
-      </c>
-      <c r="O15" s="28" t="s">
+      <c r="P15" s="23">
+        <v>1</v>
+      </c>
+      <c r="Q15" s="28" t="s">
         <v>204</v>
       </c>
-      <c r="P15" s="30" t="s">
+      <c r="R15" s="30" t="s">
         <v>123</v>
       </c>
-      <c r="Q15" s="26">
+      <c r="S15" s="26">
         <v>22</v>
       </c>
-      <c r="R15" s="27" t="s">
-        <v>108</v>
-      </c>
-      <c r="S15" s="13" t="s">
+      <c r="T15" s="27" t="s">
+        <v>108</v>
+      </c>
+      <c r="U15" s="13" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="16" spans="1:20" ht="17">
+    <row r="16" spans="1:22" ht="17">
       <c r="A16" s="20">
         <v>14</v>
       </c>
@@ -2205,44 +2488,50 @@
         <v>203</v>
       </c>
       <c r="G16" s="21" t="s">
+        <v>203</v>
+      </c>
+      <c r="H16" s="21" t="s">
         <v>180</v>
       </c>
-      <c r="H16" s="21" t="s">
-        <v>105</v>
-      </c>
       <c r="I16" s="21" t="s">
         <v>105</v>
       </c>
-      <c r="J16" s="34">
-        <v>1</v>
-      </c>
-      <c r="K16" s="21" t="s">
+      <c r="J16" s="21" t="s">
+        <v>105</v>
+      </c>
+      <c r="K16" s="34">
+        <v>1</v>
+      </c>
+      <c r="L16" s="21" t="s">
         <v>27</v>
       </c>
-      <c r="L16" s="22" t="s">
+      <c r="M16" s="21" t="s">
+        <v>238</v>
+      </c>
+      <c r="N16" s="22" t="s">
         <v>128</v>
       </c>
-      <c r="M16" s="20" t="s">
+      <c r="O16" s="20" t="s">
         <v>99</v>
       </c>
-      <c r="N16" s="23">
-        <v>0</v>
-      </c>
-      <c r="O16" s="28" t="s">
+      <c r="P16" s="23">
+        <v>0</v>
+      </c>
+      <c r="Q16" s="28" t="s">
         <v>109</v>
       </c>
-      <c r="P16" s="25" t="s">
+      <c r="R16" s="25" t="s">
         <v>176</v>
       </c>
-      <c r="Q16" s="26">
+      <c r="S16" s="26">
         <v>27</v>
       </c>
-      <c r="R16" s="27" t="s">
-        <v>108</v>
-      </c>
-      <c r="S16" s="13"/>
-    </row>
-    <row r="17" spans="1:19" ht="17">
+      <c r="T16" s="27" t="s">
+        <v>108</v>
+      </c>
+      <c r="U16" s="13"/>
+    </row>
+    <row r="17" spans="1:21" ht="17">
       <c r="A17" s="20">
         <v>15</v>
       </c>
@@ -2262,7 +2551,7 @@
         <v>185</v>
       </c>
       <c r="G17" s="21" t="s">
-        <v>106</v>
+        <v>185</v>
       </c>
       <c r="H17" s="21" t="s">
         <v>106</v>
@@ -2270,36 +2559,42 @@
       <c r="I17" s="21" t="s">
         <v>106</v>
       </c>
-      <c r="J17" s="34">
-        <v>1</v>
-      </c>
-      <c r="K17" s="21" t="s">
+      <c r="J17" s="21" t="s">
+        <v>106</v>
+      </c>
+      <c r="K17" s="34">
+        <v>1</v>
+      </c>
+      <c r="L17" s="21" t="s">
         <v>28</v>
       </c>
-      <c r="L17" s="22" t="s">
+      <c r="M17" s="21" t="s">
+        <v>239</v>
+      </c>
+      <c r="N17" s="22" t="s">
         <v>144</v>
       </c>
-      <c r="M17" s="20" t="s">
+      <c r="O17" s="20" t="s">
         <v>99</v>
       </c>
-      <c r="N17" s="23">
-        <v>0</v>
-      </c>
-      <c r="O17" s="28" t="s">
+      <c r="P17" s="23">
+        <v>0</v>
+      </c>
+      <c r="Q17" s="28" t="s">
         <v>116</v>
       </c>
-      <c r="P17" s="25" t="s">
+      <c r="R17" s="25" t="s">
         <v>176</v>
       </c>
-      <c r="Q17" s="26">
+      <c r="S17" s="26">
         <v>28</v>
       </c>
-      <c r="R17" s="27" t="s">
-        <v>108</v>
-      </c>
-      <c r="S17" s="13"/>
-    </row>
-    <row r="18" spans="1:19" ht="17">
+      <c r="T17" s="27" t="s">
+        <v>108</v>
+      </c>
+      <c r="U17" s="13"/>
+    </row>
+    <row r="18" spans="1:21" ht="17">
       <c r="A18" s="20">
         <v>16</v>
       </c>
@@ -2319,7 +2614,7 @@
         <v>185</v>
       </c>
       <c r="G18" s="21" t="s">
-        <v>106</v>
+        <v>185</v>
       </c>
       <c r="H18" s="21" t="s">
         <v>106</v>
@@ -2327,36 +2622,42 @@
       <c r="I18" s="21" t="s">
         <v>106</v>
       </c>
-      <c r="J18" s="34">
-        <v>1</v>
-      </c>
-      <c r="K18" s="21" t="s">
+      <c r="J18" s="21" t="s">
+        <v>106</v>
+      </c>
+      <c r="K18" s="34">
+        <v>1</v>
+      </c>
+      <c r="L18" s="21" t="s">
         <v>29</v>
       </c>
-      <c r="L18" s="22" t="s">
+      <c r="M18" s="21" t="s">
+        <v>240</v>
+      </c>
+      <c r="N18" s="22" t="s">
         <v>145</v>
       </c>
-      <c r="M18" s="20" t="s">
+      <c r="O18" s="20" t="s">
         <v>99</v>
       </c>
-      <c r="N18" s="23">
-        <v>0</v>
-      </c>
-      <c r="O18" s="28" t="s">
+      <c r="P18" s="23">
+        <v>0</v>
+      </c>
+      <c r="Q18" s="28" t="s">
         <v>116</v>
       </c>
-      <c r="P18" s="25" t="s">
+      <c r="R18" s="25" t="s">
         <v>176</v>
       </c>
-      <c r="Q18" s="26">
-        <v>0</v>
-      </c>
-      <c r="R18" s="27" t="s">
-        <v>108</v>
-      </c>
-      <c r="S18" s="13"/>
-    </row>
-    <row r="19" spans="1:19" ht="17">
+      <c r="S18" s="26">
+        <v>0</v>
+      </c>
+      <c r="T18" s="27" t="s">
+        <v>108</v>
+      </c>
+      <c r="U18" s="13"/>
+    </row>
+    <row r="19" spans="1:21" ht="17">
       <c r="A19" s="20">
         <v>17</v>
       </c>
@@ -2376,44 +2677,50 @@
         <v>203</v>
       </c>
       <c r="G19" s="21" t="s">
+        <v>203</v>
+      </c>
+      <c r="H19" s="21" t="s">
         <v>180</v>
       </c>
-      <c r="H19" s="21" t="s">
-        <v>105</v>
-      </c>
       <c r="I19" s="21" t="s">
         <v>105</v>
       </c>
-      <c r="J19" s="34">
-        <v>1</v>
-      </c>
-      <c r="K19" s="21" t="s">
+      <c r="J19" s="21" t="s">
+        <v>105</v>
+      </c>
+      <c r="K19" s="34">
+        <v>1</v>
+      </c>
+      <c r="L19" s="21" t="s">
         <v>31</v>
       </c>
-      <c r="L19" s="22" t="s">
+      <c r="M19" s="21" t="s">
+        <v>241</v>
+      </c>
+      <c r="N19" s="22" t="s">
         <v>129</v>
       </c>
-      <c r="M19" s="20" t="s">
+      <c r="O19" s="20" t="s">
         <v>99</v>
       </c>
-      <c r="N19" s="23">
-        <v>0</v>
-      </c>
-      <c r="O19" s="28" t="s">
+      <c r="P19" s="23">
+        <v>0</v>
+      </c>
+      <c r="Q19" s="28" t="s">
         <v>109</v>
       </c>
-      <c r="P19" s="29" t="s">
+      <c r="R19" s="29" t="s">
         <v>123</v>
       </c>
-      <c r="Q19" s="26">
+      <c r="S19" s="26">
         <v>25</v>
       </c>
-      <c r="R19" s="27" t="s">
-        <v>108</v>
-      </c>
-      <c r="S19" s="13"/>
-    </row>
-    <row r="20" spans="1:19" ht="17">
+      <c r="T19" s="27" t="s">
+        <v>108</v>
+      </c>
+      <c r="U19" s="13"/>
+    </row>
+    <row r="20" spans="1:21" ht="17">
       <c r="A20" s="20">
         <v>18</v>
       </c>
@@ -2433,7 +2740,7 @@
         <v>185</v>
       </c>
       <c r="G20" s="21" t="s">
-        <v>106</v>
+        <v>185</v>
       </c>
       <c r="H20" s="21" t="s">
         <v>106</v>
@@ -2441,36 +2748,42 @@
       <c r="I20" s="21" t="s">
         <v>106</v>
       </c>
-      <c r="J20" s="34">
-        <v>1</v>
-      </c>
-      <c r="K20" s="21" t="s">
+      <c r="J20" s="21" t="s">
+        <v>106</v>
+      </c>
+      <c r="K20" s="34">
+        <v>1</v>
+      </c>
+      <c r="L20" s="21" t="s">
         <v>32</v>
       </c>
-      <c r="L20" s="22" t="s">
+      <c r="M20" s="21" t="s">
+        <v>242</v>
+      </c>
+      <c r="N20" s="22" t="s">
         <v>151</v>
       </c>
-      <c r="M20" s="20" t="s">
+      <c r="O20" s="20" t="s">
         <v>99</v>
       </c>
-      <c r="N20" s="23">
-        <v>1</v>
-      </c>
-      <c r="O20" s="28" t="s">
+      <c r="P20" s="23">
+        <v>1</v>
+      </c>
+      <c r="Q20" s="28" t="s">
         <v>116</v>
       </c>
-      <c r="P20" s="30" t="s">
+      <c r="R20" s="30" t="s">
         <v>123</v>
       </c>
-      <c r="Q20" s="26">
+      <c r="S20" s="26">
         <v>26</v>
       </c>
-      <c r="R20" s="27" t="s">
-        <v>108</v>
-      </c>
-      <c r="S20" s="13"/>
-    </row>
-    <row r="21" spans="1:19" ht="17">
+      <c r="T20" s="27" t="s">
+        <v>108</v>
+      </c>
+      <c r="U20" s="13"/>
+    </row>
+    <row r="21" spans="1:21" ht="17">
       <c r="A21" s="20">
         <v>19</v>
       </c>
@@ -2490,7 +2803,7 @@
         <v>185</v>
       </c>
       <c r="G21" s="21" t="s">
-        <v>106</v>
+        <v>185</v>
       </c>
       <c r="H21" s="21" t="s">
         <v>106</v>
@@ -2498,36 +2811,42 @@
       <c r="I21" s="21" t="s">
         <v>106</v>
       </c>
-      <c r="J21" s="34">
-        <v>1</v>
-      </c>
-      <c r="K21" s="21" t="s">
+      <c r="J21" s="21" t="s">
+        <v>106</v>
+      </c>
+      <c r="K21" s="34">
+        <v>1</v>
+      </c>
+      <c r="L21" s="21" t="s">
         <v>33</v>
       </c>
-      <c r="L21" s="22" t="s">
+      <c r="M21" s="21" t="s">
+        <v>243</v>
+      </c>
+      <c r="N21" s="22" t="s">
         <v>146</v>
       </c>
-      <c r="M21" s="20" t="s">
+      <c r="O21" s="20" t="s">
         <v>99</v>
       </c>
-      <c r="N21" s="23">
-        <v>1</v>
-      </c>
-      <c r="O21" s="28" t="s">
+      <c r="P21" s="23">
+        <v>1</v>
+      </c>
+      <c r="Q21" s="28" t="s">
         <v>116</v>
       </c>
-      <c r="P21" s="30" t="s">
+      <c r="R21" s="30" t="s">
         <v>123</v>
       </c>
-      <c r="Q21" s="26">
-        <v>0</v>
-      </c>
-      <c r="R21" s="27" t="s">
-        <v>108</v>
-      </c>
-      <c r="S21" s="13"/>
-    </row>
-    <row r="22" spans="1:19" ht="17">
+      <c r="S21" s="26">
+        <v>0</v>
+      </c>
+      <c r="T21" s="27" t="s">
+        <v>108</v>
+      </c>
+      <c r="U21" s="13"/>
+    </row>
+    <row r="22" spans="1:21" ht="17">
       <c r="A22" s="20">
         <v>20</v>
       </c>
@@ -2547,44 +2866,50 @@
         <v>203</v>
       </c>
       <c r="G22" s="21" t="s">
+        <v>203</v>
+      </c>
+      <c r="H22" s="21" t="s">
         <v>180</v>
       </c>
-      <c r="H22" s="21" t="s">
-        <v>105</v>
-      </c>
       <c r="I22" s="21" t="s">
         <v>105</v>
       </c>
-      <c r="J22" s="34">
-        <v>1</v>
-      </c>
-      <c r="K22" s="21" t="s">
+      <c r="J22" s="21" t="s">
+        <v>105</v>
+      </c>
+      <c r="K22" s="34">
+        <v>1</v>
+      </c>
+      <c r="L22" s="21" t="s">
         <v>35</v>
       </c>
-      <c r="L22" s="22" t="s">
+      <c r="M22" s="21" t="s">
+        <v>244</v>
+      </c>
+      <c r="N22" s="22" t="s">
         <v>130</v>
       </c>
-      <c r="M22" s="20" t="s">
+      <c r="O22" s="20" t="s">
         <v>99</v>
       </c>
-      <c r="N22" s="23">
-        <v>0</v>
-      </c>
-      <c r="O22" s="28" t="s">
+      <c r="P22" s="23">
+        <v>0</v>
+      </c>
+      <c r="Q22" s="28" t="s">
         <v>109</v>
       </c>
-      <c r="P22" s="25" t="s">
+      <c r="R22" s="25" t="s">
         <v>176</v>
       </c>
-      <c r="Q22" s="26">
+      <c r="S22" s="26">
         <v>31</v>
       </c>
-      <c r="R22" s="27" t="s">
-        <v>108</v>
-      </c>
-      <c r="S22" s="13"/>
-    </row>
-    <row r="23" spans="1:19" ht="17">
+      <c r="T22" s="27" t="s">
+        <v>108</v>
+      </c>
+      <c r="U22" s="13"/>
+    </row>
+    <row r="23" spans="1:21" ht="17">
       <c r="A23" s="20">
         <v>21</v>
       </c>
@@ -2604,7 +2929,7 @@
         <v>185</v>
       </c>
       <c r="G23" s="21" t="s">
-        <v>106</v>
+        <v>185</v>
       </c>
       <c r="H23" s="21" t="s">
         <v>106</v>
@@ -2612,36 +2937,42 @@
       <c r="I23" s="21" t="s">
         <v>106</v>
       </c>
-      <c r="J23" s="34">
-        <v>1</v>
-      </c>
-      <c r="K23" s="21" t="s">
+      <c r="J23" s="21" t="s">
+        <v>106</v>
+      </c>
+      <c r="K23" s="34">
+        <v>1</v>
+      </c>
+      <c r="L23" s="21" t="s">
         <v>36</v>
       </c>
-      <c r="L23" s="22" t="s">
+      <c r="M23" s="21" t="s">
+        <v>245</v>
+      </c>
+      <c r="N23" s="22" t="s">
         <v>147</v>
       </c>
-      <c r="M23" s="20" t="s">
+      <c r="O23" s="20" t="s">
         <v>99</v>
       </c>
-      <c r="N23" s="23">
-        <v>0</v>
-      </c>
-      <c r="O23" s="28" t="s">
+      <c r="P23" s="23">
+        <v>0</v>
+      </c>
+      <c r="Q23" s="28" t="s">
         <v>116</v>
       </c>
-      <c r="P23" s="25" t="s">
+      <c r="R23" s="25" t="s">
         <v>176</v>
       </c>
-      <c r="Q23" s="26">
+      <c r="S23" s="26">
         <v>32</v>
       </c>
-      <c r="R23" s="27" t="s">
-        <v>108</v>
-      </c>
-      <c r="S23" s="13"/>
-    </row>
-    <row r="24" spans="1:19" ht="17">
+      <c r="T23" s="27" t="s">
+        <v>108</v>
+      </c>
+      <c r="U23" s="13"/>
+    </row>
+    <row r="24" spans="1:21" ht="17">
       <c r="A24" s="20">
         <v>22</v>
       </c>
@@ -2661,7 +2992,7 @@
         <v>185</v>
       </c>
       <c r="G24" s="21" t="s">
-        <v>106</v>
+        <v>185</v>
       </c>
       <c r="H24" s="21" t="s">
         <v>106</v>
@@ -2669,36 +3000,42 @@
       <c r="I24" s="21" t="s">
         <v>106</v>
       </c>
-      <c r="J24" s="34">
-        <v>1</v>
-      </c>
-      <c r="K24" s="21" t="s">
+      <c r="J24" s="21" t="s">
+        <v>106</v>
+      </c>
+      <c r="K24" s="34">
+        <v>1</v>
+      </c>
+      <c r="L24" s="21" t="s">
         <v>37</v>
       </c>
-      <c r="L24" s="22" t="s">
+      <c r="M24" s="21" t="s">
+        <v>246</v>
+      </c>
+      <c r="N24" s="22" t="s">
         <v>148</v>
       </c>
-      <c r="M24" s="20" t="s">
+      <c r="O24" s="20" t="s">
         <v>99</v>
       </c>
-      <c r="N24" s="23">
-        <v>0</v>
-      </c>
-      <c r="O24" s="28" t="s">
+      <c r="P24" s="23">
+        <v>0</v>
+      </c>
+      <c r="Q24" s="28" t="s">
         <v>116</v>
       </c>
-      <c r="P24" s="25" t="s">
+      <c r="R24" s="25" t="s">
         <v>176</v>
       </c>
-      <c r="Q24" s="26">
-        <v>0</v>
-      </c>
-      <c r="R24" s="27" t="s">
-        <v>108</v>
-      </c>
-      <c r="S24" s="13"/>
-    </row>
-    <row r="25" spans="1:19" ht="17">
+      <c r="S24" s="26">
+        <v>0</v>
+      </c>
+      <c r="T24" s="27" t="s">
+        <v>108</v>
+      </c>
+      <c r="U24" s="13"/>
+    </row>
+    <row r="25" spans="1:21" ht="17">
       <c r="A25" s="20">
         <v>23</v>
       </c>
@@ -2718,44 +3055,50 @@
         <v>203</v>
       </c>
       <c r="G25" s="21" t="s">
+        <v>203</v>
+      </c>
+      <c r="H25" s="21" t="s">
         <v>180</v>
       </c>
-      <c r="H25" s="21" t="s">
-        <v>105</v>
-      </c>
       <c r="I25" s="21" t="s">
         <v>105</v>
       </c>
-      <c r="J25" s="34">
-        <v>1</v>
-      </c>
-      <c r="K25" s="21" t="s">
+      <c r="J25" s="21" t="s">
+        <v>105</v>
+      </c>
+      <c r="K25" s="34">
+        <v>1</v>
+      </c>
+      <c r="L25" s="21" t="s">
         <v>39</v>
       </c>
-      <c r="L25" s="22" t="s">
+      <c r="M25" s="21" t="s">
+        <v>247</v>
+      </c>
+      <c r="N25" s="22" t="s">
         <v>131</v>
       </c>
-      <c r="M25" s="20" t="s">
+      <c r="O25" s="20" t="s">
         <v>99</v>
       </c>
-      <c r="N25" s="23">
-        <v>0</v>
-      </c>
-      <c r="O25" s="28" t="s">
+      <c r="P25" s="23">
+        <v>0</v>
+      </c>
+      <c r="Q25" s="28" t="s">
         <v>109</v>
       </c>
-      <c r="P25" s="29" t="s">
+      <c r="R25" s="29" t="s">
         <v>123</v>
       </c>
-      <c r="Q25" s="26">
+      <c r="S25" s="26">
         <v>29</v>
       </c>
-      <c r="R25" s="27" t="s">
-        <v>108</v>
-      </c>
-      <c r="S25" s="13"/>
-    </row>
-    <row r="26" spans="1:19" ht="17">
+      <c r="T25" s="27" t="s">
+        <v>108</v>
+      </c>
+      <c r="U25" s="13"/>
+    </row>
+    <row r="26" spans="1:21" ht="17">
       <c r="A26" s="20">
         <v>24</v>
       </c>
@@ -2775,7 +3118,7 @@
         <v>185</v>
       </c>
       <c r="G26" s="21" t="s">
-        <v>106</v>
+        <v>185</v>
       </c>
       <c r="H26" s="21" t="s">
         <v>106</v>
@@ -2783,36 +3126,42 @@
       <c r="I26" s="21" t="s">
         <v>106</v>
       </c>
-      <c r="J26" s="34">
-        <v>1</v>
-      </c>
-      <c r="K26" s="21" t="s">
+      <c r="J26" s="21" t="s">
+        <v>106</v>
+      </c>
+      <c r="K26" s="34">
+        <v>1</v>
+      </c>
+      <c r="L26" s="21" t="s">
         <v>40</v>
       </c>
-      <c r="L26" s="22" t="s">
+      <c r="M26" s="21" t="s">
+        <v>248</v>
+      </c>
+      <c r="N26" s="22" t="s">
         <v>158</v>
       </c>
-      <c r="M26" s="20" t="s">
+      <c r="O26" s="20" t="s">
         <v>99</v>
       </c>
-      <c r="N26" s="23">
-        <v>1</v>
-      </c>
-      <c r="O26" s="28" t="s">
+      <c r="P26" s="23">
+        <v>1</v>
+      </c>
+      <c r="Q26" s="28" t="s">
         <v>116</v>
       </c>
-      <c r="P26" s="30" t="s">
+      <c r="R26" s="30" t="s">
         <v>123</v>
       </c>
-      <c r="Q26" s="26">
+      <c r="S26" s="26">
         <v>30</v>
       </c>
-      <c r="R26" s="27" t="s">
-        <v>108</v>
-      </c>
-      <c r="S26" s="13"/>
-    </row>
-    <row r="27" spans="1:19" ht="17">
+      <c r="T26" s="27" t="s">
+        <v>108</v>
+      </c>
+      <c r="U26" s="13"/>
+    </row>
+    <row r="27" spans="1:21" ht="17">
       <c r="A27" s="20">
         <v>25</v>
       </c>
@@ -2832,7 +3181,7 @@
         <v>185</v>
       </c>
       <c r="G27" s="21" t="s">
-        <v>106</v>
+        <v>185</v>
       </c>
       <c r="H27" s="21" t="s">
         <v>106</v>
@@ -2840,36 +3189,42 @@
       <c r="I27" s="21" t="s">
         <v>106</v>
       </c>
-      <c r="J27" s="34">
-        <v>1</v>
-      </c>
-      <c r="K27" s="21" t="s">
+      <c r="J27" s="21" t="s">
+        <v>106</v>
+      </c>
+      <c r="K27" s="34">
+        <v>1</v>
+      </c>
+      <c r="L27" s="21" t="s">
         <v>41</v>
       </c>
-      <c r="L27" s="22" t="s">
+      <c r="M27" s="21" t="s">
+        <v>249</v>
+      </c>
+      <c r="N27" s="22" t="s">
         <v>159</v>
       </c>
-      <c r="M27" s="20" t="s">
+      <c r="O27" s="20" t="s">
         <v>99</v>
       </c>
-      <c r="N27" s="23">
-        <v>1</v>
-      </c>
-      <c r="O27" s="28" t="s">
+      <c r="P27" s="23">
+        <v>1</v>
+      </c>
+      <c r="Q27" s="28" t="s">
         <v>116</v>
       </c>
-      <c r="P27" s="30" t="s">
+      <c r="R27" s="30" t="s">
         <v>123</v>
       </c>
-      <c r="Q27" s="26">
-        <v>0</v>
-      </c>
-      <c r="R27" s="27" t="s">
-        <v>108</v>
-      </c>
-      <c r="S27" s="13"/>
-    </row>
-    <row r="28" spans="1:19" ht="17">
+      <c r="S27" s="26">
+        <v>0</v>
+      </c>
+      <c r="T27" s="27" t="s">
+        <v>108</v>
+      </c>
+      <c r="U27" s="13"/>
+    </row>
+    <row r="28" spans="1:21" ht="17">
       <c r="A28" s="20">
         <v>26</v>
       </c>
@@ -2889,44 +3244,50 @@
         <v>203</v>
       </c>
       <c r="G28" s="21" t="s">
+        <v>203</v>
+      </c>
+      <c r="H28" s="21" t="s">
         <v>180</v>
       </c>
-      <c r="H28" s="21" t="s">
-        <v>105</v>
-      </c>
       <c r="I28" s="21" t="s">
         <v>105</v>
       </c>
-      <c r="J28" s="34">
-        <v>1</v>
-      </c>
-      <c r="K28" s="21" t="s">
+      <c r="J28" s="21" t="s">
+        <v>105</v>
+      </c>
+      <c r="K28" s="34">
+        <v>1</v>
+      </c>
+      <c r="L28" s="21" t="s">
         <v>43</v>
       </c>
-      <c r="L28" s="22" t="s">
+      <c r="M28" s="21" t="s">
+        <v>250</v>
+      </c>
+      <c r="N28" s="22" t="s">
         <v>132</v>
       </c>
-      <c r="M28" s="20" t="s">
+      <c r="O28" s="20" t="s">
         <v>99</v>
       </c>
-      <c r="N28" s="23">
-        <v>0</v>
-      </c>
-      <c r="O28" s="28" t="s">
+      <c r="P28" s="23">
+        <v>0</v>
+      </c>
+      <c r="Q28" s="28" t="s">
         <v>109</v>
       </c>
-      <c r="P28" s="25" t="s">
+      <c r="R28" s="25" t="s">
         <v>176</v>
       </c>
-      <c r="Q28" s="26">
+      <c r="S28" s="26">
         <v>35</v>
       </c>
-      <c r="R28" s="27" t="s">
-        <v>108</v>
-      </c>
-      <c r="S28" s="13"/>
-    </row>
-    <row r="29" spans="1:19" ht="17">
+      <c r="T28" s="27" t="s">
+        <v>108</v>
+      </c>
+      <c r="U28" s="13"/>
+    </row>
+    <row r="29" spans="1:21" ht="17">
       <c r="A29" s="20">
         <v>27</v>
       </c>
@@ -2946,7 +3307,7 @@
         <v>185</v>
       </c>
       <c r="G29" s="21" t="s">
-        <v>106</v>
+        <v>185</v>
       </c>
       <c r="H29" s="21" t="s">
         <v>106</v>
@@ -2954,36 +3315,42 @@
       <c r="I29" s="21" t="s">
         <v>106</v>
       </c>
-      <c r="J29" s="34">
-        <v>1</v>
-      </c>
-      <c r="K29" s="21" t="s">
+      <c r="J29" s="21" t="s">
+        <v>106</v>
+      </c>
+      <c r="K29" s="34">
+        <v>1</v>
+      </c>
+      <c r="L29" s="21" t="s">
         <v>44</v>
       </c>
-      <c r="L29" s="22" t="s">
+      <c r="M29" s="21" t="s">
+        <v>251</v>
+      </c>
+      <c r="N29" s="22" t="s">
         <v>160</v>
       </c>
-      <c r="M29" s="20" t="s">
+      <c r="O29" s="20" t="s">
         <v>99</v>
       </c>
-      <c r="N29" s="23">
-        <v>0</v>
-      </c>
-      <c r="O29" s="28" t="s">
+      <c r="P29" s="23">
+        <v>0</v>
+      </c>
+      <c r="Q29" s="28" t="s">
         <v>116</v>
       </c>
-      <c r="P29" s="25" t="s">
+      <c r="R29" s="25" t="s">
         <v>176</v>
       </c>
-      <c r="Q29" s="26">
+      <c r="S29" s="26">
         <v>36</v>
       </c>
-      <c r="R29" s="27" t="s">
-        <v>108</v>
-      </c>
-      <c r="S29" s="13"/>
-    </row>
-    <row r="30" spans="1:19" ht="17">
+      <c r="T29" s="27" t="s">
+        <v>108</v>
+      </c>
+      <c r="U29" s="13"/>
+    </row>
+    <row r="30" spans="1:21" ht="17">
       <c r="A30" s="20">
         <v>28</v>
       </c>
@@ -3003,7 +3370,7 @@
         <v>185</v>
       </c>
       <c r="G30" s="21" t="s">
-        <v>106</v>
+        <v>185</v>
       </c>
       <c r="H30" s="21" t="s">
         <v>106</v>
@@ -3011,36 +3378,42 @@
       <c r="I30" s="21" t="s">
         <v>106</v>
       </c>
-      <c r="J30" s="34">
-        <v>1</v>
-      </c>
-      <c r="K30" s="21" t="s">
+      <c r="J30" s="21" t="s">
+        <v>106</v>
+      </c>
+      <c r="K30" s="34">
+        <v>1</v>
+      </c>
+      <c r="L30" s="21" t="s">
         <v>45</v>
       </c>
-      <c r="L30" s="22" t="s">
+      <c r="M30" s="21" t="s">
+        <v>252</v>
+      </c>
+      <c r="N30" s="22" t="s">
         <v>161</v>
       </c>
-      <c r="M30" s="20" t="s">
+      <c r="O30" s="20" t="s">
         <v>99</v>
       </c>
-      <c r="N30" s="23">
-        <v>0</v>
-      </c>
-      <c r="O30" s="28" t="s">
+      <c r="P30" s="23">
+        <v>0</v>
+      </c>
+      <c r="Q30" s="28" t="s">
         <v>116</v>
       </c>
-      <c r="P30" s="25" t="s">
+      <c r="R30" s="25" t="s">
         <v>176</v>
       </c>
-      <c r="Q30" s="26">
-        <v>0</v>
-      </c>
-      <c r="R30" s="27" t="s">
-        <v>108</v>
-      </c>
-      <c r="S30" s="13"/>
-    </row>
-    <row r="31" spans="1:19" ht="17">
+      <c r="S30" s="26">
+        <v>0</v>
+      </c>
+      <c r="T30" s="27" t="s">
+        <v>108</v>
+      </c>
+      <c r="U30" s="13"/>
+    </row>
+    <row r="31" spans="1:21" ht="17">
       <c r="A31" s="20">
         <v>29</v>
       </c>
@@ -3060,44 +3433,50 @@
         <v>203</v>
       </c>
       <c r="G31" s="21" t="s">
+        <v>203</v>
+      </c>
+      <c r="H31" s="21" t="s">
         <v>180</v>
       </c>
-      <c r="H31" s="21" t="s">
-        <v>105</v>
-      </c>
       <c r="I31" s="21" t="s">
         <v>105</v>
       </c>
-      <c r="J31" s="34">
-        <v>1</v>
-      </c>
-      <c r="K31" s="21" t="s">
+      <c r="J31" s="21" t="s">
+        <v>105</v>
+      </c>
+      <c r="K31" s="34">
+        <v>1</v>
+      </c>
+      <c r="L31" s="21" t="s">
         <v>47</v>
       </c>
-      <c r="L31" s="22" t="s">
+      <c r="M31" s="21" t="s">
+        <v>253</v>
+      </c>
+      <c r="N31" s="22" t="s">
         <v>133</v>
       </c>
-      <c r="M31" s="20" t="s">
+      <c r="O31" s="20" t="s">
         <v>99</v>
       </c>
-      <c r="N31" s="23">
-        <v>0</v>
-      </c>
-      <c r="O31" s="28" t="s">
+      <c r="P31" s="23">
+        <v>0</v>
+      </c>
+      <c r="Q31" s="28" t="s">
         <v>109</v>
       </c>
-      <c r="P31" s="29" t="s">
+      <c r="R31" s="29" t="s">
         <v>123</v>
       </c>
-      <c r="Q31" s="26">
+      <c r="S31" s="26">
         <v>33</v>
       </c>
-      <c r="R31" s="27" t="s">
-        <v>108</v>
-      </c>
-      <c r="S31" s="13"/>
-    </row>
-    <row r="32" spans="1:19" ht="17">
+      <c r="T31" s="27" t="s">
+        <v>108</v>
+      </c>
+      <c r="U31" s="13"/>
+    </row>
+    <row r="32" spans="1:21" ht="17">
       <c r="A32" s="20">
         <v>30</v>
       </c>
@@ -3117,7 +3496,7 @@
         <v>185</v>
       </c>
       <c r="G32" s="21" t="s">
-        <v>106</v>
+        <v>185</v>
       </c>
       <c r="H32" s="21" t="s">
         <v>106</v>
@@ -3125,36 +3504,42 @@
       <c r="I32" s="21" t="s">
         <v>106</v>
       </c>
-      <c r="J32" s="34">
-        <v>1</v>
-      </c>
-      <c r="K32" s="21" t="s">
+      <c r="J32" s="21" t="s">
+        <v>106</v>
+      </c>
+      <c r="K32" s="34">
+        <v>1</v>
+      </c>
+      <c r="L32" s="21" t="s">
         <v>48</v>
       </c>
-      <c r="L32" s="22" t="s">
+      <c r="M32" s="21" t="s">
+        <v>254</v>
+      </c>
+      <c r="N32" s="22" t="s">
         <v>162</v>
       </c>
-      <c r="M32" s="20" t="s">
+      <c r="O32" s="20" t="s">
         <v>99</v>
       </c>
-      <c r="N32" s="23">
-        <v>1</v>
-      </c>
-      <c r="O32" s="28" t="s">
+      <c r="P32" s="23">
+        <v>1</v>
+      </c>
+      <c r="Q32" s="28" t="s">
         <v>116</v>
       </c>
-      <c r="P32" s="30" t="s">
+      <c r="R32" s="30" t="s">
         <v>123</v>
       </c>
-      <c r="Q32" s="26">
+      <c r="S32" s="26">
         <v>34</v>
       </c>
-      <c r="R32" s="27" t="s">
-        <v>108</v>
-      </c>
-      <c r="S32" s="13"/>
-    </row>
-    <row r="33" spans="1:19" ht="17">
+      <c r="T32" s="27" t="s">
+        <v>108</v>
+      </c>
+      <c r="U32" s="13"/>
+    </row>
+    <row r="33" spans="1:21" ht="17">
       <c r="A33" s="20">
         <v>31</v>
       </c>
@@ -3174,7 +3559,7 @@
         <v>185</v>
       </c>
       <c r="G33" s="21" t="s">
-        <v>106</v>
+        <v>185</v>
       </c>
       <c r="H33" s="21" t="s">
         <v>106</v>
@@ -3182,36 +3567,42 @@
       <c r="I33" s="21" t="s">
         <v>106</v>
       </c>
-      <c r="J33" s="34">
-        <v>1</v>
-      </c>
-      <c r="K33" s="21" t="s">
+      <c r="J33" s="21" t="s">
+        <v>106</v>
+      </c>
+      <c r="K33" s="34">
+        <v>1</v>
+      </c>
+      <c r="L33" s="21" t="s">
         <v>49</v>
       </c>
-      <c r="L33" s="22" t="s">
+      <c r="M33" s="21" t="s">
+        <v>255</v>
+      </c>
+      <c r="N33" s="22" t="s">
         <v>163</v>
       </c>
-      <c r="M33" s="20" t="s">
+      <c r="O33" s="20" t="s">
         <v>99</v>
       </c>
-      <c r="N33" s="23">
-        <v>1</v>
-      </c>
-      <c r="O33" s="28" t="s">
+      <c r="P33" s="23">
+        <v>1</v>
+      </c>
+      <c r="Q33" s="28" t="s">
         <v>116</v>
       </c>
-      <c r="P33" s="30" t="s">
+      <c r="R33" s="30" t="s">
         <v>123</v>
       </c>
-      <c r="Q33" s="26">
-        <v>0</v>
-      </c>
-      <c r="R33" s="27" t="s">
-        <v>108</v>
-      </c>
-      <c r="S33" s="13"/>
-    </row>
-    <row r="34" spans="1:19" ht="19" customHeight="1">
+      <c r="S33" s="26">
+        <v>0</v>
+      </c>
+      <c r="T33" s="27" t="s">
+        <v>108</v>
+      </c>
+      <c r="U33" s="13"/>
+    </row>
+    <row r="34" spans="1:21" ht="19" customHeight="1">
       <c r="A34" s="8">
         <v>32</v>
       </c>
@@ -3231,44 +3622,50 @@
         <v>202</v>
       </c>
       <c r="G34" s="6" t="s">
+        <v>202</v>
+      </c>
+      <c r="H34" s="6" t="s">
         <v>181</v>
       </c>
-      <c r="H34" s="6" t="s">
-        <v>105</v>
-      </c>
       <c r="I34" s="6" t="s">
         <v>105</v>
       </c>
-      <c r="J34" s="6">
-        <v>1</v>
-      </c>
-      <c r="K34" s="6" t="s">
+      <c r="J34" s="6" t="s">
+        <v>105</v>
+      </c>
+      <c r="K34" s="6">
+        <v>1</v>
+      </c>
+      <c r="L34" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="L34" s="7" t="s">
+      <c r="M34" s="6" t="s">
+        <v>256</v>
+      </c>
+      <c r="N34" s="7" t="s">
         <v>134</v>
       </c>
-      <c r="M34" s="8" t="s">
+      <c r="O34" s="8" t="s">
         <v>50</v>
       </c>
-      <c r="N34" s="9">
-        <v>0</v>
-      </c>
-      <c r="O34" s="10" t="s">
+      <c r="P34" s="9">
+        <v>0</v>
+      </c>
+      <c r="Q34" s="10" t="s">
         <v>109</v>
       </c>
-      <c r="P34" s="6" t="s">
+      <c r="R34" s="6" t="s">
         <v>172</v>
       </c>
-      <c r="Q34" s="5">
-        <v>1</v>
-      </c>
-      <c r="R34" s="14" t="s">
-        <v>108</v>
-      </c>
-      <c r="S34" s="5"/>
-    </row>
-    <row r="35" spans="1:19" ht="17">
+      <c r="S34" s="5">
+        <v>1</v>
+      </c>
+      <c r="T34" s="14" t="s">
+        <v>108</v>
+      </c>
+      <c r="U34" s="5"/>
+    </row>
+    <row r="35" spans="1:21" ht="17">
       <c r="A35" s="8">
         <v>33</v>
       </c>
@@ -3288,44 +3685,50 @@
         <v>202</v>
       </c>
       <c r="G35" s="6" t="s">
+        <v>202</v>
+      </c>
+      <c r="H35" s="6" t="s">
         <v>181</v>
       </c>
-      <c r="H35" s="6" t="s">
-        <v>105</v>
-      </c>
       <c r="I35" s="6" t="s">
         <v>105</v>
       </c>
-      <c r="J35" s="6">
-        <v>1</v>
-      </c>
-      <c r="K35" s="6" t="s">
+      <c r="J35" s="6" t="s">
+        <v>105</v>
+      </c>
+      <c r="K35" s="6">
+        <v>1</v>
+      </c>
+      <c r="L35" s="6" t="s">
         <v>54</v>
       </c>
-      <c r="L35" s="7" t="s">
+      <c r="M35" s="6" t="s">
+        <v>257</v>
+      </c>
+      <c r="N35" s="7" t="s">
         <v>135</v>
       </c>
-      <c r="M35" s="8" t="s">
+      <c r="O35" s="8" t="s">
         <v>50</v>
       </c>
-      <c r="N35" s="9">
-        <v>0</v>
-      </c>
-      <c r="O35" s="10" t="s">
+      <c r="P35" s="9">
+        <v>0</v>
+      </c>
+      <c r="Q35" s="10" t="s">
         <v>109</v>
       </c>
-      <c r="P35" s="6" t="s">
+      <c r="R35" s="6" t="s">
         <v>172</v>
       </c>
-      <c r="Q35" s="5">
+      <c r="S35" s="5">
         <v>3</v>
       </c>
-      <c r="R35" s="14" t="s">
-        <v>108</v>
-      </c>
-      <c r="S35" s="5"/>
-    </row>
-    <row r="36" spans="1:19" ht="17">
+      <c r="T35" s="14" t="s">
+        <v>108</v>
+      </c>
+      <c r="U35" s="5"/>
+    </row>
+    <row r="36" spans="1:21" ht="17">
       <c r="A36" s="8">
         <v>35</v>
       </c>
@@ -3345,44 +3748,50 @@
         <v>202</v>
       </c>
       <c r="G36" s="6" t="s">
+        <v>202</v>
+      </c>
+      <c r="H36" s="6" t="s">
         <v>181</v>
       </c>
-      <c r="H36" s="6" t="s">
-        <v>105</v>
-      </c>
       <c r="I36" s="6" t="s">
         <v>105</v>
       </c>
-      <c r="J36" s="6">
-        <v>1</v>
-      </c>
-      <c r="K36" s="6" t="s">
+      <c r="J36" s="6" t="s">
+        <v>105</v>
+      </c>
+      <c r="K36" s="6">
+        <v>1</v>
+      </c>
+      <c r="L36" s="6" t="s">
         <v>58</v>
       </c>
-      <c r="L36" s="7" t="s">
+      <c r="M36" s="6" t="s">
+        <v>258</v>
+      </c>
+      <c r="N36" s="7" t="s">
         <v>165</v>
       </c>
-      <c r="M36" s="8" t="s">
+      <c r="O36" s="8" t="s">
         <v>50</v>
       </c>
-      <c r="N36" s="9">
-        <v>0</v>
-      </c>
-      <c r="O36" s="10" t="s">
+      <c r="P36" s="9">
+        <v>0</v>
+      </c>
+      <c r="Q36" s="10" t="s">
         <v>109</v>
       </c>
-      <c r="P36" s="15" t="s">
+      <c r="R36" s="15" t="s">
         <v>175</v>
       </c>
-      <c r="Q36" s="5">
+      <c r="S36" s="5">
         <v>2</v>
       </c>
-      <c r="R36" s="14" t="s">
-        <v>108</v>
-      </c>
-      <c r="S36" s="5"/>
-    </row>
-    <row r="37" spans="1:19" ht="17">
+      <c r="T36" s="14" t="s">
+        <v>108</v>
+      </c>
+      <c r="U36" s="5"/>
+    </row>
+    <row r="37" spans="1:21" ht="17">
       <c r="A37" s="8">
         <v>34</v>
       </c>
@@ -3402,44 +3811,50 @@
         <v>202</v>
       </c>
       <c r="G37" s="6" t="s">
+        <v>202</v>
+      </c>
+      <c r="H37" s="6" t="s">
         <v>181</v>
       </c>
-      <c r="H37" s="6" t="s">
-        <v>105</v>
-      </c>
       <c r="I37" s="6" t="s">
         <v>105</v>
       </c>
-      <c r="J37" s="6">
-        <v>1</v>
-      </c>
-      <c r="K37" s="6" t="s">
+      <c r="J37" s="6" t="s">
+        <v>105</v>
+      </c>
+      <c r="K37" s="6">
+        <v>1</v>
+      </c>
+      <c r="L37" s="6" t="s">
         <v>56</v>
       </c>
-      <c r="L37" s="7" t="s">
+      <c r="M37" s="6" t="s">
+        <v>259</v>
+      </c>
+      <c r="N37" s="7" t="s">
         <v>164</v>
       </c>
-      <c r="M37" s="8" t="s">
+      <c r="O37" s="8" t="s">
         <v>50</v>
       </c>
-      <c r="N37" s="9">
-        <v>0</v>
-      </c>
-      <c r="O37" s="10" t="s">
+      <c r="P37" s="9">
+        <v>0</v>
+      </c>
+      <c r="Q37" s="10" t="s">
         <v>109</v>
       </c>
-      <c r="P37" s="15" t="s">
+      <c r="R37" s="15" t="s">
         <v>175</v>
       </c>
-      <c r="Q37" s="5">
+      <c r="S37" s="5">
         <v>4</v>
       </c>
-      <c r="R37" s="14" t="s">
-        <v>108</v>
-      </c>
-      <c r="S37" s="5"/>
-    </row>
-    <row r="38" spans="1:19" ht="17">
+      <c r="T37" s="14" t="s">
+        <v>108</v>
+      </c>
+      <c r="U37" s="5"/>
+    </row>
+    <row r="38" spans="1:21" ht="17">
       <c r="A38" s="8">
         <v>36</v>
       </c>
@@ -3459,44 +3874,50 @@
         <v>202</v>
       </c>
       <c r="G38" s="6" t="s">
+        <v>202</v>
+      </c>
+      <c r="H38" s="6" t="s">
         <v>181</v>
       </c>
-      <c r="H38" s="6" t="s">
-        <v>105</v>
-      </c>
       <c r="I38" s="6" t="s">
         <v>105</v>
       </c>
-      <c r="J38" s="6">
-        <v>1</v>
-      </c>
-      <c r="K38" s="6" t="s">
+      <c r="J38" s="6" t="s">
+        <v>105</v>
+      </c>
+      <c r="K38" s="6">
+        <v>1</v>
+      </c>
+      <c r="L38" s="6" t="s">
         <v>60</v>
       </c>
-      <c r="L38" s="7" t="s">
+      <c r="M38" s="6" t="s">
+        <v>260</v>
+      </c>
+      <c r="N38" s="7" t="s">
         <v>166</v>
       </c>
-      <c r="M38" s="8" t="s">
+      <c r="O38" s="8" t="s">
         <v>50</v>
       </c>
-      <c r="N38" s="9">
-        <v>0</v>
-      </c>
-      <c r="O38" s="10" t="s">
+      <c r="P38" s="9">
+        <v>0</v>
+      </c>
+      <c r="Q38" s="10" t="s">
         <v>109</v>
       </c>
-      <c r="P38" s="15" t="s">
+      <c r="R38" s="15" t="s">
         <v>175</v>
       </c>
-      <c r="Q38" s="5">
+      <c r="S38" s="5">
         <v>20</v>
       </c>
-      <c r="R38" s="14" t="s">
-        <v>108</v>
-      </c>
-      <c r="S38" s="5"/>
-    </row>
-    <row r="39" spans="1:19" ht="17">
+      <c r="T38" s="14" t="s">
+        <v>108</v>
+      </c>
+      <c r="U38" s="5"/>
+    </row>
+    <row r="39" spans="1:21" ht="17">
       <c r="A39" s="8">
         <v>38</v>
       </c>
@@ -3516,44 +3937,50 @@
         <v>202</v>
       </c>
       <c r="G39" s="6" t="s">
+        <v>202</v>
+      </c>
+      <c r="H39" s="6" t="s">
         <v>181</v>
       </c>
-      <c r="H39" s="6" t="s">
-        <v>105</v>
-      </c>
       <c r="I39" s="6" t="s">
         <v>105</v>
       </c>
-      <c r="J39" s="6">
-        <v>1</v>
-      </c>
-      <c r="K39" s="6" t="s">
+      <c r="J39" s="6" t="s">
+        <v>105</v>
+      </c>
+      <c r="K39" s="6">
+        <v>1</v>
+      </c>
+      <c r="L39" s="6" t="s">
         <v>64</v>
       </c>
-      <c r="L39" s="7" t="s">
+      <c r="M39" s="6" t="s">
+        <v>261</v>
+      </c>
+      <c r="N39" s="7" t="s">
         <v>137</v>
       </c>
-      <c r="M39" s="8" t="s">
+      <c r="O39" s="8" t="s">
         <v>50</v>
       </c>
-      <c r="N39" s="9">
-        <v>0</v>
-      </c>
-      <c r="O39" s="10" t="s">
+      <c r="P39" s="9">
+        <v>0</v>
+      </c>
+      <c r="Q39" s="10" t="s">
         <v>109</v>
       </c>
-      <c r="P39" s="31" t="s">
+      <c r="R39" s="31" t="s">
         <v>173</v>
       </c>
-      <c r="Q39" s="5">
+      <c r="S39" s="5">
         <v>5</v>
       </c>
-      <c r="R39" s="14" t="s">
-        <v>108</v>
-      </c>
-      <c r="S39" s="5"/>
-    </row>
-    <row r="40" spans="1:19" ht="17">
+      <c r="T39" s="14" t="s">
+        <v>108</v>
+      </c>
+      <c r="U39" s="5"/>
+    </row>
+    <row r="40" spans="1:21" ht="17">
       <c r="A40" s="8">
         <v>37</v>
       </c>
@@ -3573,44 +4000,50 @@
         <v>202</v>
       </c>
       <c r="G40" s="6" t="s">
+        <v>202</v>
+      </c>
+      <c r="H40" s="6" t="s">
         <v>181</v>
       </c>
-      <c r="H40" s="6" t="s">
-        <v>105</v>
-      </c>
       <c r="I40" s="6" t="s">
         <v>105</v>
       </c>
-      <c r="J40" s="6">
-        <v>1</v>
-      </c>
-      <c r="K40" s="6" t="s">
+      <c r="J40" s="6" t="s">
+        <v>105</v>
+      </c>
+      <c r="K40" s="6">
+        <v>1</v>
+      </c>
+      <c r="L40" s="6" t="s">
         <v>62</v>
       </c>
-      <c r="L40" s="7" t="s">
+      <c r="M40" s="6" t="s">
+        <v>262</v>
+      </c>
+      <c r="N40" s="7" t="s">
         <v>136</v>
       </c>
-      <c r="M40" s="8" t="s">
+      <c r="O40" s="8" t="s">
         <v>50</v>
       </c>
-      <c r="N40" s="9">
-        <v>0</v>
-      </c>
-      <c r="O40" s="10" t="s">
+      <c r="P40" s="9">
+        <v>0</v>
+      </c>
+      <c r="Q40" s="10" t="s">
         <v>109</v>
       </c>
-      <c r="P40" s="31" t="s">
+      <c r="R40" s="31" t="s">
         <v>173</v>
       </c>
-      <c r="Q40" s="5">
+      <c r="S40" s="5">
         <v>6</v>
       </c>
-      <c r="R40" s="14" t="s">
-        <v>108</v>
-      </c>
-      <c r="S40" s="5"/>
-    </row>
-    <row r="41" spans="1:19" ht="17">
+      <c r="T40" s="14" t="s">
+        <v>108</v>
+      </c>
+      <c r="U40" s="5"/>
+    </row>
+    <row r="41" spans="1:21" ht="17">
       <c r="A41" s="8">
         <v>40</v>
       </c>
@@ -3630,44 +4063,50 @@
         <v>202</v>
       </c>
       <c r="G41" s="6" t="s">
+        <v>202</v>
+      </c>
+      <c r="H41" s="6" t="s">
         <v>181</v>
       </c>
-      <c r="H41" s="6" t="s">
-        <v>105</v>
-      </c>
       <c r="I41" s="6" t="s">
         <v>105</v>
       </c>
-      <c r="J41" s="6">
-        <v>1</v>
-      </c>
-      <c r="K41" s="6" t="s">
+      <c r="J41" s="6" t="s">
+        <v>105</v>
+      </c>
+      <c r="K41" s="6">
+        <v>1</v>
+      </c>
+      <c r="L41" s="6" t="s">
         <v>68</v>
       </c>
-      <c r="L41" s="7" t="s">
+      <c r="M41" s="6" t="s">
+        <v>263</v>
+      </c>
+      <c r="N41" s="7" t="s">
         <v>139</v>
       </c>
-      <c r="M41" s="8" t="s">
+      <c r="O41" s="8" t="s">
         <v>50</v>
       </c>
-      <c r="N41" s="9">
-        <v>0</v>
-      </c>
-      <c r="O41" s="10" t="s">
+      <c r="P41" s="9">
+        <v>0</v>
+      </c>
+      <c r="Q41" s="10" t="s">
         <v>109</v>
       </c>
-      <c r="P41" s="32" t="s">
+      <c r="R41" s="32" t="s">
         <v>174</v>
       </c>
-      <c r="Q41" s="5">
+      <c r="S41" s="5">
         <v>7</v>
       </c>
-      <c r="R41" s="14" t="s">
-        <v>108</v>
-      </c>
-      <c r="S41" s="5"/>
-    </row>
-    <row r="42" spans="1:19" ht="17">
+      <c r="T41" s="14" t="s">
+        <v>108</v>
+      </c>
+      <c r="U41" s="5"/>
+    </row>
+    <row r="42" spans="1:21" ht="17">
       <c r="A42" s="8">
         <v>39</v>
       </c>
@@ -3687,44 +4126,50 @@
         <v>202</v>
       </c>
       <c r="G42" s="6" t="s">
+        <v>202</v>
+      </c>
+      <c r="H42" s="6" t="s">
         <v>181</v>
       </c>
-      <c r="H42" s="6" t="s">
-        <v>105</v>
-      </c>
       <c r="I42" s="6" t="s">
         <v>105</v>
       </c>
-      <c r="J42" s="6">
-        <v>1</v>
-      </c>
-      <c r="K42" s="6" t="s">
+      <c r="J42" s="6" t="s">
+        <v>105</v>
+      </c>
+      <c r="K42" s="6">
+        <v>1</v>
+      </c>
+      <c r="L42" s="6" t="s">
         <v>66</v>
       </c>
-      <c r="L42" s="7" t="s">
+      <c r="M42" s="6" t="s">
+        <v>264</v>
+      </c>
+      <c r="N42" s="7" t="s">
         <v>138</v>
       </c>
-      <c r="M42" s="8" t="s">
+      <c r="O42" s="8" t="s">
         <v>50</v>
       </c>
-      <c r="N42" s="9">
-        <v>0</v>
-      </c>
-      <c r="O42" s="10" t="s">
+      <c r="P42" s="9">
+        <v>0</v>
+      </c>
+      <c r="Q42" s="10" t="s">
         <v>109</v>
       </c>
-      <c r="P42" s="32" t="s">
+      <c r="R42" s="32" t="s">
         <v>174</v>
       </c>
-      <c r="Q42" s="5">
+      <c r="S42" s="5">
         <v>8</v>
       </c>
-      <c r="R42" s="14" t="s">
-        <v>108</v>
-      </c>
-      <c r="S42" s="5"/>
-    </row>
-    <row r="43" spans="1:19" ht="17">
+      <c r="T42" s="14" t="s">
+        <v>108</v>
+      </c>
+      <c r="U42" s="5"/>
+    </row>
+    <row r="43" spans="1:21" ht="17">
       <c r="A43" s="8">
         <v>41</v>
       </c>
@@ -3745,44 +4190,50 @@
         <v>202</v>
       </c>
       <c r="G43" s="6" t="s">
+        <v>202</v>
+      </c>
+      <c r="H43" s="6" t="s">
         <v>181</v>
       </c>
-      <c r="H43" s="6" t="s">
-        <v>105</v>
-      </c>
       <c r="I43" s="6" t="s">
         <v>105</v>
       </c>
-      <c r="J43" s="6">
-        <v>1</v>
-      </c>
-      <c r="K43" s="6" t="s">
+      <c r="J43" s="6" t="s">
+        <v>105</v>
+      </c>
+      <c r="K43" s="6">
+        <v>1</v>
+      </c>
+      <c r="L43" s="6" t="s">
         <v>198</v>
       </c>
-      <c r="L43" s="7" t="s">
+      <c r="M43" s="6" t="s">
+        <v>265</v>
+      </c>
+      <c r="N43" s="7" t="s">
         <v>220</v>
       </c>
-      <c r="M43" s="8" t="s">
+      <c r="O43" s="8" t="s">
         <v>50</v>
       </c>
-      <c r="N43" s="9">
-        <v>0</v>
-      </c>
-      <c r="O43" s="10" t="s">
+      <c r="P43" s="9">
+        <v>0</v>
+      </c>
+      <c r="Q43" s="10" t="s">
         <v>109</v>
       </c>
-      <c r="P43" s="25" t="s">
+      <c r="R43" s="25" t="s">
         <v>176</v>
       </c>
-      <c r="Q43" s="5">
+      <c r="S43" s="5">
         <v>11</v>
       </c>
-      <c r="R43" s="14" t="s">
-        <v>108</v>
-      </c>
-      <c r="S43" s="5"/>
-    </row>
-    <row r="44" spans="1:19" ht="17">
+      <c r="T43" s="14" t="s">
+        <v>108</v>
+      </c>
+      <c r="U43" s="5"/>
+    </row>
+    <row r="44" spans="1:21" ht="17">
       <c r="A44" s="8">
         <v>42</v>
       </c>
@@ -3803,44 +4254,50 @@
         <v>202</v>
       </c>
       <c r="G44" s="6" t="s">
+        <v>202</v>
+      </c>
+      <c r="H44" s="6" t="s">
         <v>181</v>
       </c>
-      <c r="H44" s="6" t="s">
-        <v>105</v>
-      </c>
       <c r="I44" s="6" t="s">
         <v>105</v>
       </c>
-      <c r="J44" s="6">
-        <v>1</v>
-      </c>
-      <c r="K44" s="6" t="s">
+      <c r="J44" s="6" t="s">
+        <v>105</v>
+      </c>
+      <c r="K44" s="6">
+        <v>1</v>
+      </c>
+      <c r="L44" s="6" t="s">
         <v>199</v>
       </c>
-      <c r="L44" s="7" t="s">
+      <c r="M44" s="6" t="s">
+        <v>266</v>
+      </c>
+      <c r="N44" s="7" t="s">
         <v>222</v>
       </c>
-      <c r="M44" s="8" t="s">
+      <c r="O44" s="8" t="s">
         <v>50</v>
       </c>
-      <c r="N44" s="9">
-        <v>0</v>
-      </c>
-      <c r="O44" s="10" t="s">
+      <c r="P44" s="9">
+        <v>0</v>
+      </c>
+      <c r="Q44" s="10" t="s">
         <v>109</v>
       </c>
-      <c r="P44" s="25" t="s">
+      <c r="R44" s="25" t="s">
         <v>176</v>
       </c>
-      <c r="Q44" s="5">
+      <c r="S44" s="5">
         <v>12</v>
       </c>
-      <c r="R44" s="14" t="s">
-        <v>108</v>
-      </c>
-      <c r="S44" s="5"/>
-    </row>
-    <row r="45" spans="1:19" ht="17">
+      <c r="T44" s="14" t="s">
+        <v>108</v>
+      </c>
+      <c r="U44" s="5"/>
+    </row>
+    <row r="45" spans="1:21" ht="17">
       <c r="A45" s="8">
         <v>43</v>
       </c>
@@ -3861,44 +4318,50 @@
         <v>202</v>
       </c>
       <c r="G45" s="6" t="s">
+        <v>202</v>
+      </c>
+      <c r="H45" s="6" t="s">
         <v>181</v>
       </c>
-      <c r="H45" s="6" t="s">
-        <v>105</v>
-      </c>
       <c r="I45" s="6" t="s">
         <v>105</v>
       </c>
-      <c r="J45" s="6">
-        <v>1</v>
-      </c>
-      <c r="K45" s="8" t="s">
+      <c r="J45" s="6" t="s">
+        <v>105</v>
+      </c>
+      <c r="K45" s="6">
+        <v>1</v>
+      </c>
+      <c r="L45" s="8" t="s">
         <v>201</v>
       </c>
-      <c r="L45" s="7" t="s">
+      <c r="M45" s="8" t="s">
+        <v>267</v>
+      </c>
+      <c r="N45" s="7" t="s">
         <v>221</v>
       </c>
-      <c r="M45" s="8" t="s">
+      <c r="O45" s="8" t="s">
         <v>50</v>
       </c>
-      <c r="N45" s="9">
-        <v>0</v>
-      </c>
-      <c r="O45" s="10" t="s">
+      <c r="P45" s="9">
+        <v>0</v>
+      </c>
+      <c r="Q45" s="10" t="s">
         <v>109</v>
       </c>
-      <c r="P45" s="29" t="s">
+      <c r="R45" s="29" t="s">
         <v>123</v>
       </c>
-      <c r="Q45" s="5">
+      <c r="S45" s="5">
         <v>9</v>
       </c>
-      <c r="R45" s="14" t="s">
-        <v>108</v>
-      </c>
-      <c r="S45" s="5"/>
-    </row>
-    <row r="46" spans="1:19" ht="17">
+      <c r="T45" s="14" t="s">
+        <v>108</v>
+      </c>
+      <c r="U45" s="5"/>
+    </row>
+    <row r="46" spans="1:21" ht="17">
       <c r="A46" s="8">
         <v>44</v>
       </c>
@@ -3919,44 +4382,50 @@
         <v>202</v>
       </c>
       <c r="G46" s="6" t="s">
+        <v>202</v>
+      </c>
+      <c r="H46" s="6" t="s">
         <v>181</v>
       </c>
-      <c r="H46" s="6" t="s">
-        <v>105</v>
-      </c>
       <c r="I46" s="6" t="s">
         <v>105</v>
       </c>
-      <c r="J46" s="6">
-        <v>1</v>
-      </c>
-      <c r="K46" s="6" t="s">
+      <c r="J46" s="6" t="s">
+        <v>105</v>
+      </c>
+      <c r="K46" s="6">
+        <v>1</v>
+      </c>
+      <c r="L46" s="6" t="s">
         <v>200</v>
       </c>
-      <c r="L46" s="7" t="s">
+      <c r="M46" s="6" t="s">
+        <v>268</v>
+      </c>
+      <c r="N46" s="7" t="s">
         <v>223</v>
       </c>
-      <c r="M46" s="8" t="s">
+      <c r="O46" s="8" t="s">
         <v>50</v>
       </c>
-      <c r="N46" s="9">
-        <v>0</v>
-      </c>
-      <c r="O46" s="10" t="s">
+      <c r="P46" s="9">
+        <v>0</v>
+      </c>
+      <c r="Q46" s="10" t="s">
         <v>109</v>
       </c>
-      <c r="P46" s="30" t="s">
+      <c r="R46" s="30" t="s">
         <v>123</v>
       </c>
-      <c r="Q46" s="5">
+      <c r="S46" s="5">
         <v>10</v>
       </c>
-      <c r="R46" s="14" t="s">
-        <v>108</v>
-      </c>
-      <c r="S46" s="5"/>
-    </row>
-    <row r="47" spans="1:19" ht="19" customHeight="1">
+      <c r="T46" s="14" t="s">
+        <v>108</v>
+      </c>
+      <c r="U46" s="5"/>
+    </row>
+    <row r="47" spans="1:21" ht="19" customHeight="1">
       <c r="A47" s="20">
         <v>45</v>
       </c>
@@ -3977,44 +4446,50 @@
         <v>203</v>
       </c>
       <c r="G47" s="21" t="s">
+        <v>203</v>
+      </c>
+      <c r="H47" s="21" t="s">
         <v>180</v>
       </c>
-      <c r="H47" s="21" t="s">
-        <v>105</v>
-      </c>
       <c r="I47" s="21" t="s">
         <v>105</v>
       </c>
-      <c r="J47" s="6">
-        <v>1</v>
-      </c>
-      <c r="K47" s="21" t="s">
+      <c r="J47" s="21" t="s">
+        <v>105</v>
+      </c>
+      <c r="K47" s="6">
+        <v>1</v>
+      </c>
+      <c r="L47" s="21" t="s">
         <v>70</v>
       </c>
-      <c r="L47" s="22" t="s">
+      <c r="M47" s="21" t="s">
+        <v>269</v>
+      </c>
+      <c r="N47" s="22" t="s">
         <v>140</v>
       </c>
-      <c r="M47" s="20" t="s">
+      <c r="O47" s="20" t="s">
         <v>100</v>
       </c>
-      <c r="N47" s="23">
-        <v>0</v>
-      </c>
-      <c r="O47" s="28" t="s">
+      <c r="P47" s="23">
+        <v>0</v>
+      </c>
+      <c r="Q47" s="28" t="s">
         <v>109</v>
       </c>
-      <c r="P47" s="31" t="s">
+      <c r="R47" s="31" t="s">
         <v>173</v>
       </c>
-      <c r="Q47" s="26">
+      <c r="S47" s="26">
         <v>41</v>
       </c>
-      <c r="R47" s="27" t="s">
-        <v>108</v>
-      </c>
-      <c r="S47" s="13"/>
-    </row>
-    <row r="48" spans="1:19" ht="17">
+      <c r="T47" s="27" t="s">
+        <v>108</v>
+      </c>
+      <c r="U47" s="13"/>
+    </row>
+    <row r="48" spans="1:21" ht="17">
       <c r="A48" s="20">
         <v>47</v>
       </c>
@@ -4035,44 +4510,50 @@
         <v>203</v>
       </c>
       <c r="G48" s="21" t="s">
+        <v>203</v>
+      </c>
+      <c r="H48" s="21" t="s">
         <v>180</v>
       </c>
-      <c r="H48" s="21" t="s">
-        <v>105</v>
-      </c>
       <c r="I48" s="21" t="s">
         <v>105</v>
       </c>
-      <c r="J48" s="6">
-        <v>1</v>
-      </c>
-      <c r="K48" s="21" t="s">
+      <c r="J48" s="21" t="s">
+        <v>105</v>
+      </c>
+      <c r="K48" s="6">
+        <v>1</v>
+      </c>
+      <c r="L48" s="21" t="s">
         <v>74</v>
       </c>
-      <c r="L48" s="22" t="s">
+      <c r="M48" s="21" t="s">
+        <v>270</v>
+      </c>
+      <c r="N48" s="22" t="s">
         <v>141</v>
       </c>
-      <c r="M48" s="20" t="s">
+      <c r="O48" s="20" t="s">
         <v>100</v>
       </c>
-      <c r="N48" s="23">
-        <v>0</v>
-      </c>
-      <c r="O48" s="28" t="s">
+      <c r="P48" s="23">
+        <v>0</v>
+      </c>
+      <c r="Q48" s="28" t="s">
         <v>109</v>
       </c>
-      <c r="P48" s="32" t="s">
+      <c r="R48" s="32" t="s">
         <v>174</v>
       </c>
-      <c r="Q48" s="26">
+      <c r="S48" s="26">
         <v>37</v>
       </c>
-      <c r="R48" s="27" t="s">
-        <v>108</v>
-      </c>
-      <c r="S48" s="13"/>
-    </row>
-    <row r="49" spans="1:19" ht="17">
+      <c r="T48" s="27" t="s">
+        <v>108</v>
+      </c>
+      <c r="U48" s="13"/>
+    </row>
+    <row r="49" spans="1:21" ht="17">
       <c r="A49" s="20">
         <v>46</v>
       </c>
@@ -4093,7 +4574,7 @@
         <v>185</v>
       </c>
       <c r="G49" s="21" t="s">
-        <v>106</v>
+        <v>185</v>
       </c>
       <c r="H49" s="21" t="s">
         <v>106</v>
@@ -4101,36 +4582,42 @@
       <c r="I49" s="21" t="s">
         <v>106</v>
       </c>
-      <c r="J49" s="6">
-        <v>1</v>
-      </c>
-      <c r="K49" s="21" t="s">
+      <c r="J49" s="21" t="s">
+        <v>106</v>
+      </c>
+      <c r="K49" s="6">
+        <v>1</v>
+      </c>
+      <c r="L49" s="21" t="s">
         <v>72</v>
       </c>
-      <c r="L49" s="22" t="s">
+      <c r="M49" s="21" t="s">
+        <v>271</v>
+      </c>
+      <c r="N49" s="22" t="s">
         <v>156</v>
       </c>
-      <c r="M49" s="20" t="s">
+      <c r="O49" s="20" t="s">
         <v>100</v>
       </c>
-      <c r="N49" s="23">
-        <v>0</v>
-      </c>
-      <c r="O49" s="28" t="s">
+      <c r="P49" s="23">
+        <v>0</v>
+      </c>
+      <c r="Q49" s="28" t="s">
         <v>116</v>
       </c>
-      <c r="P49" s="31" t="s">
+      <c r="R49" s="31" t="s">
         <v>173</v>
       </c>
-      <c r="Q49" s="26">
+      <c r="S49" s="26">
         <v>42</v>
       </c>
-      <c r="R49" s="27" t="s">
-        <v>108</v>
-      </c>
-      <c r="S49" s="13"/>
-    </row>
-    <row r="50" spans="1:19" ht="17">
+      <c r="T49" s="27" t="s">
+        <v>108</v>
+      </c>
+      <c r="U49" s="13"/>
+    </row>
+    <row r="50" spans="1:21" ht="17">
       <c r="A50" s="20">
         <v>48</v>
       </c>
@@ -4151,7 +4638,7 @@
         <v>185</v>
       </c>
       <c r="G50" s="21" t="s">
-        <v>106</v>
+        <v>185</v>
       </c>
       <c r="H50" s="21" t="s">
         <v>106</v>
@@ -4159,36 +4646,42 @@
       <c r="I50" s="21" t="s">
         <v>106</v>
       </c>
-      <c r="J50" s="6">
-        <v>1</v>
-      </c>
-      <c r="K50" s="21" t="s">
+      <c r="J50" s="21" t="s">
+        <v>106</v>
+      </c>
+      <c r="K50" s="6">
+        <v>1</v>
+      </c>
+      <c r="L50" s="21" t="s">
         <v>76</v>
       </c>
-      <c r="L50" s="22" t="s">
+      <c r="M50" s="21" t="s">
+        <v>272</v>
+      </c>
+      <c r="N50" s="22" t="s">
         <v>157</v>
       </c>
-      <c r="M50" s="20" t="s">
+      <c r="O50" s="20" t="s">
         <v>100</v>
       </c>
-      <c r="N50" s="23">
-        <v>1</v>
-      </c>
-      <c r="O50" s="28" t="s">
+      <c r="P50" s="23">
+        <v>1</v>
+      </c>
+      <c r="Q50" s="28" t="s">
         <v>116</v>
       </c>
-      <c r="P50" s="32" t="s">
+      <c r="R50" s="32" t="s">
         <v>174</v>
       </c>
-      <c r="Q50" s="26">
+      <c r="S50" s="26">
         <v>38</v>
       </c>
-      <c r="R50" s="27" t="s">
-        <v>108</v>
-      </c>
-      <c r="S50" s="13"/>
-    </row>
-    <row r="51" spans="1:19" ht="17" customHeight="1">
+      <c r="T50" s="27" t="s">
+        <v>108</v>
+      </c>
+      <c r="U50" s="13"/>
+    </row>
+    <row r="51" spans="1:21" ht="17" customHeight="1">
       <c r="A51" s="8">
         <v>49</v>
       </c>
@@ -4209,44 +4702,50 @@
         <v>187</v>
       </c>
       <c r="G51" s="6" t="s">
+        <v>285</v>
+      </c>
+      <c r="H51" s="6" t="s">
         <v>183</v>
-      </c>
-      <c r="H51" s="6" t="s">
-        <v>104</v>
       </c>
       <c r="I51" s="6" t="s">
         <v>104</v>
       </c>
-      <c r="J51" s="6">
-        <v>1</v>
-      </c>
-      <c r="K51" s="6" t="s">
+      <c r="J51" s="6" t="s">
+        <v>104</v>
+      </c>
+      <c r="K51" s="6">
+        <v>1</v>
+      </c>
+      <c r="L51" s="6" t="s">
         <v>79</v>
       </c>
-      <c r="L51" s="7" t="s">
+      <c r="M51" s="6" t="s">
+        <v>273</v>
+      </c>
+      <c r="N51" s="7" t="s">
         <v>193</v>
       </c>
-      <c r="M51" s="8" t="s">
+      <c r="O51" s="8" t="s">
         <v>77</v>
       </c>
-      <c r="N51" s="9">
-        <v>0</v>
-      </c>
-      <c r="O51" s="10" t="s">
+      <c r="P51" s="9">
+        <v>0</v>
+      </c>
+      <c r="Q51" s="10" t="s">
         <v>111</v>
       </c>
-      <c r="P51" s="25" t="s">
+      <c r="R51" s="25" t="s">
         <v>176</v>
       </c>
-      <c r="Q51" s="5">
+      <c r="S51" s="5">
         <v>48</v>
       </c>
-      <c r="R51" s="14" t="s">
-        <v>108</v>
-      </c>
-      <c r="S51" s="5"/>
-    </row>
-    <row r="52" spans="1:19" ht="17">
+      <c r="T51" s="14" t="s">
+        <v>108</v>
+      </c>
+      <c r="U51" s="5"/>
+    </row>
+    <row r="52" spans="1:21" ht="17">
       <c r="A52" s="8">
         <v>50</v>
       </c>
@@ -4267,46 +4766,52 @@
         <v>187</v>
       </c>
       <c r="G52" s="6" t="s">
+        <v>285</v>
+      </c>
+      <c r="H52" s="6" t="s">
         <v>183</v>
-      </c>
-      <c r="H52" s="6" t="s">
-        <v>104</v>
       </c>
       <c r="I52" s="6" t="s">
         <v>104</v>
       </c>
-      <c r="J52" s="6">
-        <v>1</v>
-      </c>
-      <c r="K52" s="6" t="s">
+      <c r="J52" s="6" t="s">
+        <v>104</v>
+      </c>
+      <c r="K52" s="6">
+        <v>1</v>
+      </c>
+      <c r="L52" s="6" t="s">
         <v>81</v>
       </c>
-      <c r="L52" s="7" t="s">
+      <c r="M52" s="6" t="s">
+        <v>274</v>
+      </c>
+      <c r="N52" s="7" t="s">
         <v>167</v>
       </c>
-      <c r="M52" s="8" t="s">
+      <c r="O52" s="8" t="s">
         <v>77</v>
       </c>
-      <c r="N52" s="9">
-        <v>0</v>
-      </c>
-      <c r="O52" s="10" t="s">
+      <c r="P52" s="9">
+        <v>0</v>
+      </c>
+      <c r="Q52" s="10" t="s">
         <v>111</v>
       </c>
-      <c r="P52" s="31" t="s">
+      <c r="R52" s="31" t="s">
         <v>173</v>
       </c>
-      <c r="Q52" s="5">
+      <c r="S52" s="5">
         <v>44</v>
       </c>
-      <c r="R52" s="14" t="s">
-        <v>108</v>
-      </c>
-      <c r="S52" s="5" t="s">
+      <c r="T52" s="14" t="s">
+        <v>108</v>
+      </c>
+      <c r="U52" s="5" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="53" spans="1:19" ht="17">
+    <row r="53" spans="1:21" ht="17">
       <c r="A53" s="8">
         <v>51</v>
       </c>
@@ -4327,44 +4832,50 @@
         <v>187</v>
       </c>
       <c r="G53" s="6" t="s">
+        <v>285</v>
+      </c>
+      <c r="H53" s="6" t="s">
         <v>183</v>
-      </c>
-      <c r="H53" s="6" t="s">
-        <v>104</v>
       </c>
       <c r="I53" s="6" t="s">
         <v>104</v>
       </c>
-      <c r="J53" s="6">
-        <v>1</v>
-      </c>
-      <c r="K53" s="6" t="s">
+      <c r="J53" s="6" t="s">
+        <v>104</v>
+      </c>
+      <c r="K53" s="6">
+        <v>1</v>
+      </c>
+      <c r="L53" s="6" t="s">
         <v>83</v>
       </c>
-      <c r="L53" s="7" t="s">
+      <c r="M53" s="6" t="s">
+        <v>275</v>
+      </c>
+      <c r="N53" s="7" t="s">
         <v>142</v>
       </c>
-      <c r="M53" s="8" t="s">
+      <c r="O53" s="8" t="s">
         <v>77</v>
       </c>
-      <c r="N53" s="9">
-        <v>0</v>
-      </c>
-      <c r="O53" s="10" t="s">
+      <c r="P53" s="9">
+        <v>0</v>
+      </c>
+      <c r="Q53" s="10" t="s">
         <v>111</v>
       </c>
-      <c r="P53" s="30" t="s">
+      <c r="R53" s="30" t="s">
         <v>123</v>
       </c>
-      <c r="Q53" s="5">
+      <c r="S53" s="5">
         <v>46</v>
       </c>
-      <c r="R53" s="14" t="s">
-        <v>108</v>
-      </c>
-      <c r="S53" s="5"/>
-    </row>
-    <row r="54" spans="1:19" ht="17">
+      <c r="T53" s="14" t="s">
+        <v>108</v>
+      </c>
+      <c r="U53" s="5"/>
+    </row>
+    <row r="54" spans="1:21" ht="17">
       <c r="A54" s="8">
         <v>52</v>
       </c>
@@ -4385,46 +4896,52 @@
         <v>187</v>
       </c>
       <c r="G54" s="6" t="s">
+        <v>285</v>
+      </c>
+      <c r="H54" s="6" t="s">
         <v>183</v>
-      </c>
-      <c r="H54" s="6" t="s">
-        <v>104</v>
       </c>
       <c r="I54" s="6" t="s">
         <v>104</v>
       </c>
-      <c r="J54" s="6">
-        <v>1</v>
-      </c>
-      <c r="K54" s="6" t="s">
+      <c r="J54" s="6" t="s">
+        <v>104</v>
+      </c>
+      <c r="K54" s="6">
+        <v>1</v>
+      </c>
+      <c r="L54" s="6" t="s">
         <v>85</v>
       </c>
-      <c r="L54" s="7" t="s">
+      <c r="M54" s="6" t="s">
+        <v>276</v>
+      </c>
+      <c r="N54" s="7" t="s">
         <v>168</v>
       </c>
-      <c r="M54" s="8" t="s">
+      <c r="O54" s="8" t="s">
         <v>77</v>
       </c>
-      <c r="N54" s="9">
-        <v>0</v>
-      </c>
-      <c r="O54" s="10" t="s">
+      <c r="P54" s="9">
+        <v>0</v>
+      </c>
+      <c r="Q54" s="10" t="s">
         <v>111</v>
       </c>
-      <c r="P54" s="32" t="s">
+      <c r="R54" s="32" t="s">
         <v>174</v>
       </c>
-      <c r="Q54" s="5">
+      <c r="S54" s="5">
         <v>40</v>
       </c>
-      <c r="R54" s="14" t="s">
-        <v>108</v>
-      </c>
-      <c r="S54" s="5" t="s">
+      <c r="T54" s="14" t="s">
+        <v>108</v>
+      </c>
+      <c r="U54" s="5" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="55" spans="1:19" ht="17">
+    <row r="55" spans="1:21" ht="17">
       <c r="A55" s="8">
         <v>53</v>
       </c>
@@ -4443,42 +4960,46 @@
       </c>
       <c r="F55" s="6"/>
       <c r="G55" s="6"/>
-      <c r="H55" s="6" t="s">
-        <v>105</v>
-      </c>
+      <c r="H55" s="6"/>
       <c r="I55" s="6" t="s">
         <v>105</v>
       </c>
-      <c r="J55" s="6">
-        <v>1</v>
-      </c>
-      <c r="K55" s="6" t="s">
+      <c r="J55" s="6" t="s">
+        <v>105</v>
+      </c>
+      <c r="K55" s="6">
+        <v>1</v>
+      </c>
+      <c r="L55" s="6" t="s">
         <v>87</v>
       </c>
-      <c r="L55" s="7" t="s">
+      <c r="M55" s="6" t="s">
+        <v>277</v>
+      </c>
+      <c r="N55" s="7" t="s">
         <v>169</v>
       </c>
-      <c r="M55" s="8" t="s">
+      <c r="O55" s="8" t="s">
         <v>77</v>
       </c>
-      <c r="N55" s="9">
-        <v>0</v>
-      </c>
-      <c r="O55" s="10" t="s">
+      <c r="P55" s="9">
+        <v>0</v>
+      </c>
+      <c r="Q55" s="10" t="s">
         <v>109</v>
       </c>
-      <c r="P55" s="30" t="s">
+      <c r="R55" s="30" t="s">
         <v>123</v>
       </c>
-      <c r="Q55" s="5">
+      <c r="S55" s="5">
         <v>45</v>
       </c>
-      <c r="R55" s="14" t="s">
-        <v>108</v>
-      </c>
-      <c r="S55" s="5"/>
-    </row>
-    <row r="56" spans="1:19" ht="17">
+      <c r="T55" s="14" t="s">
+        <v>108</v>
+      </c>
+      <c r="U55" s="5"/>
+    </row>
+    <row r="56" spans="1:21" ht="17">
       <c r="A56" s="8">
         <v>54</v>
       </c>
@@ -4497,42 +5018,46 @@
       </c>
       <c r="F56" s="6"/>
       <c r="G56" s="6"/>
-      <c r="H56" s="6" t="s">
-        <v>105</v>
-      </c>
+      <c r="H56" s="6"/>
       <c r="I56" s="6" t="s">
         <v>105</v>
       </c>
-      <c r="J56" s="6">
-        <v>1</v>
-      </c>
-      <c r="K56" s="6" t="s">
+      <c r="J56" s="6" t="s">
+        <v>105</v>
+      </c>
+      <c r="K56" s="6">
+        <v>1</v>
+      </c>
+      <c r="L56" s="6" t="s">
         <v>89</v>
       </c>
-      <c r="L56" s="7" t="s">
+      <c r="M56" s="6" t="s">
+        <v>278</v>
+      </c>
+      <c r="N56" s="7" t="s">
         <v>190</v>
       </c>
-      <c r="M56" s="8" t="s">
+      <c r="O56" s="8" t="s">
         <v>77</v>
       </c>
-      <c r="N56" s="9">
-        <v>0</v>
-      </c>
-      <c r="O56" s="10" t="s">
+      <c r="P56" s="9">
+        <v>0</v>
+      </c>
+      <c r="Q56" s="10" t="s">
         <v>109</v>
       </c>
-      <c r="P56" s="25" t="s">
+      <c r="R56" s="25" t="s">
         <v>176</v>
       </c>
-      <c r="Q56" s="5">
+      <c r="S56" s="5">
         <v>47</v>
       </c>
-      <c r="R56" s="14" t="s">
-        <v>108</v>
-      </c>
-      <c r="S56" s="5"/>
-    </row>
-    <row r="57" spans="1:19" ht="17">
+      <c r="T56" s="14" t="s">
+        <v>108</v>
+      </c>
+      <c r="U56" s="5"/>
+    </row>
+    <row r="57" spans="1:21" ht="17">
       <c r="A57" s="8">
         <v>55</v>
       </c>
@@ -4551,42 +5076,46 @@
       </c>
       <c r="F57" s="6"/>
       <c r="G57" s="6"/>
-      <c r="H57" s="6" t="s">
-        <v>104</v>
-      </c>
+      <c r="H57" s="6"/>
       <c r="I57" s="6" t="s">
         <v>104</v>
       </c>
-      <c r="J57" s="6">
-        <v>1</v>
-      </c>
-      <c r="K57" s="6" t="s">
+      <c r="J57" s="6" t="s">
+        <v>104</v>
+      </c>
+      <c r="K57" s="6">
+        <v>1</v>
+      </c>
+      <c r="L57" s="6" t="s">
         <v>91</v>
       </c>
-      <c r="L57" s="7" t="s">
+      <c r="M57" s="6" t="s">
+        <v>279</v>
+      </c>
+      <c r="N57" s="7" t="s">
         <v>170</v>
       </c>
-      <c r="M57" s="8" t="s">
+      <c r="O57" s="8" t="s">
         <v>77</v>
       </c>
-      <c r="N57" s="9">
-        <v>0</v>
-      </c>
-      <c r="O57" s="10" t="s">
+      <c r="P57" s="9">
+        <v>0</v>
+      </c>
+      <c r="Q57" s="10" t="s">
         <v>111</v>
       </c>
-      <c r="P57" s="31" t="s">
+      <c r="R57" s="31" t="s">
         <v>173</v>
       </c>
-      <c r="Q57" s="5">
+      <c r="S57" s="5">
         <v>43</v>
       </c>
-      <c r="R57" s="14" t="s">
-        <v>108</v>
-      </c>
-      <c r="S57" s="5"/>
-    </row>
-    <row r="58" spans="1:19" ht="17">
+      <c r="T57" s="14" t="s">
+        <v>108</v>
+      </c>
+      <c r="U57" s="5"/>
+    </row>
+    <row r="58" spans="1:21" ht="17">
       <c r="A58" s="8">
         <v>56</v>
       </c>
@@ -4605,43 +5134,47 @@
       </c>
       <c r="F58" s="6"/>
       <c r="G58" s="6"/>
-      <c r="H58" s="6" t="s">
-        <v>104</v>
-      </c>
+      <c r="H58" s="6"/>
       <c r="I58" s="6" t="s">
         <v>104</v>
       </c>
-      <c r="J58" s="6">
-        <v>1</v>
-      </c>
-      <c r="K58" s="6" t="s">
+      <c r="J58" s="6" t="s">
+        <v>104</v>
+      </c>
+      <c r="K58" s="6">
+        <v>1</v>
+      </c>
+      <c r="L58" s="6" t="s">
         <v>93</v>
       </c>
-      <c r="L58" s="7" t="s">
+      <c r="M58" s="6" t="s">
+        <v>280</v>
+      </c>
+      <c r="N58" s="7" t="s">
         <v>171</v>
       </c>
-      <c r="M58" s="8" t="s">
+      <c r="O58" s="8" t="s">
         <v>77</v>
       </c>
-      <c r="N58" s="9">
-        <v>0</v>
-      </c>
-      <c r="O58" s="10" t="s">
+      <c r="P58" s="9">
+        <v>0</v>
+      </c>
+      <c r="Q58" s="10" t="s">
         <v>111</v>
       </c>
-      <c r="P58" s="32" t="s">
+      <c r="R58" s="32" t="s">
         <v>174</v>
       </c>
-      <c r="Q58" s="5">
+      <c r="S58" s="5">
         <v>39</v>
       </c>
-      <c r="R58" s="14" t="s">
-        <v>108</v>
-      </c>
-      <c r="S58" s="5"/>
+      <c r="T58" s="14" t="s">
+        <v>108</v>
+      </c>
+      <c r="U58" s="5"/>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:S58">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:U58">
     <sortCondition ref="A2:A58"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
change mean to averaged in rolling aggregations
</commit_message>
<xml_diff>
--- a/data-raw/params_out.xlsx
+++ b/data-raw/params_out.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tsamsonov/GitHub/grwat/data-raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1BB3FC41-12A2-DA46-A5D7-F55E8B286A57}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C436DFCD-6E0F-8B49-8128-710DE205B5F5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="560" windowWidth="51200" windowHeight="26860" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="20" yWindow="560" windowWidth="51200" windowHeight="26860" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
@@ -722,60 +722,6 @@
     <t>Minimum daily winter runoff</t>
   </si>
   <si>
-    <t>Minimum 30-day mean summer runoff</t>
-  </si>
-  <si>
-    <t>First date of minimum 30-day mean summer runoff</t>
-  </si>
-  <si>
-    <t>Last date of minimum 30-day mean summer runoff</t>
-  </si>
-  <si>
-    <t>Minimum 30-day mean winter runoff</t>
-  </si>
-  <si>
-    <t>First date of minimum 30-day mean winter runoff</t>
-  </si>
-  <si>
-    <t>Last date of minimum 30-day mean winter runoff</t>
-  </si>
-  <si>
-    <t>Minimum 10-day mean summer runoff</t>
-  </si>
-  <si>
-    <t>First date of minimum 10-day mean summer runoff</t>
-  </si>
-  <si>
-    <t>Last date of minimum 10-day mean summer runoff</t>
-  </si>
-  <si>
-    <t>Minimum 10-day mean winter runoff</t>
-  </si>
-  <si>
-    <t>First date of minimum 10-day mean winter runoff</t>
-  </si>
-  <si>
-    <t>Last date of minimum 10-day mean winter runoff</t>
-  </si>
-  <si>
-    <t>Minimum 5-day mean summer runoff</t>
-  </si>
-  <si>
-    <t>First date of minimum 5-day mean summer runoff</t>
-  </si>
-  <si>
-    <t>Last date of minimum 5-day mean summer runoff</t>
-  </si>
-  <si>
-    <t>Minimum 5-day mean winter runoff</t>
-  </si>
-  <si>
-    <t>First date of minimum 5-day mean winter runoff</t>
-  </si>
-  <si>
-    <t>Last date of minimum 5-day mean winter runoff</t>
-  </si>
-  <si>
     <t>Date of minimum daily summer runoff</t>
   </si>
   <si>
@@ -882,6 +828,60 @@
   </si>
   <si>
     <t>День місячного витрати за зиму</t>
+  </si>
+  <si>
+    <t>Minimum 30-day averaged summer runoff</t>
+  </si>
+  <si>
+    <t>First date of minimum 30-day averaged summer runoff</t>
+  </si>
+  <si>
+    <t>Last date of minimum 30-day averaged summer runoff</t>
+  </si>
+  <si>
+    <t>First date of minimum 30-day averaged winter runoff</t>
+  </si>
+  <si>
+    <t>Last date of minimum 30-day averaged winter runoff</t>
+  </si>
+  <si>
+    <t>First date of minimum 10-day averaged summer runoff</t>
+  </si>
+  <si>
+    <t>Last date of minimum 10-day averaged summer runoff</t>
+  </si>
+  <si>
+    <t>First date of minimum 10-day averaged winter runoff</t>
+  </si>
+  <si>
+    <t>Last date of minimum 10-day averaged winter runoff</t>
+  </si>
+  <si>
+    <t>First date of minimum 5-day averaged summer runoff</t>
+  </si>
+  <si>
+    <t>Last date of minimum 5-day averaged summer runoff</t>
+  </si>
+  <si>
+    <t>First date of minimum 5-day averaged winter runoff</t>
+  </si>
+  <si>
+    <t>Last date of minimum 5-day averaged winter runoff</t>
+  </si>
+  <si>
+    <t>Minimum 30-day averaged winter runoff</t>
+  </si>
+  <si>
+    <t>Minimum 10-day averaged summer runoff</t>
+  </si>
+  <si>
+    <t>Minimum 10-day averaged winter runoff</t>
+  </si>
+  <si>
+    <t>Minimum 5-day averaged summer runoff</t>
+  </si>
+  <si>
+    <t>Minimum 5-day averaged winter runoff</t>
   </si>
 </sst>
 </file>
@@ -1482,7 +1482,7 @@
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="K1" zoomScale="131" zoomScaleNormal="70" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="P13" sqref="P13"/>
+      <selection pane="bottomLeft" activeCell="N27" sqref="N27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16"/>
@@ -2051,7 +2051,7 @@
         <v>170</v>
       </c>
       <c r="N9" s="7" t="s">
-        <v>263</v>
+        <v>245</v>
       </c>
       <c r="O9" s="8" t="s">
         <v>94</v>
@@ -2114,7 +2114,7 @@
         <v>171</v>
       </c>
       <c r="N10" s="7" t="s">
-        <v>264</v>
+        <v>246</v>
       </c>
       <c r="O10" s="8" t="s">
         <v>94</v>
@@ -2177,7 +2177,7 @@
         <v>172</v>
       </c>
       <c r="N11" s="17" t="s">
-        <v>265</v>
+        <v>247</v>
       </c>
       <c r="O11" s="8" t="s">
         <v>94</v>
@@ -2235,10 +2235,10 @@
         <v>1</v>
       </c>
       <c r="L12" s="21" t="s">
-        <v>275</v>
+        <v>257</v>
       </c>
       <c r="M12" s="21" t="s">
-        <v>278</v>
+        <v>260</v>
       </c>
       <c r="N12" s="22" t="s">
         <v>226</v>
@@ -2298,13 +2298,13 @@
         <v>1</v>
       </c>
       <c r="L13" s="21" t="s">
-        <v>274</v>
+        <v>256</v>
       </c>
       <c r="M13" s="21" t="s">
-        <v>279</v>
+        <v>261</v>
       </c>
       <c r="N13" s="22" t="s">
-        <v>246</v>
+        <v>228</v>
       </c>
       <c r="O13" s="20" t="s">
         <v>95</v>
@@ -2363,10 +2363,10 @@
         <v>1</v>
       </c>
       <c r="L14" s="21" t="s">
-        <v>276</v>
+        <v>258</v>
       </c>
       <c r="M14" s="21" t="s">
-        <v>280</v>
+        <v>262</v>
       </c>
       <c r="N14" s="22" t="s">
         <v>227</v>
@@ -2426,13 +2426,13 @@
         <v>1</v>
       </c>
       <c r="L15" s="21" t="s">
-        <v>277</v>
+        <v>259</v>
       </c>
       <c r="M15" s="21" t="s">
-        <v>281</v>
+        <v>263</v>
       </c>
       <c r="N15" s="22" t="s">
-        <v>247</v>
+        <v>229</v>
       </c>
       <c r="O15" s="20" t="s">
         <v>95</v>
@@ -2497,7 +2497,7 @@
         <v>173</v>
       </c>
       <c r="N16" s="22" t="s">
-        <v>228</v>
+        <v>264</v>
       </c>
       <c r="O16" s="20" t="s">
         <v>95</v>
@@ -2560,7 +2560,7 @@
         <v>174</v>
       </c>
       <c r="N17" s="22" t="s">
-        <v>229</v>
+        <v>265</v>
       </c>
       <c r="O17" s="20" t="s">
         <v>95</v>
@@ -2623,7 +2623,7 @@
         <v>175</v>
       </c>
       <c r="N18" s="22" t="s">
-        <v>230</v>
+        <v>266</v>
       </c>
       <c r="O18" s="20" t="s">
         <v>95</v>
@@ -2686,7 +2686,7 @@
         <v>176</v>
       </c>
       <c r="N19" s="22" t="s">
-        <v>231</v>
+        <v>277</v>
       </c>
       <c r="O19" s="20" t="s">
         <v>95</v>
@@ -2749,7 +2749,7 @@
         <v>177</v>
       </c>
       <c r="N20" s="22" t="s">
-        <v>232</v>
+        <v>267</v>
       </c>
       <c r="O20" s="20" t="s">
         <v>95</v>
@@ -2812,7 +2812,7 @@
         <v>178</v>
       </c>
       <c r="N21" s="22" t="s">
-        <v>233</v>
+        <v>268</v>
       </c>
       <c r="O21" s="20" t="s">
         <v>95</v>
@@ -2875,7 +2875,7 @@
         <v>179</v>
       </c>
       <c r="N22" s="22" t="s">
-        <v>234</v>
+        <v>278</v>
       </c>
       <c r="O22" s="20" t="s">
         <v>95</v>
@@ -2938,7 +2938,7 @@
         <v>180</v>
       </c>
       <c r="N23" s="22" t="s">
-        <v>235</v>
+        <v>269</v>
       </c>
       <c r="O23" s="20" t="s">
         <v>95</v>
@@ -3001,7 +3001,7 @@
         <v>181</v>
       </c>
       <c r="N24" s="22" t="s">
-        <v>236</v>
+        <v>270</v>
       </c>
       <c r="O24" s="20" t="s">
         <v>95</v>
@@ -3064,7 +3064,7 @@
         <v>182</v>
       </c>
       <c r="N25" s="22" t="s">
-        <v>237</v>
+        <v>279</v>
       </c>
       <c r="O25" s="20" t="s">
         <v>95</v>
@@ -3127,7 +3127,7 @@
         <v>183</v>
       </c>
       <c r="N26" s="22" t="s">
-        <v>238</v>
+        <v>271</v>
       </c>
       <c r="O26" s="20" t="s">
         <v>95</v>
@@ -3190,7 +3190,7 @@
         <v>184</v>
       </c>
       <c r="N27" s="22" t="s">
-        <v>239</v>
+        <v>272</v>
       </c>
       <c r="O27" s="20" t="s">
         <v>95</v>
@@ -3253,7 +3253,7 @@
         <v>185</v>
       </c>
       <c r="N28" s="22" t="s">
-        <v>240</v>
+        <v>280</v>
       </c>
       <c r="O28" s="20" t="s">
         <v>95</v>
@@ -3316,7 +3316,7 @@
         <v>186</v>
       </c>
       <c r="N29" s="22" t="s">
-        <v>241</v>
+        <v>273</v>
       </c>
       <c r="O29" s="20" t="s">
         <v>95</v>
@@ -3379,7 +3379,7 @@
         <v>187</v>
       </c>
       <c r="N30" s="22" t="s">
-        <v>242</v>
+        <v>274</v>
       </c>
       <c r="O30" s="20" t="s">
         <v>95</v>
@@ -3442,7 +3442,7 @@
         <v>188</v>
       </c>
       <c r="N31" s="22" t="s">
-        <v>243</v>
+        <v>281</v>
       </c>
       <c r="O31" s="20" t="s">
         <v>95</v>
@@ -3505,7 +3505,7 @@
         <v>189</v>
       </c>
       <c r="N32" s="22" t="s">
-        <v>244</v>
+        <v>275</v>
       </c>
       <c r="O32" s="20" t="s">
         <v>95</v>
@@ -3568,7 +3568,7 @@
         <v>190</v>
       </c>
       <c r="N33" s="22" t="s">
-        <v>245</v>
+        <v>276</v>
       </c>
       <c r="O33" s="20" t="s">
         <v>95</v>
@@ -3631,7 +3631,7 @@
         <v>191</v>
       </c>
       <c r="N34" s="7" t="s">
-        <v>248</v>
+        <v>230</v>
       </c>
       <c r="O34" s="8" t="s">
         <v>46</v>
@@ -3694,7 +3694,7 @@
         <v>192</v>
       </c>
       <c r="N35" s="7" t="s">
-        <v>249</v>
+        <v>231</v>
       </c>
       <c r="O35" s="8" t="s">
         <v>46</v>
@@ -3757,7 +3757,7 @@
         <v>193</v>
       </c>
       <c r="N36" s="7" t="s">
-        <v>267</v>
+        <v>249</v>
       </c>
       <c r="O36" s="8" t="s">
         <v>46</v>
@@ -3820,7 +3820,7 @@
         <v>194</v>
       </c>
       <c r="N37" s="7" t="s">
-        <v>250</v>
+        <v>232</v>
       </c>
       <c r="O37" s="8" t="s">
         <v>46</v>
@@ -3883,7 +3883,7 @@
         <v>195</v>
       </c>
       <c r="N38" s="7" t="s">
-        <v>266</v>
+        <v>248</v>
       </c>
       <c r="O38" s="8" t="s">
         <v>46</v>
@@ -3946,7 +3946,7 @@
         <v>196</v>
       </c>
       <c r="N39" s="7" t="s">
-        <v>268</v>
+        <v>250</v>
       </c>
       <c r="O39" s="8" t="s">
         <v>46</v>
@@ -4009,7 +4009,7 @@
         <v>197</v>
       </c>
       <c r="N40" s="7" t="s">
-        <v>251</v>
+        <v>233</v>
       </c>
       <c r="O40" s="8" t="s">
         <v>46</v>
@@ -4072,7 +4072,7 @@
         <v>198</v>
       </c>
       <c r="N41" s="7" t="s">
-        <v>269</v>
+        <v>251</v>
       </c>
       <c r="O41" s="8" t="s">
         <v>46</v>
@@ -4135,7 +4135,7 @@
         <v>199</v>
       </c>
       <c r="N42" s="7" t="s">
-        <v>252</v>
+        <v>234</v>
       </c>
       <c r="O42" s="8" t="s">
         <v>46</v>
@@ -4199,7 +4199,7 @@
         <v>200</v>
       </c>
       <c r="N43" s="7" t="s">
-        <v>255</v>
+        <v>237</v>
       </c>
       <c r="O43" s="8" t="s">
         <v>46</v>
@@ -4263,7 +4263,7 @@
         <v>201</v>
       </c>
       <c r="N44" s="7" t="s">
-        <v>253</v>
+        <v>235</v>
       </c>
       <c r="O44" s="8" t="s">
         <v>46</v>
@@ -4327,7 +4327,7 @@
         <v>202</v>
       </c>
       <c r="N45" s="7" t="s">
-        <v>256</v>
+        <v>238</v>
       </c>
       <c r="O45" s="8" t="s">
         <v>46</v>
@@ -4391,7 +4391,7 @@
         <v>203</v>
       </c>
       <c r="N46" s="7" t="s">
-        <v>254</v>
+        <v>236</v>
       </c>
       <c r="O46" s="8" t="s">
         <v>46</v>
@@ -4455,7 +4455,7 @@
         <v>204</v>
       </c>
       <c r="N47" s="22" t="s">
-        <v>257</v>
+        <v>239</v>
       </c>
       <c r="O47" s="20" t="s">
         <v>96</v>
@@ -4519,7 +4519,7 @@
         <v>205</v>
       </c>
       <c r="N48" s="22" t="s">
-        <v>258</v>
+        <v>240</v>
       </c>
       <c r="O48" s="20" t="s">
         <v>96</v>
@@ -4583,7 +4583,7 @@
         <v>206</v>
       </c>
       <c r="N49" s="22" t="s">
-        <v>270</v>
+        <v>252</v>
       </c>
       <c r="O49" s="20" t="s">
         <v>96</v>
@@ -4647,7 +4647,7 @@
         <v>207</v>
       </c>
       <c r="N50" s="22" t="s">
-        <v>271</v>
+        <v>253</v>
       </c>
       <c r="O50" s="20" t="s">
         <v>96</v>
@@ -4711,7 +4711,7 @@
         <v>208</v>
       </c>
       <c r="N51" s="7" t="s">
-        <v>272</v>
+        <v>254</v>
       </c>
       <c r="O51" s="8" t="s">
         <v>73</v>
@@ -4775,7 +4775,7 @@
         <v>209</v>
       </c>
       <c r="N52" s="7" t="s">
-        <v>260</v>
+        <v>242</v>
       </c>
       <c r="O52" s="8" t="s">
         <v>73</v>
@@ -4841,7 +4841,7 @@
         <v>210</v>
       </c>
       <c r="N53" s="7" t="s">
-        <v>273</v>
+        <v>255</v>
       </c>
       <c r="O53" s="8" t="s">
         <v>73</v>
@@ -4905,7 +4905,7 @@
         <v>211</v>
       </c>
       <c r="N54" s="7" t="s">
-        <v>259</v>
+        <v>241</v>
       </c>
       <c r="O54" s="8" t="s">
         <v>73</v>
@@ -5081,7 +5081,7 @@
         <v>214</v>
       </c>
       <c r="N57" s="7" t="s">
-        <v>261</v>
+        <v>243</v>
       </c>
       <c r="O57" s="8" t="s">
         <v>73</v>
@@ -5139,7 +5139,7 @@
         <v>215</v>
       </c>
       <c r="N58" s="7" t="s">
-        <v>262</v>
+        <v>244</v>
       </c>
       <c r="O58" s="8" t="s">
         <v>73</v>

</xml_diff>